<commit_message>
MTP030 COP rows done. v1 of SO/LNO subdomain patching done.
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9C088B-B9AC-4F35-B365-DD126493C2ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656738A9-9772-48EB-92DF-38FA1E4DEE5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="38">
   <si>
     <t>MINISCANS</t>
   </si>
@@ -126,9 +126,6 @@
     <t>64 accumulations</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>34 (fixed=3)</t>
   </si>
   <si>
@@ -136,6 +133,18 @@
   </si>
   <si>
     <t>&lt;- add to high priority</t>
+  </si>
+  <si>
+    <t>2915 (fixed=1)</t>
+  </si>
+  <si>
+    <t>SO 6X164</t>
+  </si>
+  <si>
+    <t>3665 (fixed=1)</t>
+  </si>
+  <si>
+    <t>LNO 6x164</t>
   </si>
 </sst>
 </file>
@@ -855,7 +864,7 @@
     <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -988,6 +997,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1312,8 +1331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H115" sqref="H115"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1434,7 +1453,7 @@
         <v>107</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="15">
         <v>3</v>
@@ -1452,17 +1471,23 @@
         <v>22</v>
       </c>
       <c r="L5" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="M5" s="62">
+        <v>35</v>
+      </c>
+      <c r="M5" s="98">
         <v>3973</v>
       </c>
       <c r="N5" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
+        <v>34</v>
+      </c>
+      <c r="O5" s="15">
+        <v>10</v>
+      </c>
+      <c r="P5" s="15">
+        <v>20</v>
+      </c>
+      <c r="Q5" s="15">
+        <v>25</v>
+      </c>
       <c r="R5" s="16"/>
       <c r="S5" s="17"/>
     </row>
@@ -1474,7 +1499,7 @@
         <v>57</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="18">
         <v>3</v>
@@ -1494,17 +1519,21 @@
       <c r="J6" s="60"/>
       <c r="K6" s="60"/>
       <c r="L6" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6" s="63">
+        <v>37</v>
+      </c>
+      <c r="M6" s="99">
         <v>674</v>
       </c>
-      <c r="N6" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
+      <c r="N6" s="100" t="s">
+        <v>36</v>
+      </c>
+      <c r="O6" s="18">
+        <v>15</v>
+      </c>
+      <c r="P6" s="18">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="97"/>
       <c r="R6" s="7"/>
       <c r="S6" s="8"/>
     </row>
@@ -2036,7 +2065,7 @@
       <c r="X21" s="67"/>
       <c r="Y21" s="68"/>
       <c r="Z21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.35">
@@ -5594,7 +5623,7 @@
       <c r="O121" s="29">
         <v>17</v>
       </c>
-      <c r="P121" s="30">
+      <c r="P121" s="32">
         <v>29</v>
       </c>
       <c r="Q121" s="30"/>
@@ -5635,7 +5664,7 @@
       <c r="O122" s="56">
         <v>17</v>
       </c>
-      <c r="P122" s="30">
+      <c r="P122" s="32">
         <v>29</v>
       </c>
       <c r="Q122" s="30"/>
@@ -5679,7 +5708,7 @@
       <c r="O123" s="29">
         <v>11</v>
       </c>
-      <c r="P123" s="30">
+      <c r="P123" s="32">
         <v>29</v>
       </c>
       <c r="Q123" s="30"/>
@@ -5721,7 +5750,7 @@
       <c r="O124" s="2">
         <v>14</v>
       </c>
-      <c r="P124" s="30">
+      <c r="P124" s="32">
         <v>29</v>
       </c>
       <c r="S124" s="4"/>

</xml_diff>

<commit_message>
MTP031 new patched obs added; draft orbit plan made
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656738A9-9772-48EB-92DF-38FA1E4DEE5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA08A03-9965-4DA0-9945-2357E3395A6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -974,6 +974,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -997,16 +1007,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1332,7 +1332,7 @@
   <dimension ref="A1:AB131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1372,22 +1372,22 @@
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="92" t="s">
+      <c r="E3" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="94"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="98"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
-      <c r="O3" s="89" t="s">
+      <c r="O3" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="90"/>
-      <c r="Q3" s="90"/>
-      <c r="R3" s="90"/>
-      <c r="S3" s="91"/>
+      <c r="P3" s="94"/>
+      <c r="Q3" s="94"/>
+      <c r="R3" s="94"/>
+      <c r="S3" s="95"/>
       <c r="V3" s="27" t="s">
         <v>19</v>
       </c>
@@ -1473,22 +1473,24 @@
       <c r="L5" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="M5" s="98">
+      <c r="M5" s="90">
         <v>3973</v>
       </c>
       <c r="N5" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="O5" s="15">
+      <c r="O5" s="3">
+        <v>5</v>
+      </c>
+      <c r="P5" s="15">
         <v>10</v>
       </c>
-      <c r="P5" s="15">
+      <c r="Q5" s="15">
         <v>20</v>
       </c>
-      <c r="Q5" s="15">
+      <c r="R5" s="15">
         <v>25</v>
       </c>
-      <c r="R5" s="16"/>
       <c r="S5" s="17"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.35">
@@ -1521,10 +1523,10 @@
       <c r="L6" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="M6" s="99">
+      <c r="M6" s="91">
         <v>674</v>
       </c>
-      <c r="N6" s="100" t="s">
+      <c r="N6" s="92" t="s">
         <v>36</v>
       </c>
       <c r="O6" s="18">
@@ -1533,7 +1535,7 @@
       <c r="P6" s="18">
         <v>30</v>
       </c>
-      <c r="Q6" s="97"/>
+      <c r="Q6" s="89"/>
       <c r="R6" s="7"/>
       <c r="S6" s="8"/>
     </row>
@@ -1566,26 +1568,26 @@
       <c r="B10" s="13"/>
       <c r="C10" s="9"/>
       <c r="D10" s="59"/>
-      <c r="E10" s="95" t="s">
+      <c r="E10" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="96"/>
-      <c r="G10" s="96"/>
-      <c r="H10" s="96"/>
-      <c r="I10" s="96"/>
+      <c r="F10" s="100"/>
+      <c r="G10" s="100"/>
+      <c r="H10" s="100"/>
+      <c r="I10" s="100"/>
       <c r="K10" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L10" s="13"/>
       <c r="M10" s="9"/>
       <c r="N10" s="59"/>
-      <c r="O10" s="95" t="s">
+      <c r="O10" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="P10" s="96"/>
-      <c r="Q10" s="96"/>
-      <c r="R10" s="96"/>
-      <c r="S10" s="96"/>
+      <c r="P10" s="100"/>
+      <c r="Q10" s="100"/>
+      <c r="R10" s="100"/>
+      <c r="S10" s="100"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11" s="40" t="s">
@@ -2889,26 +2891,26 @@
       <c r="B45" s="13"/>
       <c r="C45" s="9"/>
       <c r="D45" s="59"/>
-      <c r="E45" s="95" t="s">
+      <c r="E45" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="F45" s="96"/>
-      <c r="G45" s="96"/>
-      <c r="H45" s="96"/>
-      <c r="I45" s="96"/>
+      <c r="F45" s="100"/>
+      <c r="G45" s="100"/>
+      <c r="H45" s="100"/>
+      <c r="I45" s="100"/>
       <c r="K45" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L45" s="13"/>
       <c r="M45" s="9"/>
       <c r="N45" s="59"/>
-      <c r="O45" s="95" t="s">
+      <c r="O45" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="P45" s="96"/>
-      <c r="Q45" s="96"/>
-      <c r="R45" s="96"/>
-      <c r="S45" s="96"/>
+      <c r="P45" s="100"/>
+      <c r="Q45" s="100"/>
+      <c r="R45" s="100"/>
+      <c r="S45" s="100"/>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
@@ -4084,26 +4086,26 @@
       <c r="B79" s="13"/>
       <c r="C79" s="9"/>
       <c r="D79" s="33"/>
-      <c r="E79" s="95" t="s">
+      <c r="E79" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="F79" s="96"/>
-      <c r="G79" s="96"/>
-      <c r="H79" s="96"/>
-      <c r="I79" s="96"/>
+      <c r="F79" s="100"/>
+      <c r="G79" s="100"/>
+      <c r="H79" s="100"/>
+      <c r="I79" s="100"/>
       <c r="K79" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L79" s="13"/>
       <c r="M79" s="9"/>
       <c r="N79" s="33"/>
-      <c r="O79" s="95" t="s">
+      <c r="O79" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="P79" s="96"/>
-      <c r="Q79" s="96"/>
-      <c r="R79" s="96"/>
-      <c r="S79" s="96"/>
+      <c r="P79" s="100"/>
+      <c r="Q79" s="100"/>
+      <c r="R79" s="100"/>
+      <c r="S79" s="100"/>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A80" s="9" t="s">
@@ -5286,26 +5288,26 @@
       </c>
       <c r="B113" s="41"/>
       <c r="C113" s="9"/>
-      <c r="E113" s="95" t="s">
+      <c r="E113" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="F113" s="96"/>
-      <c r="G113" s="96"/>
-      <c r="H113" s="96"/>
-      <c r="I113" s="96"/>
+      <c r="F113" s="100"/>
+      <c r="G113" s="100"/>
+      <c r="H113" s="100"/>
+      <c r="I113" s="100"/>
       <c r="K113" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L113" s="41"/>
       <c r="M113" s="9"/>
       <c r="N113" s="33"/>
-      <c r="O113" s="95" t="s">
+      <c r="O113" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="P113" s="96"/>
-      <c r="Q113" s="96"/>
-      <c r="R113" s="96"/>
-      <c r="S113" s="96"/>
+      <c r="P113" s="100"/>
+      <c r="Q113" s="100"/>
+      <c r="R113" s="100"/>
+      <c r="S113" s="100"/>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A114" s="9" t="s">

</xml_diff>

<commit_message>
MTP032 COP rows done
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF5EBA7-BBFD-4424-981A-0D50CA2C96AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174FD6E3-300C-4722-829C-C0A471CF54B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,12 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1332,25 +1326,25 @@
   <dimension ref="A1:AB131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I135" sqref="I135"/>
+      <selection activeCell="G134" sqref="G134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7265625" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" customWidth="1"/>
-    <col min="4" max="4" width="21.7265625" customWidth="1"/>
-    <col min="11" max="11" width="16.81640625" customWidth="1"/>
-    <col min="12" max="12" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.26953125" customWidth="1"/>
-    <col min="22" max="22" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.28515625" customWidth="1"/>
+    <col min="22" max="22" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1358,7 +1352,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:25" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
@@ -1369,7 +1363,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="96" t="s">
@@ -1395,7 +1389,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>12</v>
       </c>
@@ -1445,7 +1439,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
         <v>1</v>
       </c>
@@ -1493,7 +1487,7 @@
       </c>
       <c r="S5" s="17"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
         <v>2</v>
       </c>
@@ -1539,7 +1533,7 @@
       <c r="R6" s="7"/>
       <c r="S6" s="8"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E7" s="84">
         <v>23</v>
       </c>
@@ -1553,7 +1547,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>0</v>
       </c>
@@ -1561,7 +1555,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>1</v>
       </c>
@@ -1589,7 +1583,7 @@
       <c r="R10" s="100"/>
       <c r="S10" s="100"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
         <v>10</v>
       </c>
@@ -1657,7 +1651,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
         <v>105</v>
       </c>
@@ -1701,7 +1695,7 @@
       <c r="X12" s="5"/>
       <c r="Y12" s="4"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="25">
         <v>107</v>
       </c>
@@ -1739,7 +1733,7 @@
       <c r="X13" s="5"/>
       <c r="Y13" s="4"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="25">
         <v>120</v>
       </c>
@@ -1777,7 +1771,7 @@
       <c r="X14" s="5"/>
       <c r="Y14" s="4"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="51">
         <v>126</v>
       </c>
@@ -1823,7 +1817,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="25">
         <v>130</v>
       </c>
@@ -1861,7 +1855,7 @@
       <c r="X16" s="49"/>
       <c r="Y16" s="50"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="25">
         <v>134</v>
       </c>
@@ -1899,7 +1893,7 @@
       <c r="X17" s="49"/>
       <c r="Y17" s="50"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="51">
         <v>141</v>
       </c>
@@ -1945,7 +1939,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="25">
         <v>142</v>
       </c>
@@ -1983,7 +1977,7 @@
       <c r="X19" s="49"/>
       <c r="Y19" s="50"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="51">
         <v>146</v>
       </c>
@@ -2029,7 +2023,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="25">
         <v>151</v>
       </c>
@@ -2070,7 +2064,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="25">
         <v>156</v>
       </c>
@@ -2108,7 +2102,7 @@
       <c r="X22" s="49"/>
       <c r="Y22" s="50"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="51">
         <v>162</v>
       </c>
@@ -2154,7 +2148,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="25">
         <v>164</v>
       </c>
@@ -2195,7 +2189,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="25">
         <v>166</v>
       </c>
@@ -2233,7 +2227,7 @@
       <c r="X25" s="49"/>
       <c r="Y25" s="50"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="25">
         <v>167</v>
       </c>
@@ -2271,7 +2265,7 @@
       <c r="X26" s="49"/>
       <c r="Y26" s="50"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="25">
         <v>168</v>
       </c>
@@ -2309,7 +2303,7 @@
       <c r="X27" s="49"/>
       <c r="Y27" s="50"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="25">
         <v>169</v>
       </c>
@@ -2345,7 +2339,7 @@
       <c r="X28" s="49"/>
       <c r="Y28" s="50"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="25">
         <v>171</v>
       </c>
@@ -2383,7 +2377,7 @@
       <c r="X29" s="49"/>
       <c r="Y29" s="50"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="25">
         <v>172</v>
       </c>
@@ -2421,7 +2415,7 @@
       <c r="X30" s="49"/>
       <c r="Y30" s="50"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="25">
         <v>178</v>
       </c>
@@ -2459,7 +2453,7 @@
       <c r="X31" s="49"/>
       <c r="Y31" s="50"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="25">
         <v>180</v>
       </c>
@@ -2497,7 +2491,7 @@
       <c r="X32" s="49"/>
       <c r="Y32" s="50"/>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="25">
         <v>182</v>
       </c>
@@ -2535,7 +2529,7 @@
       <c r="X33" s="49"/>
       <c r="Y33" s="50"/>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="25">
         <v>188</v>
       </c>
@@ -2573,7 +2567,7 @@
       <c r="X34" s="49"/>
       <c r="Y34" s="50"/>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="25">
         <v>191</v>
       </c>
@@ -2611,7 +2605,7 @@
       <c r="X35" s="49"/>
       <c r="Y35" s="50"/>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="51">
         <v>194</v>
       </c>
@@ -2653,7 +2647,7 @@
       <c r="X36" s="49"/>
       <c r="Y36" s="50"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="25">
         <v>196</v>
       </c>
@@ -2695,7 +2689,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" s="25">
         <v>197</v>
       </c>
@@ -2733,7 +2727,7 @@
       <c r="X38" s="5"/>
       <c r="Y38" s="4"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" s="25">
         <v>199</v>
       </c>
@@ -2771,7 +2765,7 @@
       <c r="X39" s="5"/>
       <c r="Y39" s="4"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="25">
         <v>201</v>
       </c>
@@ -2807,7 +2801,7 @@
       <c r="X40" s="5"/>
       <c r="Y40" s="4"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="34">
         <v>210</v>
       </c>
@@ -2851,7 +2845,7 @@
       <c r="X41" s="5"/>
       <c r="Y41" s="4"/>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="V42" s="5">
         <v>4526.9799999999996</v>
       </c>
@@ -2861,7 +2855,7 @@
       <c r="X42" s="6"/>
       <c r="Y42" s="8"/>
     </row>
-    <row r="43" spans="1:25" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="s">
         <v>0</v>
       </c>
@@ -2873,7 +2867,7 @@
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2884,7 +2878,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>1</v>
       </c>
@@ -2912,7 +2906,7 @@
       <c r="R45" s="100"/>
       <c r="S45" s="100"/>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>10</v>
       </c>
@@ -2968,7 +2962,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="72">
         <v>119</v>
       </c>
@@ -3002,7 +2996,7 @@
       </c>
       <c r="S47" s="4"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <f>A47+3</f>
         <v>122</v>
@@ -3036,7 +3030,7 @@
       <c r="O48" s="5"/>
       <c r="S48" s="4"/>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="29">
         <f t="shared" ref="A49:A75" si="0">A48+3</f>
         <v>125</v>
@@ -3085,7 +3079,7 @@
       <c r="R49" s="30"/>
       <c r="S49" s="31"/>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <f t="shared" si="0"/>
         <v>128</v>
@@ -3119,7 +3113,7 @@
       <c r="O50" s="5"/>
       <c r="S50" s="4"/>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <f t="shared" si="0"/>
         <v>131</v>
@@ -3153,7 +3147,7 @@
       <c r="O51" s="5"/>
       <c r="S51" s="4"/>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="72">
         <f t="shared" si="0"/>
         <v>134</v>
@@ -3191,7 +3185,7 @@
       </c>
       <c r="S52" s="4"/>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <f t="shared" si="0"/>
         <v>137</v>
@@ -3225,7 +3219,7 @@
       <c r="O53" s="5"/>
       <c r="S53" s="4"/>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="29">
         <f t="shared" si="0"/>
         <v>140</v>
@@ -3274,7 +3268,7 @@
       <c r="R54" s="30"/>
       <c r="S54" s="31"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <f t="shared" si="0"/>
         <v>143</v>
@@ -3308,7 +3302,7 @@
       <c r="O55" s="5"/>
       <c r="S55" s="4"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="29">
         <f t="shared" si="0"/>
         <v>146</v>
@@ -3357,7 +3351,7 @@
       <c r="R56" s="30"/>
       <c r="S56" s="31"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <f t="shared" si="0"/>
         <v>149</v>
@@ -3391,7 +3385,7 @@
       <c r="O57" s="5"/>
       <c r="S57" s="4"/>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <f t="shared" si="0"/>
         <v>152</v>
@@ -3425,7 +3419,7 @@
       <c r="O58" s="35"/>
       <c r="S58" s="4"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <f t="shared" si="0"/>
         <v>155</v>
@@ -3459,7 +3453,7 @@
       <c r="O59" s="5"/>
       <c r="S59" s="4"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <f t="shared" si="0"/>
         <v>158</v>
@@ -3493,7 +3487,7 @@
       <c r="O60" s="5"/>
       <c r="S60" s="4"/>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="29">
         <f t="shared" si="0"/>
         <v>161</v>
@@ -3542,7 +3536,7 @@
       <c r="R61" s="30"/>
       <c r="S61" s="31"/>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="72">
         <f t="shared" si="0"/>
         <v>164</v>
@@ -3586,7 +3580,7 @@
       </c>
       <c r="S62" s="4"/>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="72">
         <f t="shared" si="0"/>
         <v>167</v>
@@ -3624,7 +3618,7 @@
       </c>
       <c r="S63" s="4"/>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="72">
         <f t="shared" si="0"/>
         <v>170</v>
@@ -3658,7 +3652,7 @@
       <c r="O64" s="5"/>
       <c r="S64" s="4"/>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="72">
         <f t="shared" si="0"/>
         <v>173</v>
@@ -3692,7 +3686,7 @@
       <c r="O65" s="5"/>
       <c r="S65" s="4"/>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="72">
         <f t="shared" si="0"/>
         <v>176</v>
@@ -3726,7 +3720,7 @@
       <c r="O66" s="5"/>
       <c r="S66" s="4"/>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="72">
         <f t="shared" si="0"/>
         <v>179</v>
@@ -3760,7 +3754,7 @@
       <c r="O67" s="5"/>
       <c r="S67" s="4"/>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="72">
         <f t="shared" si="0"/>
         <v>182</v>
@@ -3794,7 +3788,7 @@
       <c r="O68" s="5"/>
       <c r="S68" s="4"/>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="72">
         <f t="shared" si="0"/>
         <v>185</v>
@@ -3832,7 +3826,7 @@
       </c>
       <c r="S69" s="4"/>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="72">
         <f t="shared" si="0"/>
         <v>188</v>
@@ -3870,7 +3864,7 @@
       </c>
       <c r="S70" s="4"/>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <f t="shared" si="0"/>
         <v>191</v>
@@ -3904,7 +3898,7 @@
       <c r="O71" s="5"/>
       <c r="S71" s="4"/>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="29">
         <f t="shared" si="0"/>
         <v>194</v>
@@ -3949,7 +3943,7 @@
       <c r="R72" s="30"/>
       <c r="S72" s="31"/>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <f t="shared" si="0"/>
         <v>197</v>
@@ -3983,7 +3977,7 @@
       <c r="O73" s="5"/>
       <c r="S73" s="4"/>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <f t="shared" si="0"/>
         <v>200</v>
@@ -4017,7 +4011,7 @@
       <c r="O74" s="5"/>
       <c r="S74" s="4"/>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
         <f t="shared" si="0"/>
         <v>203</v>
@@ -4057,7 +4051,7 @@
       <c r="R75" s="7"/>
       <c r="S75" s="8"/>
     </row>
-    <row r="77" spans="1:19" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A77" s="14" t="s">
         <v>0</v>
       </c>
@@ -4071,7 +4065,7 @@
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -4079,7 +4073,7 @@
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>1</v>
       </c>
@@ -4107,7 +4101,7 @@
       <c r="R79" s="100"/>
       <c r="S79" s="100"/>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>10</v>
       </c>
@@ -4163,7 +4157,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>119</v>
       </c>
@@ -4193,7 +4187,7 @@
       <c r="O81" s="5"/>
       <c r="S81" s="4"/>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <f>A81+3</f>
         <v>122</v>
@@ -4231,7 +4225,7 @@
       </c>
       <c r="S82" s="4"/>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" s="29">
         <f t="shared" ref="A83:A109" si="5">A82+3</f>
         <v>125</v>
@@ -4276,7 +4270,7 @@
       <c r="R83" s="30"/>
       <c r="S83" s="31"/>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <f t="shared" si="5"/>
         <v>128</v>
@@ -4310,7 +4304,7 @@
       <c r="O84" s="5"/>
       <c r="S84" s="4"/>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <f t="shared" si="5"/>
         <v>131</v>
@@ -4344,7 +4338,7 @@
       <c r="O85" s="5"/>
       <c r="S85" s="4"/>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <f t="shared" si="5"/>
         <v>134</v>
@@ -4378,7 +4372,7 @@
       <c r="O86" s="5"/>
       <c r="S86" s="4"/>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <f t="shared" si="5"/>
         <v>137</v>
@@ -4416,7 +4410,7 @@
       </c>
       <c r="S87" s="4"/>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" s="29">
         <f t="shared" si="5"/>
         <v>140</v>
@@ -4465,7 +4459,7 @@
       <c r="R88" s="30"/>
       <c r="S88" s="31"/>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <f t="shared" si="5"/>
         <v>143</v>
@@ -4499,7 +4493,7 @@
       <c r="O89" s="5"/>
       <c r="S89" s="4"/>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" s="29">
         <f t="shared" si="5"/>
         <v>146</v>
@@ -4546,7 +4540,7 @@
       <c r="R90" s="30"/>
       <c r="S90" s="31"/>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" s="29">
         <f t="shared" si="5"/>
         <v>149</v>
@@ -4588,7 +4582,7 @@
       <c r="R91" s="30"/>
       <c r="S91" s="31"/>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <f t="shared" si="5"/>
         <v>152</v>
@@ -4622,7 +4616,7 @@
       <c r="O92" s="35"/>
       <c r="S92" s="4"/>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <f t="shared" si="5"/>
         <v>155</v>
@@ -4656,7 +4650,7 @@
       <c r="O93" s="5"/>
       <c r="S93" s="4"/>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <f t="shared" si="5"/>
         <v>158</v>
@@ -4694,7 +4688,7 @@
       </c>
       <c r="S94" s="4"/>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" s="29">
         <f t="shared" si="5"/>
         <v>161</v>
@@ -4741,7 +4735,7 @@
       <c r="R95" s="30"/>
       <c r="S95" s="31"/>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <f t="shared" si="5"/>
         <v>164</v>
@@ -4775,7 +4769,7 @@
       <c r="O96" s="5"/>
       <c r="S96" s="4"/>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <f t="shared" si="5"/>
         <v>167</v>
@@ -4813,7 +4807,7 @@
       </c>
       <c r="S97" s="4"/>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <f t="shared" si="5"/>
         <v>170</v>
@@ -4851,7 +4845,7 @@
       </c>
       <c r="S98" s="4"/>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <f t="shared" si="5"/>
         <v>173</v>
@@ -4887,7 +4881,7 @@
       <c r="O99" s="5"/>
       <c r="S99" s="4"/>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <f t="shared" si="5"/>
         <v>176</v>
@@ -4923,7 +4917,7 @@
       <c r="O100" s="5"/>
       <c r="S100" s="4"/>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
         <f t="shared" si="5"/>
         <v>179</v>
@@ -4959,7 +4953,7 @@
       <c r="O101" s="5"/>
       <c r="S101" s="4"/>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <f t="shared" si="5"/>
         <v>182</v>
@@ -4995,7 +4989,7 @@
       <c r="O102" s="5"/>
       <c r="S102" s="4"/>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <f t="shared" si="5"/>
         <v>185</v>
@@ -5029,7 +5023,7 @@
       <c r="O103" s="5"/>
       <c r="S103" s="4"/>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <f t="shared" si="5"/>
         <v>188</v>
@@ -5063,7 +5057,7 @@
       <c r="O104" s="5"/>
       <c r="S104" s="4"/>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <f t="shared" si="5"/>
         <v>191</v>
@@ -5101,7 +5095,7 @@
       </c>
       <c r="S105" s="4"/>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106" s="29">
         <f t="shared" si="5"/>
         <v>194</v>
@@ -5150,7 +5144,7 @@
       <c r="R106" s="30"/>
       <c r="S106" s="31"/>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
         <f t="shared" si="5"/>
         <v>197</v>
@@ -5188,7 +5182,7 @@
       </c>
       <c r="S107" s="4"/>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <f t="shared" si="5"/>
         <v>200</v>
@@ -5222,7 +5216,7 @@
       <c r="O108" s="5"/>
       <c r="S108" s="4"/>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109" s="6">
         <f t="shared" si="5"/>
         <v>203</v>
@@ -5262,7 +5256,7 @@
       <c r="R109" s="7"/>
       <c r="S109" s="8"/>
     </row>
-    <row r="111" spans="1:19" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A111" s="14" t="s">
         <v>0</v>
       </c>
@@ -5274,7 +5268,7 @@
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -5282,7 +5276,7 @@
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113" s="9" t="s">
         <v>1</v>
       </c>
@@ -5309,7 +5303,7 @@
       <c r="R113" s="100"/>
       <c r="S113" s="100"/>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" s="9" t="s">
         <v>10</v>
       </c>
@@ -5365,7 +5359,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>110</v>
       </c>
@@ -5399,7 +5393,7 @@
       <c r="R115" s="30"/>
       <c r="S115" s="31"/>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>116</v>
       </c>
@@ -5429,7 +5423,7 @@
       <c r="O116" s="5"/>
       <c r="S116" s="4"/>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A117" s="32">
         <v>122</v>
       </c>
@@ -5473,7 +5467,7 @@
       <c r="R117" s="30"/>
       <c r="S117" s="31"/>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>128</v>
       </c>
@@ -5489,7 +5483,9 @@
       <c r="E118" s="2">
         <v>14</v>
       </c>
-      <c r="F118" s="60"/>
+      <c r="F118" s="71">
+        <v>32</v>
+      </c>
       <c r="I118" s="4"/>
       <c r="K118" s="5">
         <v>128</v>
@@ -5508,7 +5504,7 @@
       </c>
       <c r="S118" s="4"/>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>134</v>
       </c>
@@ -5524,7 +5520,9 @@
       <c r="E119" s="2">
         <v>14</v>
       </c>
-      <c r="F119" s="60"/>
+      <c r="F119" s="71">
+        <v>32</v>
+      </c>
       <c r="I119" s="4"/>
       <c r="K119" s="5">
         <v>134</v>
@@ -5543,7 +5541,7 @@
       </c>
       <c r="S119" s="4"/>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" s="32">
         <v>140</v>
       </c>
@@ -5588,7 +5586,7 @@
       <c r="R120" s="30"/>
       <c r="S120" s="31"/>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" s="32">
         <v>146</v>
       </c>
@@ -5632,7 +5630,7 @@
       <c r="R121" s="30"/>
       <c r="S121" s="31"/>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>152</v>
       </c>
@@ -5673,7 +5671,7 @@
       <c r="R122" s="30"/>
       <c r="S122" s="31"/>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A123" s="32">
         <v>158</v>
       </c>
@@ -5717,7 +5715,7 @@
       <c r="R123" s="30"/>
       <c r="S123" s="31"/>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>164</v>
       </c>
@@ -5757,7 +5755,7 @@
       </c>
       <c r="S124" s="4"/>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>170</v>
       </c>
@@ -5797,7 +5795,7 @@
       </c>
       <c r="S125" s="4"/>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>176</v>
       </c>
@@ -5837,7 +5835,7 @@
       </c>
       <c r="S126" s="4"/>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>182</v>
       </c>
@@ -5880,7 +5878,7 @@
       <c r="R127" s="57"/>
       <c r="S127" s="58"/>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>188</v>
       </c>
@@ -5910,7 +5908,7 @@
       <c r="O128" s="5"/>
       <c r="S128" s="4"/>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A129" s="32">
         <v>194</v>
       </c>
@@ -5954,7 +5952,7 @@
       <c r="R129" s="30"/>
       <c r="S129" s="31"/>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>200</v>
       </c>
@@ -5984,7 +5982,7 @@
       <c r="O130" s="5"/>
       <c r="S130" s="4"/>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131" s="7">
         <v>206</v>
       </c>

</xml_diff>

<commit_message>
MTP033 done. Extra ACS joint obs added. Bug fixed in UVIS nightside COP row reader
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174FD6E3-300C-4722-829C-C0A471CF54B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F1D1F3-2683-4B63-9668-2368C2068D31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -858,7 +858,7 @@
     <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -962,7 +962,6 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1325,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G134" sqref="G134"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1366,22 +1365,22 @@
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="96" t="s">
+      <c r="E3" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="98"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="97"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
-      <c r="O3" s="93" t="s">
+      <c r="O3" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="94"/>
-      <c r="Q3" s="94"/>
-      <c r="R3" s="94"/>
-      <c r="S3" s="95"/>
+      <c r="P3" s="93"/>
+      <c r="Q3" s="93"/>
+      <c r="R3" s="93"/>
+      <c r="S3" s="94"/>
       <c r="V3" s="27" t="s">
         <v>19</v>
       </c>
@@ -1467,7 +1466,7 @@
       <c r="L5" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="M5" s="90">
+      <c r="M5" s="89">
         <v>3973</v>
       </c>
       <c r="N5" s="36" t="s">
@@ -1517,10 +1516,10 @@
       <c r="L6" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="M6" s="91">
+      <c r="M6" s="90">
         <v>674</v>
       </c>
-      <c r="N6" s="92" t="s">
+      <c r="N6" s="91" t="s">
         <v>36</v>
       </c>
       <c r="O6" s="18">
@@ -1529,20 +1528,20 @@
       <c r="P6" s="18">
         <v>30</v>
       </c>
-      <c r="Q6" s="89"/>
+      <c r="Q6" s="88"/>
       <c r="R6" s="7"/>
       <c r="S6" s="8"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="E7" s="84">
+      <c r="E7" s="83">
         <v>23</v>
       </c>
-      <c r="F7" s="85">
-        <v>26</v>
-      </c>
-      <c r="G7" s="86"/>
-      <c r="H7" s="86"/>
-      <c r="I7" s="87"/>
+      <c r="F7" s="84">
+        <v>26</v>
+      </c>
+      <c r="G7" s="85"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="86"/>
       <c r="L7" t="s">
         <v>29</v>
       </c>
@@ -1562,26 +1561,26 @@
       <c r="B10" s="13"/>
       <c r="C10" s="9"/>
       <c r="D10" s="59"/>
-      <c r="E10" s="99" t="s">
+      <c r="E10" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="100"/>
-      <c r="G10" s="100"/>
-      <c r="H10" s="100"/>
-      <c r="I10" s="100"/>
+      <c r="F10" s="99"/>
+      <c r="G10" s="99"/>
+      <c r="H10" s="99"/>
+      <c r="I10" s="99"/>
       <c r="K10" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L10" s="13"/>
       <c r="M10" s="9"/>
       <c r="N10" s="59"/>
-      <c r="O10" s="99" t="s">
+      <c r="O10" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="P10" s="100"/>
-      <c r="Q10" s="100"/>
-      <c r="R10" s="100"/>
-      <c r="S10" s="100"/>
+      <c r="P10" s="99"/>
+      <c r="Q10" s="99"/>
+      <c r="R10" s="99"/>
+      <c r="S10" s="99"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
@@ -2885,26 +2884,26 @@
       <c r="B45" s="13"/>
       <c r="C45" s="9"/>
       <c r="D45" s="59"/>
-      <c r="E45" s="99" t="s">
+      <c r="E45" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="F45" s="100"/>
-      <c r="G45" s="100"/>
-      <c r="H45" s="100"/>
-      <c r="I45" s="100"/>
+      <c r="F45" s="99"/>
+      <c r="G45" s="99"/>
+      <c r="H45" s="99"/>
+      <c r="I45" s="99"/>
       <c r="K45" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L45" s="13"/>
       <c r="M45" s="9"/>
       <c r="N45" s="59"/>
-      <c r="O45" s="99" t="s">
+      <c r="O45" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="P45" s="100"/>
-      <c r="Q45" s="100"/>
-      <c r="R45" s="100"/>
-      <c r="S45" s="100"/>
+      <c r="P45" s="99"/>
+      <c r="Q45" s="99"/>
+      <c r="R45" s="99"/>
+      <c r="S45" s="99"/>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
@@ -4080,26 +4079,26 @@
       <c r="B79" s="13"/>
       <c r="C79" s="9"/>
       <c r="D79" s="33"/>
-      <c r="E79" s="99" t="s">
+      <c r="E79" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="F79" s="100"/>
-      <c r="G79" s="100"/>
-      <c r="H79" s="100"/>
-      <c r="I79" s="100"/>
+      <c r="F79" s="99"/>
+      <c r="G79" s="99"/>
+      <c r="H79" s="99"/>
+      <c r="I79" s="99"/>
       <c r="K79" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L79" s="13"/>
       <c r="M79" s="9"/>
       <c r="N79" s="33"/>
-      <c r="O79" s="99" t="s">
+      <c r="O79" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="P79" s="100"/>
-      <c r="Q79" s="100"/>
-      <c r="R79" s="100"/>
-      <c r="S79" s="100"/>
+      <c r="P79" s="99"/>
+      <c r="Q79" s="99"/>
+      <c r="R79" s="99"/>
+      <c r="S79" s="99"/>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
@@ -4860,7 +4859,7 @@
       <c r="D99" s="61">
         <v>207</v>
       </c>
-      <c r="E99" s="5">
+      <c r="E99" s="2">
         <v>27</v>
       </c>
       <c r="I99" s="4"/>
@@ -4896,7 +4895,7 @@
       <c r="D100" s="61">
         <v>208</v>
       </c>
-      <c r="E100" s="5">
+      <c r="E100" s="2">
         <v>27</v>
       </c>
       <c r="I100" s="4"/>
@@ -4932,7 +4931,7 @@
       <c r="D101" s="61">
         <v>209</v>
       </c>
-      <c r="E101" s="5">
+      <c r="E101" s="2">
         <v>27</v>
       </c>
       <c r="I101" s="4"/>
@@ -4968,7 +4967,7 @@
       <c r="D102" s="61">
         <v>210</v>
       </c>
-      <c r="E102" s="5">
+      <c r="E102" s="2">
         <v>27</v>
       </c>
       <c r="I102" s="4"/>
@@ -5282,26 +5281,26 @@
       </c>
       <c r="B113" s="41"/>
       <c r="C113" s="9"/>
-      <c r="E113" s="99" t="s">
+      <c r="E113" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="F113" s="100"/>
-      <c r="G113" s="100"/>
-      <c r="H113" s="100"/>
-      <c r="I113" s="100"/>
+      <c r="F113" s="99"/>
+      <c r="G113" s="99"/>
+      <c r="H113" s="99"/>
+      <c r="I113" s="99"/>
       <c r="K113" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L113" s="41"/>
       <c r="M113" s="9"/>
       <c r="N113" s="33"/>
-      <c r="O113" s="99" t="s">
+      <c r="O113" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="P113" s="100"/>
-      <c r="Q113" s="100"/>
-      <c r="R113" s="100"/>
-      <c r="S113" s="100"/>
+      <c r="P113" s="99"/>
+      <c r="Q113" s="99"/>
+      <c r="R113" s="99"/>
+      <c r="S113" s="99"/>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" s="9" t="s">
@@ -5501,6 +5500,9 @@
       </c>
       <c r="O118" s="2">
         <v>17</v>
+      </c>
+      <c r="P118" s="3">
+        <v>33</v>
       </c>
       <c r="S118" s="4"/>
     </row>
@@ -5646,7 +5648,9 @@
       <c r="E122" s="2">
         <v>14</v>
       </c>
-      <c r="F122" s="83"/>
+      <c r="F122" s="70">
+        <v>33</v>
+      </c>
       <c r="I122" s="4"/>
       <c r="J122" s="30"/>
       <c r="K122" s="5">
@@ -5731,7 +5735,7 @@
       <c r="E124" s="2">
         <v>18</v>
       </c>
-      <c r="F124" s="88">
+      <c r="F124" s="87">
         <v>28</v>
       </c>
       <c r="I124" s="4"/>
@@ -5771,7 +5775,7 @@
       <c r="E125" s="2">
         <v>18</v>
       </c>
-      <c r="F125" s="88">
+      <c r="F125" s="87">
         <v>28</v>
       </c>
       <c r="I125" s="4"/>
@@ -5891,7 +5895,9 @@
       <c r="D128" s="61">
         <v>233</v>
       </c>
-      <c r="E128" s="5"/>
+      <c r="E128" s="2">
+        <v>33</v>
+      </c>
       <c r="I128" s="4"/>
       <c r="K128" s="5">
         <v>188</v>
@@ -5905,7 +5911,9 @@
       <c r="N128" s="61">
         <v>280</v>
       </c>
-      <c r="O128" s="5"/>
+      <c r="O128" s="2">
+        <v>33</v>
+      </c>
       <c r="S128" s="4"/>
     </row>
     <row r="129" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
MTP034 done; merged/grazing bug fixed; last 2 COP patches added to website
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F1D1F3-2683-4B63-9668-2368C2068D31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776A39BB-C0AB-4DF7-B3C2-7EA89E6B3483}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1324,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F88" sqref="F88"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1463,6 +1463,9 @@
       <c r="I5" s="64">
         <v>22</v>
       </c>
+      <c r="J5" s="71">
+        <v>34</v>
+      </c>
       <c r="L5" s="19" t="s">
         <v>35</v>
       </c>
@@ -1539,7 +1542,9 @@
       <c r="F7" s="84">
         <v>26</v>
       </c>
-      <c r="G7" s="85"/>
+      <c r="G7" s="84">
+        <v>34</v>
+      </c>
       <c r="H7" s="85"/>
       <c r="I7" s="86"/>
       <c r="L7" t="s">

</xml_diff>

<commit_message>
MTP037 COP rows regenerated with extra Mike Smith CO2/CO COP row combinations
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776A39BB-C0AB-4DF7-B3C2-7EA89E6B3483}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0DF539-E3F1-44C0-8480-E8B2467998A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1324,26 +1324,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G117" sqref="G117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.88671875" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.28515625" customWidth="1"/>
-    <col min="22" max="22" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.33203125" customWidth="1"/>
+    <col min="22" max="22" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1351,7 +1351,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="95" t="s">
@@ -1388,7 +1388,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B4" s="13" t="s">
         <v>12</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B5" s="19" t="s">
         <v>1</v>
       </c>
@@ -1489,7 +1489,7 @@
       </c>
       <c r="S5" s="17"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B6" s="20" t="s">
         <v>2</v>
       </c>
@@ -1535,7 +1535,7 @@
       <c r="R6" s="7"/>
       <c r="S6" s="8"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="E7" s="83">
         <v>23</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>0</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>1</v>
       </c>
@@ -1587,7 +1587,7 @@
       <c r="R10" s="99"/>
       <c r="S10" s="99"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="40" t="s">
         <v>10</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="26">
         <v>105</v>
       </c>
@@ -1699,7 +1699,7 @@
       <c r="X12" s="5"/>
       <c r="Y12" s="4"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="25">
         <v>107</v>
       </c>
@@ -1737,7 +1737,7 @@
       <c r="X13" s="5"/>
       <c r="Y13" s="4"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="25">
         <v>120</v>
       </c>
@@ -1775,7 +1775,7 @@
       <c r="X14" s="5"/>
       <c r="Y14" s="4"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="51">
         <v>126</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="25">
         <v>130</v>
       </c>
@@ -1859,7 +1859,7 @@
       <c r="X16" s="49"/>
       <c r="Y16" s="50"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" s="25">
         <v>134</v>
       </c>
@@ -1897,7 +1897,7 @@
       <c r="X17" s="49"/>
       <c r="Y17" s="50"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18" s="51">
         <v>141</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" s="25">
         <v>142</v>
       </c>
@@ -1981,7 +1981,7 @@
       <c r="X19" s="49"/>
       <c r="Y19" s="50"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" s="51">
         <v>146</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" s="25">
         <v>151</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A22" s="25">
         <v>156</v>
       </c>
@@ -2106,7 +2106,7 @@
       <c r="X22" s="49"/>
       <c r="Y22" s="50"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A23" s="51">
         <v>162</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A24" s="25">
         <v>164</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A25" s="25">
         <v>166</v>
       </c>
@@ -2231,7 +2231,7 @@
       <c r="X25" s="49"/>
       <c r="Y25" s="50"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A26" s="25">
         <v>167</v>
       </c>
@@ -2269,7 +2269,7 @@
       <c r="X26" s="49"/>
       <c r="Y26" s="50"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A27" s="25">
         <v>168</v>
       </c>
@@ -2307,7 +2307,7 @@
       <c r="X27" s="49"/>
       <c r="Y27" s="50"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A28" s="25">
         <v>169</v>
       </c>
@@ -2343,7 +2343,7 @@
       <c r="X28" s="49"/>
       <c r="Y28" s="50"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" s="25">
         <v>171</v>
       </c>
@@ -2381,7 +2381,7 @@
       <c r="X29" s="49"/>
       <c r="Y29" s="50"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A30" s="25">
         <v>172</v>
       </c>
@@ -2419,7 +2419,7 @@
       <c r="X30" s="49"/>
       <c r="Y30" s="50"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" s="25">
         <v>178</v>
       </c>
@@ -2457,7 +2457,7 @@
       <c r="X31" s="49"/>
       <c r="Y31" s="50"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A32" s="25">
         <v>180</v>
       </c>
@@ -2495,7 +2495,7 @@
       <c r="X32" s="49"/>
       <c r="Y32" s="50"/>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="25">
         <v>182</v>
       </c>
@@ -2533,7 +2533,7 @@
       <c r="X33" s="49"/>
       <c r="Y33" s="50"/>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="25">
         <v>188</v>
       </c>
@@ -2571,7 +2571,7 @@
       <c r="X34" s="49"/>
       <c r="Y34" s="50"/>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="25">
         <v>191</v>
       </c>
@@ -2609,7 +2609,7 @@
       <c r="X35" s="49"/>
       <c r="Y35" s="50"/>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="51">
         <v>194</v>
       </c>
@@ -2651,7 +2651,7 @@
       <c r="X36" s="49"/>
       <c r="Y36" s="50"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" s="25">
         <v>196</v>
       </c>
@@ -2693,7 +2693,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A38" s="25">
         <v>197</v>
       </c>
@@ -2731,7 +2731,7 @@
       <c r="X38" s="5"/>
       <c r="Y38" s="4"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39" s="25">
         <v>199</v>
       </c>
@@ -2769,7 +2769,7 @@
       <c r="X39" s="5"/>
       <c r="Y39" s="4"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A40" s="25">
         <v>201</v>
       </c>
@@ -2805,7 +2805,7 @@
       <c r="X40" s="5"/>
       <c r="Y40" s="4"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A41" s="34">
         <v>210</v>
       </c>
@@ -2849,7 +2849,7 @@
       <c r="X41" s="5"/>
       <c r="Y41" s="4"/>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="V42" s="5">
         <v>4526.9799999999996</v>
       </c>
@@ -2859,7 +2859,7 @@
       <c r="X42" s="6"/>
       <c r="Y42" s="8"/>
     </row>
-    <row r="43" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:25" ht="18" x14ac:dyDescent="0.35">
       <c r="A43" s="14" t="s">
         <v>0</v>
       </c>
@@ -2871,7 +2871,7 @@
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2882,7 +2882,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>1</v>
       </c>
@@ -2910,7 +2910,7 @@
       <c r="R45" s="99"/>
       <c r="S45" s="99"/>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
         <v>10</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A47" s="72">
         <v>119</v>
       </c>
@@ -3000,7 +3000,7 @@
       </c>
       <c r="S47" s="4"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <f>A47+3</f>
         <v>122</v>
@@ -3034,7 +3034,7 @@
       <c r="O48" s="5"/>
       <c r="S48" s="4"/>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" s="29">
         <f t="shared" ref="A49:A75" si="0">A48+3</f>
         <v>125</v>
@@ -3083,7 +3083,7 @@
       <c r="R49" s="30"/>
       <c r="S49" s="31"/>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <f t="shared" si="0"/>
         <v>128</v>
@@ -3117,7 +3117,7 @@
       <c r="O50" s="5"/>
       <c r="S50" s="4"/>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <f t="shared" si="0"/>
         <v>131</v>
@@ -3151,7 +3151,7 @@
       <c r="O51" s="5"/>
       <c r="S51" s="4"/>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" s="72">
         <f t="shared" si="0"/>
         <v>134</v>
@@ -3189,7 +3189,7 @@
       </c>
       <c r="S52" s="4"/>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <f t="shared" si="0"/>
         <v>137</v>
@@ -3223,7 +3223,7 @@
       <c r="O53" s="5"/>
       <c r="S53" s="4"/>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54" s="29">
         <f t="shared" si="0"/>
         <v>140</v>
@@ -3272,7 +3272,7 @@
       <c r="R54" s="30"/>
       <c r="S54" s="31"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <f t="shared" si="0"/>
         <v>143</v>
@@ -3306,7 +3306,7 @@
       <c r="O55" s="5"/>
       <c r="S55" s="4"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" s="29">
         <f t="shared" si="0"/>
         <v>146</v>
@@ -3355,7 +3355,7 @@
       <c r="R56" s="30"/>
       <c r="S56" s="31"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <f t="shared" si="0"/>
         <v>149</v>
@@ -3389,7 +3389,7 @@
       <c r="O57" s="5"/>
       <c r="S57" s="4"/>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <f t="shared" si="0"/>
         <v>152</v>
@@ -3423,7 +3423,7 @@
       <c r="O58" s="35"/>
       <c r="S58" s="4"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <f t="shared" si="0"/>
         <v>155</v>
@@ -3457,7 +3457,7 @@
       <c r="O59" s="5"/>
       <c r="S59" s="4"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <f t="shared" si="0"/>
         <v>158</v>
@@ -3491,7 +3491,7 @@
       <c r="O60" s="5"/>
       <c r="S60" s="4"/>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61" s="29">
         <f t="shared" si="0"/>
         <v>161</v>
@@ -3540,7 +3540,7 @@
       <c r="R61" s="30"/>
       <c r="S61" s="31"/>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" s="72">
         <f t="shared" si="0"/>
         <v>164</v>
@@ -3584,7 +3584,7 @@
       </c>
       <c r="S62" s="4"/>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63" s="72">
         <f t="shared" si="0"/>
         <v>167</v>
@@ -3622,7 +3622,7 @@
       </c>
       <c r="S63" s="4"/>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" s="72">
         <f t="shared" si="0"/>
         <v>170</v>
@@ -3656,7 +3656,7 @@
       <c r="O64" s="5"/>
       <c r="S64" s="4"/>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A65" s="72">
         <f t="shared" si="0"/>
         <v>173</v>
@@ -3690,7 +3690,7 @@
       <c r="O65" s="5"/>
       <c r="S65" s="4"/>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A66" s="72">
         <f t="shared" si="0"/>
         <v>176</v>
@@ -3724,7 +3724,7 @@
       <c r="O66" s="5"/>
       <c r="S66" s="4"/>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A67" s="72">
         <f t="shared" si="0"/>
         <v>179</v>
@@ -3758,7 +3758,7 @@
       <c r="O67" s="5"/>
       <c r="S67" s="4"/>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A68" s="72">
         <f t="shared" si="0"/>
         <v>182</v>
@@ -3792,7 +3792,7 @@
       <c r="O68" s="5"/>
       <c r="S68" s="4"/>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A69" s="72">
         <f t="shared" si="0"/>
         <v>185</v>
@@ -3830,7 +3830,7 @@
       </c>
       <c r="S69" s="4"/>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A70" s="72">
         <f t="shared" si="0"/>
         <v>188</v>
@@ -3868,7 +3868,7 @@
       </c>
       <c r="S70" s="4"/>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A71" s="5">
         <f t="shared" si="0"/>
         <v>191</v>
@@ -3902,7 +3902,7 @@
       <c r="O71" s="5"/>
       <c r="S71" s="4"/>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A72" s="29">
         <f t="shared" si="0"/>
         <v>194</v>
@@ -3947,7 +3947,7 @@
       <c r="R72" s="30"/>
       <c r="S72" s="31"/>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A73" s="5">
         <f t="shared" si="0"/>
         <v>197</v>
@@ -3981,7 +3981,7 @@
       <c r="O73" s="5"/>
       <c r="S73" s="4"/>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A74" s="5">
         <f t="shared" si="0"/>
         <v>200</v>
@@ -4015,7 +4015,7 @@
       <c r="O74" s="5"/>
       <c r="S74" s="4"/>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A75" s="6">
         <f t="shared" si="0"/>
         <v>203</v>
@@ -4055,7 +4055,7 @@
       <c r="R75" s="7"/>
       <c r="S75" s="8"/>
     </row>
-    <row r="77" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A77" s="14" t="s">
         <v>0</v>
       </c>
@@ -4069,7 +4069,7 @@
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -4077,7 +4077,7 @@
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A79" s="9" t="s">
         <v>1</v>
       </c>
@@ -4105,7 +4105,7 @@
       <c r="R79" s="99"/>
       <c r="S79" s="99"/>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A80" s="9" t="s">
         <v>10</v>
       </c>
@@ -4161,7 +4161,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A81" s="5">
         <v>119</v>
       </c>
@@ -4191,7 +4191,7 @@
       <c r="O81" s="5"/>
       <c r="S81" s="4"/>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A82" s="5">
         <f>A81+3</f>
         <v>122</v>
@@ -4229,7 +4229,7 @@
       </c>
       <c r="S82" s="4"/>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A83" s="29">
         <f t="shared" ref="A83:A109" si="5">A82+3</f>
         <v>125</v>
@@ -4274,7 +4274,7 @@
       <c r="R83" s="30"/>
       <c r="S83" s="31"/>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A84" s="5">
         <f t="shared" si="5"/>
         <v>128</v>
@@ -4308,7 +4308,7 @@
       <c r="O84" s="5"/>
       <c r="S84" s="4"/>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A85" s="5">
         <f t="shared" si="5"/>
         <v>131</v>
@@ -4342,7 +4342,7 @@
       <c r="O85" s="5"/>
       <c r="S85" s="4"/>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="5">
         <f t="shared" si="5"/>
         <v>134</v>
@@ -4376,7 +4376,7 @@
       <c r="O86" s="5"/>
       <c r="S86" s="4"/>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A87" s="5">
         <f t="shared" si="5"/>
         <v>137</v>
@@ -4414,7 +4414,7 @@
       </c>
       <c r="S87" s="4"/>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A88" s="29">
         <f t="shared" si="5"/>
         <v>140</v>
@@ -4463,7 +4463,7 @@
       <c r="R88" s="30"/>
       <c r="S88" s="31"/>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A89" s="5">
         <f t="shared" si="5"/>
         <v>143</v>
@@ -4497,7 +4497,7 @@
       <c r="O89" s="5"/>
       <c r="S89" s="4"/>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A90" s="29">
         <f t="shared" si="5"/>
         <v>146</v>
@@ -4544,7 +4544,7 @@
       <c r="R90" s="30"/>
       <c r="S90" s="31"/>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A91" s="29">
         <f t="shared" si="5"/>
         <v>149</v>
@@ -4586,7 +4586,7 @@
       <c r="R91" s="30"/>
       <c r="S91" s="31"/>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A92" s="5">
         <f t="shared" si="5"/>
         <v>152</v>
@@ -4620,7 +4620,7 @@
       <c r="O92" s="35"/>
       <c r="S92" s="4"/>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A93" s="5">
         <f t="shared" si="5"/>
         <v>155</v>
@@ -4654,7 +4654,7 @@
       <c r="O93" s="5"/>
       <c r="S93" s="4"/>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A94" s="5">
         <f t="shared" si="5"/>
         <v>158</v>
@@ -4692,7 +4692,7 @@
       </c>
       <c r="S94" s="4"/>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A95" s="29">
         <f t="shared" si="5"/>
         <v>161</v>
@@ -4739,7 +4739,7 @@
       <c r="R95" s="30"/>
       <c r="S95" s="31"/>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A96" s="5">
         <f t="shared" si="5"/>
         <v>164</v>
@@ -4773,7 +4773,7 @@
       <c r="O96" s="5"/>
       <c r="S96" s="4"/>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <f t="shared" si="5"/>
         <v>167</v>
@@ -4811,7 +4811,7 @@
       </c>
       <c r="S97" s="4"/>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A98" s="5">
         <f t="shared" si="5"/>
         <v>170</v>
@@ -4849,7 +4849,7 @@
       </c>
       <c r="S98" s="4"/>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A99" s="5">
         <f t="shared" si="5"/>
         <v>173</v>
@@ -4885,7 +4885,7 @@
       <c r="O99" s="5"/>
       <c r="S99" s="4"/>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A100" s="5">
         <f t="shared" si="5"/>
         <v>176</v>
@@ -4921,7 +4921,7 @@
       <c r="O100" s="5"/>
       <c r="S100" s="4"/>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A101" s="5">
         <f t="shared" si="5"/>
         <v>179</v>
@@ -4957,7 +4957,7 @@
       <c r="O101" s="5"/>
       <c r="S101" s="4"/>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A102" s="5">
         <f t="shared" si="5"/>
         <v>182</v>
@@ -4993,7 +4993,7 @@
       <c r="O102" s="5"/>
       <c r="S102" s="4"/>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A103" s="5">
         <f t="shared" si="5"/>
         <v>185</v>
@@ -5027,7 +5027,7 @@
       <c r="O103" s="5"/>
       <c r="S103" s="4"/>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A104" s="5">
         <f t="shared" si="5"/>
         <v>188</v>
@@ -5061,7 +5061,7 @@
       <c r="O104" s="5"/>
       <c r="S104" s="4"/>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A105" s="5">
         <f t="shared" si="5"/>
         <v>191</v>
@@ -5099,7 +5099,7 @@
       </c>
       <c r="S105" s="4"/>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A106" s="29">
         <f t="shared" si="5"/>
         <v>194</v>
@@ -5148,7 +5148,7 @@
       <c r="R106" s="30"/>
       <c r="S106" s="31"/>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A107" s="5">
         <f t="shared" si="5"/>
         <v>197</v>
@@ -5186,7 +5186,7 @@
       </c>
       <c r="S107" s="4"/>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A108" s="5">
         <f t="shared" si="5"/>
         <v>200</v>
@@ -5220,7 +5220,7 @@
       <c r="O108" s="5"/>
       <c r="S108" s="4"/>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A109" s="6">
         <f t="shared" si="5"/>
         <v>203</v>
@@ -5260,7 +5260,7 @@
       <c r="R109" s="7"/>
       <c r="S109" s="8"/>
     </row>
-    <row r="111" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A111" s="14" t="s">
         <v>0</v>
       </c>
@@ -5272,7 +5272,7 @@
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -5280,7 +5280,7 @@
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A113" s="9" t="s">
         <v>1</v>
       </c>
@@ -5307,7 +5307,7 @@
       <c r="R113" s="99"/>
       <c r="S113" s="99"/>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A114" s="9" t="s">
         <v>10</v>
       </c>
@@ -5363,7 +5363,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>110</v>
       </c>
@@ -5397,7 +5397,7 @@
       <c r="R115" s="30"/>
       <c r="S115" s="31"/>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>116</v>
       </c>
@@ -5427,7 +5427,7 @@
       <c r="O116" s="5"/>
       <c r="S116" s="4"/>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A117" s="32">
         <v>122</v>
       </c>
@@ -5446,7 +5446,9 @@
       <c r="F117" s="32">
         <v>12</v>
       </c>
-      <c r="G117" s="30"/>
+      <c r="G117" s="32">
+        <v>37</v>
+      </c>
       <c r="H117" s="30"/>
       <c r="I117" s="31"/>
       <c r="K117" s="29">
@@ -5471,7 +5473,7 @@
       <c r="R117" s="30"/>
       <c r="S117" s="31"/>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>128</v>
       </c>
@@ -5511,7 +5513,7 @@
       </c>
       <c r="S118" s="4"/>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>134</v>
       </c>
@@ -5546,9 +5548,12 @@
       <c r="O119" s="2">
         <v>17</v>
       </c>
+      <c r="P119" s="3">
+        <v>37</v>
+      </c>
       <c r="S119" s="4"/>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A120" s="32">
         <v>140</v>
       </c>
@@ -5593,7 +5598,7 @@
       <c r="R120" s="30"/>
       <c r="S120" s="31"/>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A121" s="32">
         <v>146</v>
       </c>
@@ -5637,7 +5642,7 @@
       <c r="R121" s="30"/>
       <c r="S121" s="31"/>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>152</v>
       </c>
@@ -5680,7 +5685,7 @@
       <c r="R122" s="30"/>
       <c r="S122" s="31"/>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A123" s="32">
         <v>158</v>
       </c>
@@ -5724,7 +5729,7 @@
       <c r="R123" s="30"/>
       <c r="S123" s="31"/>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>164</v>
       </c>
@@ -5764,7 +5769,7 @@
       </c>
       <c r="S124" s="4"/>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>170</v>
       </c>
@@ -5804,7 +5809,7 @@
       </c>
       <c r="S125" s="4"/>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>176</v>
       </c>
@@ -5844,7 +5849,7 @@
       </c>
       <c r="S126" s="4"/>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>182</v>
       </c>
@@ -5887,7 +5892,7 @@
       <c r="R127" s="57"/>
       <c r="S127" s="58"/>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>188</v>
       </c>
@@ -5902,6 +5907,9 @@
       </c>
       <c r="E128" s="2">
         <v>33</v>
+      </c>
+      <c r="F128" s="3">
+        <v>37</v>
       </c>
       <c r="I128" s="4"/>
       <c r="K128" s="5">
@@ -5919,9 +5927,12 @@
       <c r="O128" s="2">
         <v>33</v>
       </c>
+      <c r="P128" s="32">
+        <v>37</v>
+      </c>
       <c r="S128" s="4"/>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A129" s="32">
         <v>194</v>
       </c>
@@ -5965,7 +5976,7 @@
       <c r="R129" s="30"/>
       <c r="S129" s="31"/>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>200</v>
       </c>
@@ -5995,7 +6006,7 @@
       <c r="O130" s="5"/>
       <c r="S130" s="4"/>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A131" s="7">
         <v>206</v>
       </c>

</xml_diff>

<commit_message>
MTP038 COP rows delivered
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0DF539-E3F1-44C0-8480-E8B2467998A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B08A73-96DF-4795-BD61-61172703BBE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1324,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G117" sqref="G117"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O104" sqref="O104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5008,7 +5008,9 @@
       <c r="D103" s="61">
         <v>211</v>
       </c>
-      <c r="E103" s="5"/>
+      <c r="E103" s="2">
+        <v>38</v>
+      </c>
       <c r="I103" s="4"/>
       <c r="K103" s="5">
         <f t="shared" si="7"/>
@@ -5024,7 +5026,9 @@
       <c r="N103" s="60">
         <v>258</v>
       </c>
-      <c r="O103" s="5"/>
+      <c r="O103" s="2">
+        <v>38</v>
+      </c>
       <c r="S103" s="4"/>
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.3">
@@ -5042,7 +5046,9 @@
       <c r="D104" s="61">
         <v>212</v>
       </c>
-      <c r="E104" s="5"/>
+      <c r="E104" s="2">
+        <v>38</v>
+      </c>
       <c r="I104" s="4"/>
       <c r="K104" s="5">
         <f t="shared" si="7"/>
@@ -5058,7 +5064,9 @@
       <c r="N104" s="60">
         <v>259</v>
       </c>
-      <c r="O104" s="5"/>
+      <c r="O104" s="2">
+        <v>38</v>
+      </c>
       <c r="S104" s="4"/>
     </row>
     <row r="105" spans="1:19" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Final MTP039 COP rows delivered
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B08A73-96DF-4795-BD61-61172703BBE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BC9D1C-460E-4FFE-BC54-B1644E090163}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -858,7 +858,7 @@
     <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -964,7 +964,6 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1324,8 +1323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O104" sqref="O104"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1365,22 +1364,22 @@
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="95" t="s">
+      <c r="E3" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="97"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="96"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
-      <c r="O3" s="92" t="s">
+      <c r="O3" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="93"/>
-      <c r="Q3" s="93"/>
-      <c r="R3" s="93"/>
-      <c r="S3" s="94"/>
+      <c r="P3" s="92"/>
+      <c r="Q3" s="92"/>
+      <c r="R3" s="92"/>
+      <c r="S3" s="93"/>
       <c r="V3" s="27" t="s">
         <v>19</v>
       </c>
@@ -1469,7 +1468,7 @@
       <c r="L5" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="M5" s="89">
+      <c r="M5" s="88">
         <v>3973</v>
       </c>
       <c r="N5" s="36" t="s">
@@ -1519,10 +1518,10 @@
       <c r="L6" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="M6" s="90">
+      <c r="M6" s="89">
         <v>674</v>
       </c>
-      <c r="N6" s="91" t="s">
+      <c r="N6" s="90" t="s">
         <v>36</v>
       </c>
       <c r="O6" s="18">
@@ -1531,7 +1530,7 @@
       <c r="P6" s="18">
         <v>30</v>
       </c>
-      <c r="Q6" s="88"/>
+      <c r="Q6" s="87"/>
       <c r="R6" s="7"/>
       <c r="S6" s="8"/>
     </row>
@@ -1545,8 +1544,10 @@
       <c r="G7" s="84">
         <v>34</v>
       </c>
-      <c r="H7" s="85"/>
-      <c r="I7" s="86"/>
+      <c r="H7" s="84">
+        <v>39</v>
+      </c>
+      <c r="I7" s="85"/>
       <c r="L7" t="s">
         <v>29</v>
       </c>
@@ -1566,26 +1567,26 @@
       <c r="B10" s="13"/>
       <c r="C10" s="9"/>
       <c r="D10" s="59"/>
-      <c r="E10" s="98" t="s">
+      <c r="E10" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="99"/>
-      <c r="G10" s="99"/>
-      <c r="H10" s="99"/>
-      <c r="I10" s="99"/>
+      <c r="F10" s="98"/>
+      <c r="G10" s="98"/>
+      <c r="H10" s="98"/>
+      <c r="I10" s="98"/>
       <c r="K10" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L10" s="13"/>
       <c r="M10" s="9"/>
       <c r="N10" s="59"/>
-      <c r="O10" s="98" t="s">
+      <c r="O10" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="P10" s="99"/>
-      <c r="Q10" s="99"/>
-      <c r="R10" s="99"/>
-      <c r="S10" s="99"/>
+      <c r="P10" s="98"/>
+      <c r="Q10" s="98"/>
+      <c r="R10" s="98"/>
+      <c r="S10" s="98"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="40" t="s">
@@ -2889,26 +2890,26 @@
       <c r="B45" s="13"/>
       <c r="C45" s="9"/>
       <c r="D45" s="59"/>
-      <c r="E45" s="98" t="s">
+      <c r="E45" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="F45" s="99"/>
-      <c r="G45" s="99"/>
-      <c r="H45" s="99"/>
-      <c r="I45" s="99"/>
+      <c r="F45" s="98"/>
+      <c r="G45" s="98"/>
+      <c r="H45" s="98"/>
+      <c r="I45" s="98"/>
       <c r="K45" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L45" s="13"/>
       <c r="M45" s="9"/>
       <c r="N45" s="59"/>
-      <c r="O45" s="98" t="s">
+      <c r="O45" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="P45" s="99"/>
-      <c r="Q45" s="99"/>
-      <c r="R45" s="99"/>
-      <c r="S45" s="99"/>
+      <c r="P45" s="98"/>
+      <c r="Q45" s="98"/>
+      <c r="R45" s="98"/>
+      <c r="S45" s="98"/>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
@@ -4084,26 +4085,26 @@
       <c r="B79" s="13"/>
       <c r="C79" s="9"/>
       <c r="D79" s="33"/>
-      <c r="E79" s="98" t="s">
+      <c r="E79" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="F79" s="99"/>
-      <c r="G79" s="99"/>
-      <c r="H79" s="99"/>
-      <c r="I79" s="99"/>
+      <c r="F79" s="98"/>
+      <c r="G79" s="98"/>
+      <c r="H79" s="98"/>
+      <c r="I79" s="98"/>
       <c r="K79" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L79" s="13"/>
       <c r="M79" s="9"/>
       <c r="N79" s="33"/>
-      <c r="O79" s="98" t="s">
+      <c r="O79" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="P79" s="99"/>
-      <c r="Q79" s="99"/>
-      <c r="R79" s="99"/>
-      <c r="S79" s="99"/>
+      <c r="P79" s="98"/>
+      <c r="Q79" s="98"/>
+      <c r="R79" s="98"/>
+      <c r="S79" s="98"/>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A80" s="9" t="s">
@@ -4494,7 +4495,9 @@
       <c r="N89" s="60">
         <v>244</v>
       </c>
-      <c r="O89" s="5"/>
+      <c r="O89" s="2">
+        <v>39</v>
+      </c>
       <c r="S89" s="4"/>
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.3">
@@ -4882,7 +4885,9 @@
       <c r="N99" s="60">
         <v>254</v>
       </c>
-      <c r="O99" s="5"/>
+      <c r="O99" s="2">
+        <v>39</v>
+      </c>
       <c r="S99" s="4"/>
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.3">
@@ -5294,26 +5299,26 @@
       </c>
       <c r="B113" s="41"/>
       <c r="C113" s="9"/>
-      <c r="E113" s="98" t="s">
+      <c r="E113" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="F113" s="99"/>
-      <c r="G113" s="99"/>
-      <c r="H113" s="99"/>
-      <c r="I113" s="99"/>
+      <c r="F113" s="98"/>
+      <c r="G113" s="98"/>
+      <c r="H113" s="98"/>
+      <c r="I113" s="98"/>
       <c r="K113" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L113" s="41"/>
       <c r="M113" s="9"/>
       <c r="N113" s="33"/>
-      <c r="O113" s="98" t="s">
+      <c r="O113" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="P113" s="99"/>
-      <c r="Q113" s="99"/>
-      <c r="R113" s="99"/>
-      <c r="S113" s="99"/>
+      <c r="P113" s="98"/>
+      <c r="Q113" s="98"/>
+      <c r="R113" s="98"/>
+      <c r="S113" s="98"/>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A114" s="9" t="s">
@@ -5753,7 +5758,7 @@
       <c r="E124" s="2">
         <v>18</v>
       </c>
-      <c r="F124" s="87">
+      <c r="F124" s="86">
         <v>28</v>
       </c>
       <c r="I124" s="4"/>
@@ -5793,7 +5798,7 @@
       <c r="E125" s="2">
         <v>18</v>
       </c>
-      <c r="F125" s="87">
+      <c r="F125" s="86">
         <v>28</v>
       </c>
       <c r="I125" s="4"/>

</xml_diff>

<commit_message>
Old COP tables added to repo, empty MRO overlap orbit files added to old MTPs, local sqlite db now generated if no access to BIRA server
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BC9D1C-460E-4FFE-BC54-B1644E090163}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC3B57F-1AFA-4FA5-87CE-720C358AA539}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1323,8 +1323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N126" sqref="N126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5841,6 +5841,9 @@
       <c r="F126" s="3">
         <v>28</v>
       </c>
+      <c r="G126" s="3">
+        <v>40</v>
+      </c>
       <c r="I126" s="4"/>
       <c r="K126" s="5">
         <v>176</v>
@@ -5859,6 +5862,9 @@
       </c>
       <c r="P126" s="32">
         <v>31</v>
+      </c>
+      <c r="Q126">
+        <v>40</v>
       </c>
       <c r="S126" s="4"/>
     </row>
@@ -5924,6 +5930,9 @@
       <c r="F128" s="3">
         <v>37</v>
       </c>
+      <c r="G128" s="3">
+        <v>40</v>
+      </c>
       <c r="I128" s="4"/>
       <c r="K128" s="5">
         <v>188</v>
@@ -5942,6 +5951,9 @@
       </c>
       <c r="P128" s="32">
         <v>37</v>
+      </c>
+      <c r="Q128">
+        <v>40</v>
       </c>
       <c r="S128" s="4"/>
     </row>

</xml_diff>

<commit_message>
MTP041 done; all MTPs reprocessed to add obs info to sqlite db
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC3B57F-1AFA-4FA5-87CE-720C358AA539}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB93B20-3A3E-4ED4-AD27-8DA384D3877C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1323,8 +1323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N126" sqref="N126"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K133" sqref="K133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5842,7 +5842,7 @@
         <v>28</v>
       </c>
       <c r="G126" s="3">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I126" s="4"/>
       <c r="K126" s="5">
@@ -5863,8 +5863,8 @@
       <c r="P126" s="32">
         <v>31</v>
       </c>
-      <c r="Q126">
-        <v>40</v>
+      <c r="Q126" s="3">
+        <v>41</v>
       </c>
       <c r="S126" s="4"/>
     </row>
@@ -5886,6 +5886,9 @@
       </c>
       <c r="F127" s="3">
         <v>28</v>
+      </c>
+      <c r="G127">
+        <v>42</v>
       </c>
       <c r="I127" s="4"/>
       <c r="J127" s="30"/>
@@ -5907,7 +5910,9 @@
       <c r="P127" s="32">
         <v>31</v>
       </c>
-      <c r="Q127" s="57"/>
+      <c r="Q127" s="57">
+        <v>42</v>
+      </c>
       <c r="R127" s="57"/>
       <c r="S127" s="58"/>
     </row>
@@ -5931,7 +5936,7 @@
         <v>37</v>
       </c>
       <c r="G128" s="3">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I128" s="4"/>
       <c r="K128" s="5">
@@ -5952,8 +5957,8 @@
       <c r="P128" s="32">
         <v>37</v>
       </c>
-      <c r="Q128">
-        <v>40</v>
+      <c r="Q128" s="3">
+        <v>41</v>
       </c>
       <c r="S128" s="4"/>
     </row>
@@ -5976,7 +5981,9 @@
       <c r="F129" s="32">
         <v>12</v>
       </c>
-      <c r="G129" s="30"/>
+      <c r="G129" s="30">
+        <v>42</v>
+      </c>
       <c r="H129" s="30"/>
       <c r="I129" s="31"/>
       <c r="K129" s="29">
@@ -5997,7 +6004,9 @@
       <c r="P129" s="32">
         <v>31</v>
       </c>
-      <c r="Q129" s="30"/>
+      <c r="Q129" s="30">
+        <v>42</v>
+      </c>
       <c r="R129" s="30"/>
       <c r="S129" s="31"/>
     </row>

</xml_diff>

<commit_message>
MTP044 orbit plan and COP rows generated
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB93B20-3A3E-4ED4-AD27-8DA384D3877C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D0D3D0-E96A-4FE0-99C5-14FFF0AB3EE6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1323,8 +1323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K133" sqref="K133"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2585,7 +2585,9 @@
       <c r="D35" s="61">
         <v>77</v>
       </c>
-      <c r="E35" s="5"/>
+      <c r="E35" s="2">
+        <v>43</v>
+      </c>
       <c r="I35" s="4"/>
       <c r="K35" s="25">
         <v>191</v>
@@ -2599,7 +2601,9 @@
       <c r="N35" s="61">
         <v>124</v>
       </c>
-      <c r="O35" s="5"/>
+      <c r="O35" s="2">
+        <v>43</v>
+      </c>
       <c r="S35" s="4"/>
       <c r="V35" s="5">
         <v>4242.13</v>
@@ -2626,6 +2630,9 @@
       <c r="E36" s="2">
         <v>13</v>
       </c>
+      <c r="F36" s="3">
+        <v>43</v>
+      </c>
       <c r="I36" s="4"/>
       <c r="K36" s="51">
         <v>194</v>
@@ -2641,6 +2648,9 @@
       </c>
       <c r="O36" s="2">
         <v>13</v>
+      </c>
+      <c r="P36" s="3">
+        <v>43</v>
       </c>
       <c r="S36" s="4"/>
       <c r="V36" s="5">

</xml_diff>

<commit_message>
MTP044 COP rows sent
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D0D3D0-E96A-4FE0-99C5-14FFF0AB3EE6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12DC61D-16F9-4E2A-9A37-5DBC9FC8498D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="4968" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -858,7 +858,7 @@
     <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -966,7 +966,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1324,7 +1323,7 @@
   <dimension ref="A1:AB131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1364,22 +1363,22 @@
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="94" t="s">
+      <c r="E3" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="96"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="95"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
-      <c r="O3" s="91" t="s">
+      <c r="O3" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="92"/>
-      <c r="R3" s="92"/>
-      <c r="S3" s="93"/>
+      <c r="P3" s="91"/>
+      <c r="Q3" s="91"/>
+      <c r="R3" s="91"/>
+      <c r="S3" s="92"/>
       <c r="V3" s="27" t="s">
         <v>19</v>
       </c>
@@ -1468,7 +1467,7 @@
       <c r="L5" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="M5" s="88">
+      <c r="M5" s="87">
         <v>3973</v>
       </c>
       <c r="N5" s="36" t="s">
@@ -1518,10 +1517,10 @@
       <c r="L6" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="M6" s="89">
+      <c r="M6" s="88">
         <v>674</v>
       </c>
-      <c r="N6" s="90" t="s">
+      <c r="N6" s="89" t="s">
         <v>36</v>
       </c>
       <c r="O6" s="18">
@@ -1530,7 +1529,9 @@
       <c r="P6" s="18">
         <v>30</v>
       </c>
-      <c r="Q6" s="87"/>
+      <c r="Q6" s="18">
+        <v>44</v>
+      </c>
       <c r="R6" s="7"/>
       <c r="S6" s="8"/>
     </row>
@@ -1567,26 +1568,26 @@
       <c r="B10" s="13"/>
       <c r="C10" s="9"/>
       <c r="D10" s="59"/>
-      <c r="E10" s="97" t="s">
+      <c r="E10" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="98"/>
-      <c r="G10" s="98"/>
-      <c r="H10" s="98"/>
-      <c r="I10" s="98"/>
+      <c r="F10" s="97"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="97"/>
+      <c r="I10" s="97"/>
       <c r="K10" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L10" s="13"/>
       <c r="M10" s="9"/>
       <c r="N10" s="59"/>
-      <c r="O10" s="97" t="s">
+      <c r="O10" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="P10" s="98"/>
-      <c r="Q10" s="98"/>
-      <c r="R10" s="98"/>
-      <c r="S10" s="98"/>
+      <c r="P10" s="97"/>
+      <c r="Q10" s="97"/>
+      <c r="R10" s="97"/>
+      <c r="S10" s="97"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="40" t="s">
@@ -2900,26 +2901,26 @@
       <c r="B45" s="13"/>
       <c r="C45" s="9"/>
       <c r="D45" s="59"/>
-      <c r="E45" s="97" t="s">
+      <c r="E45" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="F45" s="98"/>
-      <c r="G45" s="98"/>
-      <c r="H45" s="98"/>
-      <c r="I45" s="98"/>
+      <c r="F45" s="97"/>
+      <c r="G45" s="97"/>
+      <c r="H45" s="97"/>
+      <c r="I45" s="97"/>
       <c r="K45" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L45" s="13"/>
       <c r="M45" s="9"/>
       <c r="N45" s="59"/>
-      <c r="O45" s="97" t="s">
+      <c r="O45" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="P45" s="98"/>
-      <c r="Q45" s="98"/>
-      <c r="R45" s="98"/>
-      <c r="S45" s="98"/>
+      <c r="P45" s="97"/>
+      <c r="Q45" s="97"/>
+      <c r="R45" s="97"/>
+      <c r="S45" s="97"/>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
@@ -4095,26 +4096,26 @@
       <c r="B79" s="13"/>
       <c r="C79" s="9"/>
       <c r="D79" s="33"/>
-      <c r="E79" s="97" t="s">
+      <c r="E79" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="F79" s="98"/>
-      <c r="G79" s="98"/>
-      <c r="H79" s="98"/>
-      <c r="I79" s="98"/>
+      <c r="F79" s="97"/>
+      <c r="G79" s="97"/>
+      <c r="H79" s="97"/>
+      <c r="I79" s="97"/>
       <c r="K79" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L79" s="13"/>
       <c r="M79" s="9"/>
       <c r="N79" s="33"/>
-      <c r="O79" s="97" t="s">
+      <c r="O79" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="P79" s="98"/>
-      <c r="Q79" s="98"/>
-      <c r="R79" s="98"/>
-      <c r="S79" s="98"/>
+      <c r="P79" s="97"/>
+      <c r="Q79" s="97"/>
+      <c r="R79" s="97"/>
+      <c r="S79" s="97"/>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A80" s="9" t="s">
@@ -5309,26 +5310,26 @@
       </c>
       <c r="B113" s="41"/>
       <c r="C113" s="9"/>
-      <c r="E113" s="97" t="s">
+      <c r="E113" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="F113" s="98"/>
-      <c r="G113" s="98"/>
-      <c r="H113" s="98"/>
-      <c r="I113" s="98"/>
+      <c r="F113" s="97"/>
+      <c r="G113" s="97"/>
+      <c r="H113" s="97"/>
+      <c r="I113" s="97"/>
       <c r="K113" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L113" s="41"/>
       <c r="M113" s="9"/>
       <c r="N113" s="33"/>
-      <c r="O113" s="97" t="s">
+      <c r="O113" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="P113" s="98"/>
-      <c r="Q113" s="98"/>
-      <c r="R113" s="98"/>
-      <c r="S113" s="98"/>
+      <c r="P113" s="97"/>
+      <c r="Q113" s="97"/>
+      <c r="R113" s="97"/>
+      <c r="S113" s="97"/>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A114" s="9" t="s">

</xml_diff>

<commit_message>
MTP046 COP rows made
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12DC61D-16F9-4E2A-9A37-5DBC9FC8498D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFFA6BD-4B3A-4907-8D2C-2B4949DE8B30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="4968" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1322,26 +1322,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N61" sqref="N61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.88671875" customWidth="1"/>
-    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.33203125" customWidth="1"/>
-    <col min="22" max="22" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.28515625" customWidth="1"/>
+    <col min="22" max="22" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1349,7 +1349,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:25" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="93" t="s">
@@ -1386,7 +1386,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>12</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
         <v>1</v>
       </c>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="S5" s="17"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
         <v>2</v>
       </c>
@@ -1535,7 +1535,7 @@
       <c r="R6" s="7"/>
       <c r="S6" s="8"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E7" s="83">
         <v>23</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>0</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>1</v>
       </c>
@@ -1589,7 +1589,7 @@
       <c r="R10" s="97"/>
       <c r="S10" s="97"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
         <v>10</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
         <v>105</v>
       </c>
@@ -1701,7 +1701,7 @@
       <c r="X12" s="5"/>
       <c r="Y12" s="4"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="25">
         <v>107</v>
       </c>
@@ -1739,7 +1739,7 @@
       <c r="X13" s="5"/>
       <c r="Y13" s="4"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="25">
         <v>120</v>
       </c>
@@ -1777,7 +1777,7 @@
       <c r="X14" s="5"/>
       <c r="Y14" s="4"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="51">
         <v>126</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="25">
         <v>130</v>
       </c>
@@ -1861,7 +1861,7 @@
       <c r="X16" s="49"/>
       <c r="Y16" s="50"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="25">
         <v>134</v>
       </c>
@@ -1899,7 +1899,7 @@
       <c r="X17" s="49"/>
       <c r="Y17" s="50"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="51">
         <v>141</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="25">
         <v>142</v>
       </c>
@@ -1983,7 +1983,7 @@
       <c r="X19" s="49"/>
       <c r="Y19" s="50"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="51">
         <v>146</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="25">
         <v>151</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="25">
         <v>156</v>
       </c>
@@ -2108,7 +2108,7 @@
       <c r="X22" s="49"/>
       <c r="Y22" s="50"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="51">
         <v>162</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="25">
         <v>164</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="25">
         <v>166</v>
       </c>
@@ -2233,7 +2233,7 @@
       <c r="X25" s="49"/>
       <c r="Y25" s="50"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="25">
         <v>167</v>
       </c>
@@ -2271,7 +2271,7 @@
       <c r="X26" s="49"/>
       <c r="Y26" s="50"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="25">
         <v>168</v>
       </c>
@@ -2309,7 +2309,7 @@
       <c r="X27" s="49"/>
       <c r="Y27" s="50"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="25">
         <v>169</v>
       </c>
@@ -2345,7 +2345,7 @@
       <c r="X28" s="49"/>
       <c r="Y28" s="50"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="25">
         <v>171</v>
       </c>
@@ -2383,7 +2383,7 @@
       <c r="X29" s="49"/>
       <c r="Y29" s="50"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="25">
         <v>172</v>
       </c>
@@ -2421,7 +2421,7 @@
       <c r="X30" s="49"/>
       <c r="Y30" s="50"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="25">
         <v>178</v>
       </c>
@@ -2459,7 +2459,7 @@
       <c r="X31" s="49"/>
       <c r="Y31" s="50"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="25">
         <v>180</v>
       </c>
@@ -2497,7 +2497,7 @@
       <c r="X32" s="49"/>
       <c r="Y32" s="50"/>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="25">
         <v>182</v>
       </c>
@@ -2535,7 +2535,7 @@
       <c r="X33" s="49"/>
       <c r="Y33" s="50"/>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="25">
         <v>188</v>
       </c>
@@ -2548,7 +2548,9 @@
       <c r="D34" s="61">
         <v>76</v>
       </c>
-      <c r="E34" s="5"/>
+      <c r="E34" s="2">
+        <v>45</v>
+      </c>
       <c r="I34" s="4"/>
       <c r="K34" s="25">
         <v>188</v>
@@ -2573,7 +2575,7 @@
       <c r="X34" s="49"/>
       <c r="Y34" s="50"/>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="25">
         <v>191</v>
       </c>
@@ -2615,7 +2617,7 @@
       <c r="X35" s="49"/>
       <c r="Y35" s="50"/>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="51">
         <v>194</v>
       </c>
@@ -2663,7 +2665,7 @@
       <c r="X36" s="49"/>
       <c r="Y36" s="50"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="25">
         <v>196</v>
       </c>
@@ -2705,7 +2707,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" s="25">
         <v>197</v>
       </c>
@@ -2743,7 +2745,7 @@
       <c r="X38" s="5"/>
       <c r="Y38" s="4"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" s="25">
         <v>199</v>
       </c>
@@ -2781,7 +2783,7 @@
       <c r="X39" s="5"/>
       <c r="Y39" s="4"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="25">
         <v>201</v>
       </c>
@@ -2817,7 +2819,7 @@
       <c r="X40" s="5"/>
       <c r="Y40" s="4"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="34">
         <v>210</v>
       </c>
@@ -2861,7 +2863,7 @@
       <c r="X41" s="5"/>
       <c r="Y41" s="4"/>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="V42" s="5">
         <v>4526.9799999999996</v>
       </c>
@@ -2871,7 +2873,7 @@
       <c r="X42" s="6"/>
       <c r="Y42" s="8"/>
     </row>
-    <row r="43" spans="1:25" ht="18" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="s">
         <v>0</v>
       </c>
@@ -2883,7 +2885,7 @@
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2894,7 +2896,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>1</v>
       </c>
@@ -2922,7 +2924,7 @@
       <c r="R45" s="97"/>
       <c r="S45" s="97"/>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>10</v>
       </c>
@@ -2978,7 +2980,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="72">
         <v>119</v>
       </c>
@@ -3012,7 +3014,7 @@
       </c>
       <c r="S47" s="4"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <f>A47+3</f>
         <v>122</v>
@@ -3046,7 +3048,7 @@
       <c r="O48" s="5"/>
       <c r="S48" s="4"/>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="29">
         <f t="shared" ref="A49:A75" si="0">A48+3</f>
         <v>125</v>
@@ -3095,7 +3097,7 @@
       <c r="R49" s="30"/>
       <c r="S49" s="31"/>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <f t="shared" si="0"/>
         <v>128</v>
@@ -3129,7 +3131,7 @@
       <c r="O50" s="5"/>
       <c r="S50" s="4"/>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <f t="shared" si="0"/>
         <v>131</v>
@@ -3163,7 +3165,7 @@
       <c r="O51" s="5"/>
       <c r="S51" s="4"/>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="72">
         <f t="shared" si="0"/>
         <v>134</v>
@@ -3201,7 +3203,7 @@
       </c>
       <c r="S52" s="4"/>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <f t="shared" si="0"/>
         <v>137</v>
@@ -3235,7 +3237,7 @@
       <c r="O53" s="5"/>
       <c r="S53" s="4"/>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="29">
         <f t="shared" si="0"/>
         <v>140</v>
@@ -3284,7 +3286,7 @@
       <c r="R54" s="30"/>
       <c r="S54" s="31"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <f t="shared" si="0"/>
         <v>143</v>
@@ -3318,7 +3320,7 @@
       <c r="O55" s="5"/>
       <c r="S55" s="4"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="29">
         <f t="shared" si="0"/>
         <v>146</v>
@@ -3367,7 +3369,7 @@
       <c r="R56" s="30"/>
       <c r="S56" s="31"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <f t="shared" si="0"/>
         <v>149</v>
@@ -3401,7 +3403,7 @@
       <c r="O57" s="5"/>
       <c r="S57" s="4"/>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <f t="shared" si="0"/>
         <v>152</v>
@@ -3435,7 +3437,7 @@
       <c r="O58" s="35"/>
       <c r="S58" s="4"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <f t="shared" si="0"/>
         <v>155</v>
@@ -3469,7 +3471,7 @@
       <c r="O59" s="5"/>
       <c r="S59" s="4"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <f t="shared" si="0"/>
         <v>158</v>
@@ -3503,7 +3505,7 @@
       <c r="O60" s="5"/>
       <c r="S60" s="4"/>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="29">
         <f t="shared" si="0"/>
         <v>161</v>
@@ -3552,7 +3554,7 @@
       <c r="R61" s="30"/>
       <c r="S61" s="31"/>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="72">
         <f t="shared" si="0"/>
         <v>164</v>
@@ -3596,7 +3598,7 @@
       </c>
       <c r="S62" s="4"/>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="72">
         <f t="shared" si="0"/>
         <v>167</v>
@@ -3634,7 +3636,7 @@
       </c>
       <c r="S63" s="4"/>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="72">
         <f t="shared" si="0"/>
         <v>170</v>
@@ -3668,7 +3670,7 @@
       <c r="O64" s="5"/>
       <c r="S64" s="4"/>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="72">
         <f t="shared" si="0"/>
         <v>173</v>
@@ -3702,7 +3704,7 @@
       <c r="O65" s="5"/>
       <c r="S65" s="4"/>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="72">
         <f t="shared" si="0"/>
         <v>176</v>
@@ -3736,7 +3738,7 @@
       <c r="O66" s="5"/>
       <c r="S66" s="4"/>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="72">
         <f t="shared" si="0"/>
         <v>179</v>
@@ -3770,7 +3772,7 @@
       <c r="O67" s="5"/>
       <c r="S67" s="4"/>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="72">
         <f t="shared" si="0"/>
         <v>182</v>
@@ -3804,7 +3806,7 @@
       <c r="O68" s="5"/>
       <c r="S68" s="4"/>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="72">
         <f t="shared" si="0"/>
         <v>185</v>
@@ -3842,7 +3844,7 @@
       </c>
       <c r="S69" s="4"/>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="72">
         <f t="shared" si="0"/>
         <v>188</v>
@@ -3859,6 +3861,9 @@
       </c>
       <c r="E70" s="2">
         <v>4</v>
+      </c>
+      <c r="F70" s="3">
+        <v>45</v>
       </c>
       <c r="I70" s="4"/>
       <c r="K70" s="72">
@@ -3880,7 +3885,7 @@
       </c>
       <c r="S70" s="4"/>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <f t="shared" si="0"/>
         <v>191</v>
@@ -3914,7 +3919,7 @@
       <c r="O71" s="5"/>
       <c r="S71" s="4"/>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="29">
         <f t="shared" si="0"/>
         <v>194</v>
@@ -3959,7 +3964,7 @@
       <c r="R72" s="30"/>
       <c r="S72" s="31"/>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <f t="shared" si="0"/>
         <v>197</v>
@@ -3993,7 +3998,7 @@
       <c r="O73" s="5"/>
       <c r="S73" s="4"/>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <f t="shared" si="0"/>
         <v>200</v>
@@ -4027,7 +4032,7 @@
       <c r="O74" s="5"/>
       <c r="S74" s="4"/>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
         <f t="shared" si="0"/>
         <v>203</v>
@@ -4067,7 +4072,7 @@
       <c r="R75" s="7"/>
       <c r="S75" s="8"/>
     </row>
-    <row r="77" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A77" s="14" t="s">
         <v>0</v>
       </c>
@@ -4081,7 +4086,7 @@
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -4089,7 +4094,7 @@
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>1</v>
       </c>
@@ -4117,7 +4122,7 @@
       <c r="R79" s="97"/>
       <c r="S79" s="97"/>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>10</v>
       </c>
@@ -4173,7 +4178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>119</v>
       </c>
@@ -4203,7 +4208,7 @@
       <c r="O81" s="5"/>
       <c r="S81" s="4"/>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <f>A81+3</f>
         <v>122</v>
@@ -4241,7 +4246,7 @@
       </c>
       <c r="S82" s="4"/>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" s="29">
         <f t="shared" ref="A83:A109" si="5">A82+3</f>
         <v>125</v>
@@ -4286,7 +4291,7 @@
       <c r="R83" s="30"/>
       <c r="S83" s="31"/>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <f t="shared" si="5"/>
         <v>128</v>
@@ -4320,7 +4325,7 @@
       <c r="O84" s="5"/>
       <c r="S84" s="4"/>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <f t="shared" si="5"/>
         <v>131</v>
@@ -4354,7 +4359,7 @@
       <c r="O85" s="5"/>
       <c r="S85" s="4"/>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <f t="shared" si="5"/>
         <v>134</v>
@@ -4388,7 +4393,7 @@
       <c r="O86" s="5"/>
       <c r="S86" s="4"/>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <f t="shared" si="5"/>
         <v>137</v>
@@ -4426,7 +4431,7 @@
       </c>
       <c r="S87" s="4"/>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" s="29">
         <f t="shared" si="5"/>
         <v>140</v>
@@ -4475,7 +4480,7 @@
       <c r="R88" s="30"/>
       <c r="S88" s="31"/>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <f t="shared" si="5"/>
         <v>143</v>
@@ -4511,7 +4516,7 @@
       </c>
       <c r="S89" s="4"/>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" s="29">
         <f t="shared" si="5"/>
         <v>146</v>
@@ -4558,7 +4563,7 @@
       <c r="R90" s="30"/>
       <c r="S90" s="31"/>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" s="29">
         <f t="shared" si="5"/>
         <v>149</v>
@@ -4600,7 +4605,7 @@
       <c r="R91" s="30"/>
       <c r="S91" s="31"/>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <f t="shared" si="5"/>
         <v>152</v>
@@ -4634,7 +4639,7 @@
       <c r="O92" s="35"/>
       <c r="S92" s="4"/>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <f t="shared" si="5"/>
         <v>155</v>
@@ -4668,7 +4673,7 @@
       <c r="O93" s="5"/>
       <c r="S93" s="4"/>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <f t="shared" si="5"/>
         <v>158</v>
@@ -4706,7 +4711,7 @@
       </c>
       <c r="S94" s="4"/>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" s="29">
         <f t="shared" si="5"/>
         <v>161</v>
@@ -4753,7 +4758,7 @@
       <c r="R95" s="30"/>
       <c r="S95" s="31"/>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <f t="shared" si="5"/>
         <v>164</v>
@@ -4787,7 +4792,7 @@
       <c r="O96" s="5"/>
       <c r="S96" s="4"/>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <f t="shared" si="5"/>
         <v>167</v>
@@ -4825,7 +4830,7 @@
       </c>
       <c r="S97" s="4"/>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <f t="shared" si="5"/>
         <v>170</v>
@@ -4863,7 +4868,7 @@
       </c>
       <c r="S98" s="4"/>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <f t="shared" si="5"/>
         <v>173</v>
@@ -4901,7 +4906,7 @@
       </c>
       <c r="S99" s="4"/>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <f t="shared" si="5"/>
         <v>176</v>
@@ -4937,7 +4942,7 @@
       <c r="O100" s="5"/>
       <c r="S100" s="4"/>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
         <f t="shared" si="5"/>
         <v>179</v>
@@ -4973,7 +4978,7 @@
       <c r="O101" s="5"/>
       <c r="S101" s="4"/>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <f t="shared" si="5"/>
         <v>182</v>
@@ -5009,7 +5014,7 @@
       <c r="O102" s="5"/>
       <c r="S102" s="4"/>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <f t="shared" si="5"/>
         <v>185</v>
@@ -5047,7 +5052,7 @@
       </c>
       <c r="S103" s="4"/>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <f t="shared" si="5"/>
         <v>188</v>
@@ -5085,7 +5090,7 @@
       </c>
       <c r="S104" s="4"/>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <f t="shared" si="5"/>
         <v>191</v>
@@ -5123,7 +5128,7 @@
       </c>
       <c r="S105" s="4"/>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106" s="29">
         <f t="shared" si="5"/>
         <v>194</v>
@@ -5172,7 +5177,7 @@
       <c r="R106" s="30"/>
       <c r="S106" s="31"/>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
         <f t="shared" si="5"/>
         <v>197</v>
@@ -5210,7 +5215,7 @@
       </c>
       <c r="S107" s="4"/>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <f t="shared" si="5"/>
         <v>200</v>
@@ -5244,7 +5249,7 @@
       <c r="O108" s="5"/>
       <c r="S108" s="4"/>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109" s="6">
         <f t="shared" si="5"/>
         <v>203</v>
@@ -5284,7 +5289,7 @@
       <c r="R109" s="7"/>
       <c r="S109" s="8"/>
     </row>
-    <row r="111" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A111" s="14" t="s">
         <v>0</v>
       </c>
@@ -5296,7 +5301,7 @@
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -5304,7 +5309,7 @@
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113" s="9" t="s">
         <v>1</v>
       </c>
@@ -5331,7 +5336,7 @@
       <c r="R113" s="97"/>
       <c r="S113" s="97"/>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" s="9" t="s">
         <v>10</v>
       </c>
@@ -5387,7 +5392,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>110</v>
       </c>
@@ -5421,7 +5426,7 @@
       <c r="R115" s="30"/>
       <c r="S115" s="31"/>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>116</v>
       </c>
@@ -5451,7 +5456,7 @@
       <c r="O116" s="5"/>
       <c r="S116" s="4"/>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A117" s="32">
         <v>122</v>
       </c>
@@ -5497,7 +5502,7 @@
       <c r="R117" s="30"/>
       <c r="S117" s="31"/>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>128</v>
       </c>
@@ -5537,7 +5542,7 @@
       </c>
       <c r="S118" s="4"/>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>134</v>
       </c>
@@ -5577,7 +5582,7 @@
       </c>
       <c r="S119" s="4"/>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" s="32">
         <v>140</v>
       </c>
@@ -5622,7 +5627,7 @@
       <c r="R120" s="30"/>
       <c r="S120" s="31"/>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" s="32">
         <v>146</v>
       </c>
@@ -5666,7 +5671,7 @@
       <c r="R121" s="30"/>
       <c r="S121" s="31"/>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>152</v>
       </c>
@@ -5709,7 +5714,7 @@
       <c r="R122" s="30"/>
       <c r="S122" s="31"/>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A123" s="32">
         <v>158</v>
       </c>
@@ -5753,7 +5758,7 @@
       <c r="R123" s="30"/>
       <c r="S123" s="31"/>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>164</v>
       </c>
@@ -5793,7 +5798,7 @@
       </c>
       <c r="S124" s="4"/>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>170</v>
       </c>
@@ -5833,7 +5838,7 @@
       </c>
       <c r="S125" s="4"/>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>176</v>
       </c>
@@ -5879,7 +5884,7 @@
       </c>
       <c r="S126" s="4"/>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>182</v>
       </c>
@@ -5927,7 +5932,7 @@
       <c r="R127" s="57"/>
       <c r="S127" s="58"/>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>188</v>
       </c>
@@ -5973,7 +5978,7 @@
       </c>
       <c r="S128" s="4"/>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A129" s="32">
         <v>194</v>
       </c>
@@ -6021,7 +6026,7 @@
       <c r="R129" s="30"/>
       <c r="S129" s="31"/>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>200</v>
       </c>
@@ -6051,7 +6056,7 @@
       <c r="O130" s="5"/>
       <c r="S130" s="4"/>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131" s="7">
         <v>206</v>
       </c>

</xml_diff>

<commit_message>
MTP050 COP rows delivered; new event codes added
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36CA7BC-4D1D-4EF8-BFE3-B8C36056F22B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA1DA92-9734-4038-89FF-001D3D8A03CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -977,18 +977,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1014,6 +1002,18 @@
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -1337,26 +1337,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17:I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.88671875" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.28515625" customWidth="1"/>
-    <col min="22" max="22" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.33203125" customWidth="1"/>
+    <col min="22" max="22" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1364,12 +1364,12 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" ht="18" x14ac:dyDescent="0.35">
       <c r="V2" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B4" s="13" t="s">
         <v>12</v>
       </c>
@@ -1395,33 +1395,33 @@
       <c r="E4" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="89"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="88"/>
-      <c r="P4" s="88"/>
-      <c r="Q4" s="88"/>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="88"/>
-      <c r="V4" s="88"/>
-      <c r="W4" s="88"/>
-      <c r="X4" s="88"/>
-      <c r="Y4" s="88"/>
-      <c r="Z4" s="88"/>
-      <c r="AA4" s="88"/>
-      <c r="AB4" s="88"/>
-      <c r="AC4" s="88"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="84"/>
+      <c r="L4" s="84"/>
+      <c r="M4" s="84"/>
+      <c r="N4" s="84"/>
+      <c r="O4" s="84"/>
+      <c r="P4" s="84"/>
+      <c r="Q4" s="84"/>
+      <c r="R4" s="84"/>
+      <c r="S4" s="84"/>
+      <c r="T4" s="84"/>
+      <c r="U4" s="84"/>
+      <c r="V4" s="84"/>
+      <c r="W4" s="84"/>
+      <c r="X4" s="84"/>
+      <c r="Y4" s="84"/>
+      <c r="Z4" s="84"/>
+      <c r="AA4" s="84"/>
+      <c r="AB4" s="84"/>
+      <c r="AC4" s="84"/>
       <c r="AD4" s="76"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B5" s="19" t="s">
         <v>1</v>
       </c>
@@ -1452,27 +1452,27 @@
       <c r="K5" s="64">
         <v>49</v>
       </c>
-      <c r="L5" s="85"/>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="85"/>
-      <c r="S5" s="85"/>
-      <c r="T5" s="85"/>
-      <c r="U5" s="85"/>
-      <c r="V5" s="85"/>
-      <c r="W5" s="85"/>
-      <c r="X5" s="85"/>
-      <c r="Y5" s="85"/>
-      <c r="Z5" s="85"/>
-      <c r="AA5" s="85"/>
-      <c r="AB5" s="85"/>
-      <c r="AC5" s="85"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="81"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="81"/>
+      <c r="P5" s="81"/>
+      <c r="Q5" s="81"/>
+      <c r="R5" s="81"/>
+      <c r="S5" s="81"/>
+      <c r="T5" s="81"/>
+      <c r="U5" s="81"/>
+      <c r="V5" s="81"/>
+      <c r="W5" s="81"/>
+      <c r="X5" s="81"/>
+      <c r="Y5" s="81"/>
+      <c r="Z5" s="81"/>
+      <c r="AA5" s="81"/>
+      <c r="AB5" s="81"/>
+      <c r="AC5" s="81"/>
       <c r="AD5" s="4"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B6" s="20" t="s">
         <v>2</v>
       </c>
@@ -1482,7 +1482,7 @@
       <c r="D6" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="86">
+      <c r="E6" s="82">
         <v>3</v>
       </c>
       <c r="F6" s="18">
@@ -1529,7 +1529,7 @@
       <c r="AC6" s="7"/>
       <c r="AD6" s="8"/>
     </row>
-    <row r="8" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C8"/>
       <c r="D8"/>
       <c r="E8"/>
@@ -1538,7 +1538,7 @@
       <c r="H8"/>
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:30" s="60" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>24</v>
       </c>
@@ -1546,7 +1546,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="13" t="s">
         <v>12</v>
       </c>
@@ -1556,36 +1556,36 @@
       <c r="D10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="81" t="s">
+      <c r="E10" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
-      <c r="I10" s="82"/>
-      <c r="J10" s="88"/>
-      <c r="K10" s="88"/>
-      <c r="L10" s="88"/>
-      <c r="M10" s="88"/>
-      <c r="N10" s="88"/>
-      <c r="O10" s="88"/>
-      <c r="P10" s="88"/>
-      <c r="Q10" s="88"/>
-      <c r="R10" s="88"/>
-      <c r="S10" s="88"/>
-      <c r="T10" s="88"/>
-      <c r="U10" s="88"/>
-      <c r="V10" s="88"/>
-      <c r="W10" s="88"/>
-      <c r="X10" s="88"/>
-      <c r="Y10" s="88"/>
-      <c r="Z10" s="88"/>
-      <c r="AA10" s="88"/>
-      <c r="AB10" s="88"/>
-      <c r="AC10" s="88"/>
+      <c r="F10" s="103"/>
+      <c r="G10" s="103"/>
+      <c r="H10" s="103"/>
+      <c r="I10" s="103"/>
+      <c r="J10" s="84"/>
+      <c r="K10" s="84"/>
+      <c r="L10" s="84"/>
+      <c r="M10" s="84"/>
+      <c r="N10" s="84"/>
+      <c r="O10" s="84"/>
+      <c r="P10" s="84"/>
+      <c r="Q10" s="84"/>
+      <c r="R10" s="84"/>
+      <c r="S10" s="84"/>
+      <c r="T10" s="84"/>
+      <c r="U10" s="84"/>
+      <c r="V10" s="84"/>
+      <c r="W10" s="84"/>
+      <c r="X10" s="84"/>
+      <c r="Y10" s="84"/>
+      <c r="Z10" s="84"/>
+      <c r="AA10" s="84"/>
+      <c r="AB10" s="84"/>
+      <c r="AC10" s="84"/>
       <c r="AD10" s="76"/>
     </row>
-    <row r="11" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>34</v>
       </c>
@@ -1595,7 +1595,7 @@
       <c r="D11" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="87">
+      <c r="E11" s="83">
         <v>5</v>
       </c>
       <c r="F11" s="15">
@@ -1616,7 +1616,9 @@
       <c r="K11" s="15">
         <v>48</v>
       </c>
-      <c r="L11" s="16"/>
+      <c r="L11" s="15">
+        <v>50</v>
+      </c>
       <c r="M11" s="16"/>
       <c r="N11" s="16"/>
       <c r="O11" s="16"/>
@@ -1636,7 +1638,7 @@
       <c r="AC11" s="16"/>
       <c r="AD11" s="17"/>
     </row>
-    <row r="12" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="20" t="s">
         <v>36</v>
       </c>
@@ -1646,7 +1648,7 @@
       <c r="D12" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="86">
+      <c r="E12" s="82">
         <v>15</v>
       </c>
       <c r="F12" s="18">
@@ -1679,7 +1681,7 @@
       <c r="AC12" s="7"/>
       <c r="AD12" s="8"/>
     </row>
-    <row r="13" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>28</v>
       </c>
@@ -1691,14 +1693,14 @@
       <c r="H13"/>
       <c r="I13"/>
     </row>
-    <row r="14" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E14" s="59"/>
       <c r="F14" s="59"/>
       <c r="G14" s="59"/>
       <c r="H14" s="59"/>
       <c r="I14" s="59"/>
     </row>
-    <row r="15" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="s">
         <v>0</v>
       </c>
@@ -1708,44 +1710,44 @@
       <c r="C15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="104" t="s">
+      <c r="E15" s="100" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="AB16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="9"/>
       <c r="D17" s="58"/>
-      <c r="E17" s="83" t="s">
+      <c r="E17" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="84"/>
-      <c r="G17" s="84"/>
-      <c r="H17" s="84"/>
-      <c r="I17" s="84"/>
+      <c r="F17" s="105"/>
+      <c r="G17" s="105"/>
+      <c r="H17" s="105"/>
+      <c r="I17" s="105"/>
       <c r="K17" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L17" s="13"/>
       <c r="M17" s="9"/>
       <c r="N17" s="58"/>
-      <c r="O17" s="83" t="s">
+      <c r="O17" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="P17" s="84"/>
-      <c r="Q17" s="84"/>
-      <c r="R17" s="84"/>
-      <c r="S17" s="84"/>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="P17" s="105"/>
+      <c r="Q17" s="105"/>
+      <c r="R17" s="105"/>
+      <c r="S17" s="105"/>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18" s="39" t="s">
         <v>10</v>
       </c>
@@ -1820,7 +1822,7 @@
       </c>
       <c r="AD18" s="9"/>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19" s="26">
         <v>105</v>
       </c>
@@ -1863,14 +1865,14 @@
       </c>
       <c r="X19" s="5"/>
       <c r="Y19" s="4"/>
-      <c r="AB19" s="90">
+      <c r="AB19" s="86">
         <v>2927.1</v>
       </c>
-      <c r="AC19" s="90">
+      <c r="AC19" s="86">
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20" s="25">
         <v>107</v>
       </c>
@@ -1907,14 +1909,14 @@
       </c>
       <c r="X20" s="5"/>
       <c r="Y20" s="4"/>
-      <c r="AB20" s="90">
+      <c r="AB20" s="86">
         <v>3172.9</v>
       </c>
-      <c r="AC20" s="90">
+      <c r="AC20" s="86">
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" s="25">
         <v>120</v>
       </c>
@@ -1951,40 +1953,40 @@
       </c>
       <c r="X21" s="5"/>
       <c r="Y21" s="4"/>
-      <c r="AB21" s="90">
+      <c r="AB21" s="86">
         <v>3289.6</v>
       </c>
-      <c r="AC21" s="90">
+      <c r="AC21" s="86">
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A22" s="94">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A22" s="90">
         <v>126</v>
       </c>
-      <c r="B22" s="95" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="96">
+      <c r="B22" s="91" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="92">
         <v>298</v>
       </c>
-      <c r="D22" s="97">
+      <c r="D22" s="93">
         <v>57</v>
       </c>
       <c r="E22" s="2">
         <v>11</v>
       </c>
       <c r="I22" s="4"/>
-      <c r="K22" s="94">
+      <c r="K22" s="90">
         <v>126</v>
       </c>
-      <c r="L22" s="95" t="s">
-        <v>25</v>
-      </c>
-      <c r="M22" s="96">
+      <c r="L22" s="91" t="s">
+        <v>25</v>
+      </c>
+      <c r="M22" s="92">
         <v>331</v>
       </c>
-      <c r="N22" s="97">
+      <c r="N22" s="93">
         <v>104</v>
       </c>
       <c r="O22" s="2">
@@ -2003,14 +2005,14 @@
       <c r="Y22" s="49">
         <v>126</v>
       </c>
-      <c r="AB22" s="90">
+      <c r="AB22" s="86">
         <v>3750.1</v>
       </c>
-      <c r="AC22" s="91">
+      <c r="AC22" s="87">
         <v>166</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" s="25">
         <v>130</v>
       </c>
@@ -2047,14 +2049,14 @@
       </c>
       <c r="X23" s="48"/>
       <c r="Y23" s="49"/>
-      <c r="AB23" s="90">
+      <c r="AB23" s="86">
         <v>3787.9</v>
       </c>
-      <c r="AC23" s="91">
+      <c r="AC23" s="87">
         <v>168</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24" s="25">
         <v>134</v>
       </c>
@@ -2091,40 +2093,40 @@
       </c>
       <c r="X24" s="48"/>
       <c r="Y24" s="49"/>
-      <c r="AB24" s="90">
+      <c r="AB24" s="86">
         <v>4276.1000000000004</v>
       </c>
-      <c r="AC24" s="91">
+      <c r="AC24" s="87">
         <v>189</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A25" s="94">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A25" s="90">
         <v>141</v>
       </c>
-      <c r="B25" s="95" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="96">
+      <c r="B25" s="91" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="92">
         <v>301</v>
       </c>
-      <c r="D25" s="97">
+      <c r="D25" s="93">
         <v>60</v>
       </c>
       <c r="E25" s="2">
         <v>11</v>
       </c>
       <c r="I25" s="4"/>
-      <c r="K25" s="94">
+      <c r="K25" s="90">
         <v>141</v>
       </c>
-      <c r="L25" s="95" t="s">
-        <v>25</v>
-      </c>
-      <c r="M25" s="96">
+      <c r="L25" s="91" t="s">
+        <v>25</v>
+      </c>
+      <c r="M25" s="92">
         <v>334</v>
       </c>
-      <c r="N25" s="97">
+      <c r="N25" s="93">
         <v>107</v>
       </c>
       <c r="O25" s="2">
@@ -2143,14 +2145,14 @@
       <c r="Y25" s="49">
         <v>141</v>
       </c>
-      <c r="AB25" s="90">
+      <c r="AB25" s="86">
         <v>4383.5</v>
       </c>
-      <c r="AC25" s="91">
+      <c r="AC25" s="87">
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A26" s="25">
         <v>142</v>
       </c>
@@ -2187,40 +2189,40 @@
       </c>
       <c r="X26" s="48"/>
       <c r="Y26" s="49"/>
-      <c r="AB26" s="90">
+      <c r="AB26" s="86">
         <v>4448.5</v>
       </c>
-      <c r="AC26" s="91">
+      <c r="AC26" s="87">
         <v>197</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A27" s="94">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A27" s="90">
         <v>146</v>
       </c>
-      <c r="B27" s="95" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="96">
+      <c r="B27" s="91" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="92">
         <v>303</v>
       </c>
-      <c r="D27" s="97">
+      <c r="D27" s="93">
         <v>62</v>
       </c>
       <c r="E27" s="2">
         <v>11</v>
       </c>
       <c r="I27" s="4"/>
-      <c r="K27" s="94">
+      <c r="K27" s="90">
         <v>146</v>
       </c>
-      <c r="L27" s="95" t="s">
-        <v>25</v>
-      </c>
-      <c r="M27" s="96">
+      <c r="L27" s="91" t="s">
+        <v>25</v>
+      </c>
+      <c r="M27" s="92">
         <v>336</v>
       </c>
-      <c r="N27" s="97">
+      <c r="N27" s="93">
         <v>109</v>
       </c>
       <c r="O27" s="2">
@@ -2240,7 +2242,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28" s="25">
         <v>151</v>
       </c>
@@ -2272,7 +2274,7 @@
       <c r="V28" s="75">
         <v>3414.35</v>
       </c>
-      <c r="W28" s="105">
+      <c r="W28" s="101">
         <v>151</v>
       </c>
       <c r="X28" t="s">
@@ -2280,7 +2282,7 @@
       </c>
       <c r="Y28" s="61"/>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A29" s="25">
         <v>156</v>
       </c>
@@ -2318,7 +2320,7 @@
       <c r="X29" s="48"/>
       <c r="Y29" s="49"/>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A30" s="50">
         <v>162</v>
       </c>
@@ -2364,7 +2366,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A31" s="25">
         <v>164</v>
       </c>
@@ -2377,7 +2379,9 @@
       <c r="D31" s="60">
         <v>66</v>
       </c>
-      <c r="E31" s="5"/>
+      <c r="E31" s="2">
+        <v>50</v>
+      </c>
       <c r="I31" s="4"/>
       <c r="K31" s="25">
         <v>164</v>
@@ -2402,31 +2406,33 @@
       <c r="X31" s="48"/>
       <c r="Y31" s="49"/>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A32" s="92">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A32" s="88">
         <v>166</v>
       </c>
-      <c r="B32" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="93">
+      <c r="B32" s="88" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="89">
         <v>308</v>
       </c>
-      <c r="D32" s="90">
+      <c r="D32" s="86">
         <v>67</v>
       </c>
-      <c r="E32" s="5"/>
+      <c r="E32" s="2">
+        <v>50</v>
+      </c>
       <c r="I32" s="4"/>
-      <c r="K32" s="92">
+      <c r="K32" s="88">
         <v>166</v>
       </c>
-      <c r="L32" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="M32" s="93">
+      <c r="L32" s="88" t="s">
+        <v>25</v>
+      </c>
+      <c r="M32" s="89">
         <v>341</v>
       </c>
-      <c r="N32" s="90">
+      <c r="N32" s="86">
         <v>114</v>
       </c>
       <c r="O32" s="5"/>
@@ -2440,7 +2446,7 @@
       <c r="X32" s="48"/>
       <c r="Y32" s="49"/>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="25">
         <v>167</v>
       </c>
@@ -2453,7 +2459,9 @@
       <c r="D33" s="60">
         <v>68</v>
       </c>
-      <c r="E33" s="5"/>
+      <c r="E33" s="2">
+        <v>50</v>
+      </c>
       <c r="I33" s="4"/>
       <c r="K33" s="25">
         <v>167</v>
@@ -2478,31 +2486,33 @@
       <c r="X33" s="48"/>
       <c r="Y33" s="49"/>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A34" s="92">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A34" s="88">
         <v>168</v>
       </c>
-      <c r="B34" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="C34" s="93">
+      <c r="B34" s="88" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="89">
         <v>310</v>
       </c>
-      <c r="D34" s="90">
+      <c r="D34" s="86">
         <v>69</v>
       </c>
-      <c r="E34" s="5"/>
+      <c r="E34" s="2">
+        <v>50</v>
+      </c>
       <c r="I34" s="4"/>
-      <c r="K34" s="92">
+      <c r="K34" s="88">
         <v>168</v>
       </c>
-      <c r="L34" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="M34" s="93">
+      <c r="L34" s="88" t="s">
+        <v>25</v>
+      </c>
+      <c r="M34" s="89">
         <v>343</v>
       </c>
-      <c r="N34" s="90">
+      <c r="N34" s="86">
         <v>116</v>
       </c>
       <c r="O34" s="5"/>
@@ -2516,7 +2526,7 @@
       <c r="X34" s="48"/>
       <c r="Y34" s="49"/>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="25">
         <v>169</v>
       </c>
@@ -2554,7 +2564,7 @@
       <c r="X35" s="48"/>
       <c r="Y35" s="49"/>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="25">
         <v>171</v>
       </c>
@@ -2592,7 +2602,7 @@
       <c r="X36" s="48"/>
       <c r="Y36" s="49"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" s="25">
         <v>172</v>
       </c>
@@ -2630,7 +2640,7 @@
       <c r="X37" s="48"/>
       <c r="Y37" s="49"/>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A38" s="25">
         <v>178</v>
       </c>
@@ -2668,7 +2678,7 @@
       <c r="X38" s="48"/>
       <c r="Y38" s="49"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39" s="25">
         <v>180</v>
       </c>
@@ -2706,7 +2716,7 @@
       <c r="X39" s="48"/>
       <c r="Y39" s="49"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A40" s="25">
         <v>182</v>
       </c>
@@ -2744,17 +2754,17 @@
       <c r="X40" s="48"/>
       <c r="Y40" s="49"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A41" s="92">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A41" s="88">
         <v>188</v>
       </c>
-      <c r="B41" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41" s="93">
+      <c r="B41" s="88" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="89">
         <v>317</v>
       </c>
-      <c r="D41" s="90">
+      <c r="D41" s="86">
         <v>76</v>
       </c>
       <c r="E41" s="2">
@@ -2764,16 +2774,16 @@
         <v>49</v>
       </c>
       <c r="I41" s="4"/>
-      <c r="K41" s="92">
+      <c r="K41" s="88">
         <v>188</v>
       </c>
-      <c r="L41" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="M41" s="93">
+      <c r="L41" s="88" t="s">
+        <v>25</v>
+      </c>
+      <c r="M41" s="89">
         <v>350</v>
       </c>
-      <c r="N41" s="90">
+      <c r="N41" s="86">
         <v>123</v>
       </c>
       <c r="O41" s="5"/>
@@ -2787,7 +2797,7 @@
       <c r="X41" s="48"/>
       <c r="Y41" s="49"/>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42" s="25">
         <v>191</v>
       </c>
@@ -2832,17 +2842,17 @@
       <c r="X42" s="48"/>
       <c r="Y42" s="49"/>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A43" s="94">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A43" s="90">
         <v>194</v>
       </c>
-      <c r="B43" s="95" t="s">
-        <v>25</v>
-      </c>
-      <c r="C43" s="96">
+      <c r="B43" s="91" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="92">
         <v>319</v>
       </c>
-      <c r="D43" s="97">
+      <c r="D43" s="93">
         <v>78</v>
       </c>
       <c r="E43" s="2">
@@ -2855,16 +2865,16 @@
         <v>49</v>
       </c>
       <c r="I43" s="4"/>
-      <c r="K43" s="94">
+      <c r="K43" s="90">
         <v>194</v>
       </c>
-      <c r="L43" s="95" t="s">
-        <v>25</v>
-      </c>
-      <c r="M43" s="96">
+      <c r="L43" s="91" t="s">
+        <v>25</v>
+      </c>
+      <c r="M43" s="92">
         <v>352</v>
       </c>
-      <c r="N43" s="97">
+      <c r="N43" s="93">
         <v>125</v>
       </c>
       <c r="O43" s="2">
@@ -2883,7 +2893,7 @@
       <c r="X43" s="48"/>
       <c r="Y43" s="49"/>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A44" s="25">
         <v>196</v>
       </c>
@@ -2925,31 +2935,31 @@
         <v>194</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A45" s="92">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A45" s="88">
         <v>197</v>
       </c>
-      <c r="B45" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="C45" s="93">
+      <c r="B45" s="88" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="89">
         <v>321</v>
       </c>
-      <c r="D45" s="90">
+      <c r="D45" s="86">
         <v>80</v>
       </c>
       <c r="E45" s="5"/>
       <c r="I45" s="4"/>
-      <c r="K45" s="92">
+      <c r="K45" s="88">
         <v>197</v>
       </c>
-      <c r="L45" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="M45" s="93">
+      <c r="L45" s="88" t="s">
+        <v>25</v>
+      </c>
+      <c r="M45" s="89">
         <v>354</v>
       </c>
-      <c r="N45" s="90">
+      <c r="N45" s="86">
         <v>127</v>
       </c>
       <c r="O45" s="5"/>
@@ -2963,7 +2973,7 @@
       <c r="X45" s="5"/>
       <c r="Y45" s="4"/>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46" s="25">
         <v>199</v>
       </c>
@@ -3001,7 +3011,7 @@
       <c r="X46" s="5"/>
       <c r="Y46" s="4"/>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A47" s="25">
         <v>201</v>
       </c>
@@ -3037,7 +3047,7 @@
       <c r="X47" s="5"/>
       <c r="Y47" s="4"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A48" s="34">
         <v>210</v>
       </c>
@@ -3081,7 +3091,7 @@
       <c r="X48" s="5"/>
       <c r="Y48" s="4"/>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
       <c r="V49" s="5">
         <v>4526.9799999999996</v>
       </c>
@@ -3091,7 +3101,7 @@
       <c r="X49" s="6"/>
       <c r="Y49" s="8"/>
     </row>
-    <row r="50" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:25" ht="18" x14ac:dyDescent="0.35">
       <c r="A50" s="14" t="s">
         <v>0</v>
       </c>
@@ -3103,7 +3113,7 @@
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -3114,35 +3124,35 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B52" s="13"/>
       <c r="C52" s="9"/>
       <c r="D52" s="58"/>
-      <c r="E52" s="83" t="s">
+      <c r="E52" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="F52" s="84"/>
-      <c r="G52" s="84"/>
-      <c r="H52" s="84"/>
-      <c r="I52" s="84"/>
+      <c r="F52" s="105"/>
+      <c r="G52" s="105"/>
+      <c r="H52" s="105"/>
+      <c r="I52" s="105"/>
       <c r="K52" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L52" s="13"/>
       <c r="M52" s="9"/>
       <c r="N52" s="58"/>
-      <c r="O52" s="83" t="s">
+      <c r="O52" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="P52" s="84"/>
-      <c r="Q52" s="84"/>
-      <c r="R52" s="84"/>
-      <c r="S52" s="84"/>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="P52" s="105"/>
+      <c r="Q52" s="105"/>
+      <c r="R52" s="105"/>
+      <c r="S52" s="105"/>
+    </row>
+    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="s">
         <v>10</v>
       </c>
@@ -3198,7 +3208,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A54" s="65">
         <v>119</v>
       </c>
@@ -3232,7 +3242,7 @@
       </c>
       <c r="S54" s="4"/>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <f>A54+3</f>
         <v>122</v>
@@ -3266,7 +3276,7 @@
       <c r="O55" s="5"/>
       <c r="S55" s="4"/>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A56" s="29">
         <f t="shared" ref="A56:A82" si="0">A55+3</f>
         <v>125</v>
@@ -3315,41 +3325,41 @@
       <c r="R56" s="30"/>
       <c r="S56" s="31"/>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A57" s="35">
         <f t="shared" si="0"/>
         <v>128</v>
       </c>
-      <c r="B57" s="92">
+      <c r="B57" s="88">
         <f t="shared" si="1"/>
         <v>316</v>
       </c>
-      <c r="C57" s="93">
+      <c r="C57" s="89">
         <v>335</v>
       </c>
-      <c r="D57" s="90">
+      <c r="D57" s="86">
         <v>90</v>
       </c>
       <c r="E57" s="5"/>
       <c r="I57" s="4"/>
-      <c r="K57" s="99">
+      <c r="K57" s="95">
         <f t="shared" si="2"/>
         <v>128</v>
       </c>
-      <c r="L57" s="100">
+      <c r="L57" s="96">
         <f t="shared" si="3"/>
         <v>349</v>
       </c>
-      <c r="M57" s="93">
+      <c r="M57" s="89">
         <v>368</v>
       </c>
-      <c r="N57" s="90">
+      <c r="N57" s="86">
         <v>137</v>
       </c>
       <c r="O57" s="5"/>
       <c r="S57" s="4"/>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <f t="shared" si="0"/>
         <v>131</v>
@@ -3383,7 +3393,7 @@
       <c r="O58" s="5"/>
       <c r="S58" s="4"/>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A59" s="65">
         <f t="shared" si="0"/>
         <v>134</v>
@@ -3421,7 +3431,7 @@
       </c>
       <c r="S59" s="4"/>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <f t="shared" si="0"/>
         <v>137</v>
@@ -3455,19 +3465,19 @@
       <c r="O60" s="5"/>
       <c r="S60" s="4"/>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A61" s="98">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A61" s="94">
         <f t="shared" si="0"/>
         <v>140</v>
       </c>
-      <c r="B61" s="95">
+      <c r="B61" s="91">
         <f t="shared" si="1"/>
         <v>324</v>
       </c>
-      <c r="C61" s="96">
+      <c r="C61" s="92">
         <v>339</v>
       </c>
-      <c r="D61" s="97">
+      <c r="D61" s="93">
         <v>94</v>
       </c>
       <c r="E61" s="29">
@@ -3480,18 +3490,18 @@
       <c r="H61" s="30"/>
       <c r="I61" s="31"/>
       <c r="J61" s="30"/>
-      <c r="K61" s="98">
+      <c r="K61" s="94">
         <f t="shared" si="2"/>
         <v>140</v>
       </c>
-      <c r="L61" s="95">
+      <c r="L61" s="91">
         <f t="shared" si="3"/>
         <v>357</v>
       </c>
-      <c r="M61" s="96">
+      <c r="M61" s="92">
         <v>372</v>
       </c>
-      <c r="N61" s="97">
+      <c r="N61" s="93">
         <v>141</v>
       </c>
       <c r="O61" s="29">
@@ -3504,7 +3514,7 @@
       <c r="R61" s="30"/>
       <c r="S61" s="31"/>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A62" s="5">
         <f t="shared" si="0"/>
         <v>143</v>
@@ -3538,19 +3548,19 @@
       <c r="O62" s="5"/>
       <c r="S62" s="4"/>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A63" s="98">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A63" s="94">
         <f t="shared" si="0"/>
         <v>146</v>
       </c>
-      <c r="B63" s="95">
+      <c r="B63" s="91">
         <f t="shared" si="1"/>
         <v>328</v>
       </c>
-      <c r="C63" s="96">
+      <c r="C63" s="92">
         <v>341</v>
       </c>
-      <c r="D63" s="97">
+      <c r="D63" s="93">
         <v>96</v>
       </c>
       <c r="E63" s="29">
@@ -3563,18 +3573,18 @@
       <c r="H63" s="30"/>
       <c r="I63" s="31"/>
       <c r="J63" s="30"/>
-      <c r="K63" s="98">
+      <c r="K63" s="94">
         <f t="shared" si="2"/>
         <v>146</v>
       </c>
-      <c r="L63" s="95">
+      <c r="L63" s="91">
         <f t="shared" si="3"/>
         <v>361</v>
       </c>
-      <c r="M63" s="96">
+      <c r="M63" s="92">
         <v>374</v>
       </c>
-      <c r="N63" s="97">
+      <c r="N63" s="93">
         <v>143</v>
       </c>
       <c r="O63" s="29">
@@ -3587,7 +3597,7 @@
       <c r="R63" s="30"/>
       <c r="S63" s="31"/>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A64" s="5">
         <f t="shared" si="0"/>
         <v>149</v>
@@ -3621,7 +3631,7 @@
       <c r="O64" s="5"/>
       <c r="S64" s="4"/>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A65" s="5">
         <f t="shared" si="0"/>
         <v>152</v>
@@ -3655,7 +3665,7 @@
       <c r="O65" s="35"/>
       <c r="S65" s="4"/>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A66" s="5">
         <f t="shared" si="0"/>
         <v>155</v>
@@ -3689,7 +3699,7 @@
       <c r="O66" s="5"/>
       <c r="S66" s="4"/>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A67" s="5">
         <f t="shared" si="0"/>
         <v>158</v>
@@ -3723,7 +3733,7 @@
       <c r="O67" s="5"/>
       <c r="S67" s="4"/>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A68" s="29">
         <f t="shared" si="0"/>
         <v>161</v>
@@ -3772,19 +3782,19 @@
       <c r="R68" s="30"/>
       <c r="S68" s="31"/>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A69" s="99">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A69" s="95">
         <f t="shared" si="0"/>
         <v>164</v>
       </c>
-      <c r="B69" s="100">
+      <c r="B69" s="96">
         <f t="shared" si="1"/>
         <v>340</v>
       </c>
-      <c r="C69" s="93">
+      <c r="C69" s="89">
         <v>347</v>
       </c>
-      <c r="D69" s="90">
+      <c r="D69" s="86">
         <v>102</v>
       </c>
       <c r="E69" s="2">
@@ -3794,18 +3804,18 @@
         <v>7</v>
       </c>
       <c r="I69" s="4"/>
-      <c r="K69" s="99">
+      <c r="K69" s="95">
         <f t="shared" si="2"/>
         <v>164</v>
       </c>
-      <c r="L69" s="100">
+      <c r="L69" s="96">
         <f t="shared" si="3"/>
         <v>373</v>
       </c>
-      <c r="M69" s="93">
+      <c r="M69" s="89">
         <v>380</v>
       </c>
-      <c r="N69" s="90">
+      <c r="N69" s="86">
         <v>149</v>
       </c>
       <c r="O69" s="2">
@@ -3816,37 +3826,37 @@
       </c>
       <c r="S69" s="4"/>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A70" s="99">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A70" s="95">
         <f t="shared" si="0"/>
         <v>167</v>
       </c>
-      <c r="B70" s="100">
+      <c r="B70" s="96">
         <f t="shared" si="1"/>
         <v>342</v>
       </c>
-      <c r="C70" s="93">
+      <c r="C70" s="89">
         <v>348</v>
       </c>
-      <c r="D70" s="90">
+      <c r="D70" s="86">
         <v>103</v>
       </c>
       <c r="E70" s="2">
         <v>4</v>
       </c>
       <c r="I70" s="4"/>
-      <c r="K70" s="99">
+      <c r="K70" s="95">
         <f t="shared" si="2"/>
         <v>167</v>
       </c>
-      <c r="L70" s="100">
+      <c r="L70" s="96">
         <f t="shared" si="3"/>
         <v>375</v>
       </c>
-      <c r="M70" s="93">
+      <c r="M70" s="89">
         <v>381</v>
       </c>
-      <c r="N70" s="90">
+      <c r="N70" s="86">
         <v>150</v>
       </c>
       <c r="O70" s="2">
@@ -3854,7 +3864,7 @@
       </c>
       <c r="S70" s="4"/>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A71" s="65">
         <f t="shared" si="0"/>
         <v>170</v>
@@ -3888,7 +3898,7 @@
       <c r="O71" s="5"/>
       <c r="S71" s="4"/>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A72" s="65">
         <f t="shared" si="0"/>
         <v>173</v>
@@ -3922,7 +3932,7 @@
       <c r="O72" s="5"/>
       <c r="S72" s="4"/>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A73" s="65">
         <f t="shared" si="0"/>
         <v>176</v>
@@ -3956,7 +3966,7 @@
       <c r="O73" s="5"/>
       <c r="S73" s="4"/>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A74" s="65">
         <f t="shared" si="0"/>
         <v>179</v>
@@ -3990,7 +4000,7 @@
       <c r="O74" s="5"/>
       <c r="S74" s="4"/>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A75" s="65">
         <f t="shared" si="0"/>
         <v>182</v>
@@ -4024,7 +4034,7 @@
       <c r="O75" s="5"/>
       <c r="S75" s="4"/>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A76" s="65">
         <f t="shared" si="0"/>
         <v>185</v>
@@ -4062,19 +4072,19 @@
       </c>
       <c r="S76" s="4"/>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A77" s="99">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A77" s="95">
         <f t="shared" si="0"/>
         <v>188</v>
       </c>
-      <c r="B77" s="100">
+      <c r="B77" s="96">
         <f t="shared" si="1"/>
         <v>356</v>
       </c>
-      <c r="C77" s="93">
+      <c r="C77" s="89">
         <v>355</v>
       </c>
-      <c r="D77" s="90">
+      <c r="D77" s="86">
         <v>110</v>
       </c>
       <c r="E77" s="2">
@@ -4084,18 +4094,18 @@
         <v>45</v>
       </c>
       <c r="I77" s="4"/>
-      <c r="K77" s="99">
+      <c r="K77" s="95">
         <f t="shared" si="2"/>
         <v>188</v>
       </c>
-      <c r="L77" s="100">
+      <c r="L77" s="96">
         <f t="shared" si="3"/>
         <v>389</v>
       </c>
-      <c r="M77" s="93">
+      <c r="M77" s="89">
         <v>388</v>
       </c>
-      <c r="N77" s="90">
+      <c r="N77" s="86">
         <v>157</v>
       </c>
       <c r="O77" s="2">
@@ -4103,7 +4113,7 @@
       </c>
       <c r="S77" s="4"/>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A78" s="5">
         <f t="shared" si="0"/>
         <v>191</v>
@@ -4137,19 +4147,19 @@
       <c r="O78" s="5"/>
       <c r="S78" s="4"/>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A79" s="98">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A79" s="94">
         <f t="shared" si="0"/>
         <v>194</v>
       </c>
-      <c r="B79" s="95">
+      <c r="B79" s="91">
         <f t="shared" si="1"/>
         <v>360</v>
       </c>
-      <c r="C79" s="96">
+      <c r="C79" s="92">
         <v>357</v>
       </c>
-      <c r="D79" s="97">
+      <c r="D79" s="93">
         <v>112</v>
       </c>
       <c r="E79" s="29">
@@ -4160,18 +4170,18 @@
       <c r="H79" s="30"/>
       <c r="I79" s="31"/>
       <c r="J79" s="30"/>
-      <c r="K79" s="98">
+      <c r="K79" s="94">
         <f t="shared" si="2"/>
         <v>194</v>
       </c>
-      <c r="L79" s="95">
+      <c r="L79" s="91">
         <f t="shared" si="3"/>
         <v>393</v>
       </c>
-      <c r="M79" s="96">
+      <c r="M79" s="92">
         <v>390</v>
       </c>
-      <c r="N79" s="97">
+      <c r="N79" s="93">
         <v>159</v>
       </c>
       <c r="O79" s="29">
@@ -4182,19 +4192,19 @@
       <c r="R79" s="30"/>
       <c r="S79" s="31"/>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A80" s="35">
         <f t="shared" si="0"/>
         <v>197</v>
       </c>
-      <c r="B80" s="92">
+      <c r="B80" s="88">
         <f t="shared" si="1"/>
         <v>362</v>
       </c>
-      <c r="C80" s="93">
+      <c r="C80" s="89">
         <v>358</v>
       </c>
-      <c r="D80" s="90">
+      <c r="D80" s="86">
         <v>113</v>
       </c>
       <c r="E80" s="5"/>
@@ -4203,20 +4213,20 @@
         <f t="shared" si="2"/>
         <v>197</v>
       </c>
-      <c r="L80" s="92">
+      <c r="L80" s="88">
         <f t="shared" si="3"/>
         <v>395</v>
       </c>
-      <c r="M80" s="93">
+      <c r="M80" s="89">
         <v>391</v>
       </c>
-      <c r="N80" s="90">
+      <c r="N80" s="86">
         <v>160</v>
       </c>
       <c r="O80" s="5"/>
       <c r="S80" s="4"/>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A81" s="5">
         <f t="shared" si="0"/>
         <v>200</v>
@@ -4250,7 +4260,7 @@
       <c r="O81" s="5"/>
       <c r="S81" s="4"/>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A82" s="6">
         <f t="shared" si="0"/>
         <v>203</v>
@@ -4290,7 +4300,7 @@
       <c r="R82" s="7"/>
       <c r="S82" s="8"/>
     </row>
-    <row r="84" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A84" s="14" t="s">
         <v>0</v>
       </c>
@@ -4304,7 +4314,7 @@
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -4312,35 +4322,35 @@
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B86" s="13"/>
       <c r="C86" s="9"/>
       <c r="D86" s="33"/>
-      <c r="E86" s="83" t="s">
+      <c r="E86" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="F86" s="84"/>
-      <c r="G86" s="84"/>
-      <c r="H86" s="84"/>
-      <c r="I86" s="84"/>
+      <c r="F86" s="105"/>
+      <c r="G86" s="105"/>
+      <c r="H86" s="105"/>
+      <c r="I86" s="105"/>
       <c r="K86" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L86" s="13"/>
       <c r="M86" s="9"/>
       <c r="N86" s="33"/>
-      <c r="O86" s="83" t="s">
+      <c r="O86" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="P86" s="84"/>
-      <c r="Q86" s="84"/>
-      <c r="R86" s="84"/>
-      <c r="S86" s="84"/>
-    </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P86" s="105"/>
+      <c r="Q86" s="105"/>
+      <c r="R86" s="105"/>
+      <c r="S86" s="105"/>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A87" s="9" t="s">
         <v>10</v>
       </c>
@@ -4396,7 +4406,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A88" s="5">
         <v>119</v>
       </c>
@@ -4426,7 +4436,7 @@
       <c r="O88" s="5"/>
       <c r="S88" s="4"/>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A89" s="5">
         <f>A88+3</f>
         <v>122</v>
@@ -4464,7 +4474,7 @@
       </c>
       <c r="S89" s="4"/>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A90" s="29">
         <f t="shared" ref="A90:A116" si="5">A89+3</f>
         <v>125</v>
@@ -4509,19 +4519,19 @@
       <c r="R90" s="30"/>
       <c r="S90" s="31"/>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A91" s="35">
         <f t="shared" si="5"/>
         <v>128</v>
       </c>
-      <c r="B91" s="92">
+      <c r="B91" s="88">
         <f t="shared" si="6"/>
         <v>392</v>
       </c>
-      <c r="C91" s="93">
+      <c r="C91" s="89">
         <v>373</v>
       </c>
-      <c r="D91" s="90">
+      <c r="D91" s="86">
         <v>192</v>
       </c>
       <c r="E91" s="5"/>
@@ -4530,20 +4540,20 @@
         <f t="shared" si="7"/>
         <v>128</v>
       </c>
-      <c r="L91" s="92">
+      <c r="L91" s="88">
         <f t="shared" si="4"/>
         <v>425</v>
       </c>
-      <c r="M91" s="93">
+      <c r="M91" s="89">
         <v>406</v>
       </c>
-      <c r="N91" s="91">
+      <c r="N91" s="87">
         <v>239</v>
       </c>
       <c r="O91" s="5"/>
       <c r="S91" s="4"/>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A92" s="5">
         <f t="shared" si="5"/>
         <v>131</v>
@@ -4577,7 +4587,7 @@
       <c r="O92" s="5"/>
       <c r="S92" s="4"/>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A93" s="5">
         <f t="shared" si="5"/>
         <v>134</v>
@@ -4611,7 +4621,7 @@
       <c r="O93" s="5"/>
       <c r="S93" s="4"/>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A94" s="5">
         <f t="shared" si="5"/>
         <v>137</v>
@@ -4649,19 +4659,19 @@
       </c>
       <c r="S94" s="4"/>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A95" s="98">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A95" s="94">
         <f t="shared" si="5"/>
         <v>140</v>
       </c>
-      <c r="B95" s="95">
+      <c r="B95" s="91">
         <f t="shared" si="6"/>
         <v>400</v>
       </c>
-      <c r="C95" s="96">
+      <c r="C95" s="92">
         <v>377</v>
       </c>
-      <c r="D95" s="97">
+      <c r="D95" s="93">
         <v>196</v>
       </c>
       <c r="E95" s="29">
@@ -4674,18 +4684,18 @@
       <c r="H95" s="30"/>
       <c r="I95" s="31"/>
       <c r="J95" s="30"/>
-      <c r="K95" s="98">
+      <c r="K95" s="94">
         <f t="shared" si="7"/>
         <v>140</v>
       </c>
-      <c r="L95" s="95">
+      <c r="L95" s="91">
         <f t="shared" si="4"/>
         <v>433</v>
       </c>
-      <c r="M95" s="96">
+      <c r="M95" s="92">
         <v>410</v>
       </c>
-      <c r="N95" s="102">
+      <c r="N95" s="98">
         <v>243</v>
       </c>
       <c r="O95" s="29">
@@ -4698,7 +4708,7 @@
       <c r="R95" s="30"/>
       <c r="S95" s="31"/>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A96" s="5">
         <f t="shared" si="5"/>
         <v>143</v>
@@ -4734,19 +4744,19 @@
       </c>
       <c r="S96" s="4"/>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A97" s="98">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A97" s="94">
         <f t="shared" si="5"/>
         <v>146</v>
       </c>
-      <c r="B97" s="95">
+      <c r="B97" s="91">
         <f t="shared" si="6"/>
         <v>404</v>
       </c>
-      <c r="C97" s="96">
+      <c r="C97" s="92">
         <v>379</v>
       </c>
-      <c r="D97" s="97">
+      <c r="D97" s="93">
         <v>198</v>
       </c>
       <c r="E97" s="29">
@@ -4759,18 +4769,18 @@
       <c r="H97" s="30"/>
       <c r="I97" s="31"/>
       <c r="J97" s="30"/>
-      <c r="K97" s="98">
+      <c r="K97" s="94">
         <f t="shared" si="7"/>
         <v>146</v>
       </c>
-      <c r="L97" s="95">
+      <c r="L97" s="91">
         <f t="shared" si="4"/>
         <v>437</v>
       </c>
-      <c r="M97" s="96">
+      <c r="M97" s="92">
         <v>412</v>
       </c>
-      <c r="N97" s="102">
+      <c r="N97" s="98">
         <v>245</v>
       </c>
       <c r="O97" s="29">
@@ -4781,7 +4791,7 @@
       <c r="R97" s="30"/>
       <c r="S97" s="31"/>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A98" s="29">
         <f t="shared" si="5"/>
         <v>149</v>
@@ -4823,7 +4833,7 @@
       <c r="R98" s="30"/>
       <c r="S98" s="31"/>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A99" s="5">
         <f t="shared" si="5"/>
         <v>152</v>
@@ -4857,7 +4867,7 @@
       <c r="O99" s="35"/>
       <c r="S99" s="4"/>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A100" s="5">
         <f t="shared" si="5"/>
         <v>155</v>
@@ -4891,7 +4901,7 @@
       <c r="O100" s="5"/>
       <c r="S100" s="4"/>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A101" s="5">
         <f t="shared" si="5"/>
         <v>158</v>
@@ -4929,7 +4939,7 @@
       </c>
       <c r="S101" s="4"/>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A102" s="29">
         <f t="shared" si="5"/>
         <v>161</v>
@@ -4976,19 +4986,19 @@
       <c r="R102" s="30"/>
       <c r="S102" s="31"/>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A103" s="35">
         <f t="shared" si="5"/>
         <v>164</v>
       </c>
-      <c r="B103" s="92">
+      <c r="B103" s="88">
         <f t="shared" si="6"/>
         <v>416</v>
       </c>
-      <c r="C103" s="93">
+      <c r="C103" s="89">
         <v>385</v>
       </c>
-      <c r="D103" s="90">
+      <c r="D103" s="86">
         <v>204</v>
       </c>
       <c r="E103" s="2">
@@ -4999,32 +5009,32 @@
         <f t="shared" si="7"/>
         <v>164</v>
       </c>
-      <c r="L103" s="92">
+      <c r="L103" s="88">
         <f t="shared" si="4"/>
         <v>449</v>
       </c>
-      <c r="M103" s="93">
+      <c r="M103" s="89">
         <v>418</v>
       </c>
-      <c r="N103" s="91">
+      <c r="N103" s="87">
         <v>251</v>
       </c>
       <c r="O103" s="5"/>
       <c r="S103" s="4"/>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A104" s="101">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A104" s="97">
         <f t="shared" si="5"/>
         <v>167</v>
       </c>
-      <c r="B104" s="95">
+      <c r="B104" s="91">
         <f t="shared" si="6"/>
         <v>418</v>
       </c>
-      <c r="C104" s="93">
+      <c r="C104" s="89">
         <v>386</v>
       </c>
-      <c r="D104" s="90">
+      <c r="D104" s="86">
         <v>205</v>
       </c>
       <c r="E104" s="2">
@@ -5034,18 +5044,18 @@
         <v>47</v>
       </c>
       <c r="I104" s="4"/>
-      <c r="K104" s="101">
+      <c r="K104" s="97">
         <f t="shared" si="7"/>
         <v>167</v>
       </c>
-      <c r="L104" s="95">
+      <c r="L104" s="91">
         <f t="shared" si="4"/>
         <v>451</v>
       </c>
-      <c r="M104" s="96">
+      <c r="M104" s="92">
         <v>419</v>
       </c>
-      <c r="N104" s="91">
+      <c r="N104" s="87">
         <v>252</v>
       </c>
       <c r="O104" s="2">
@@ -5053,7 +5063,7 @@
       </c>
       <c r="S104" s="4"/>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A105" s="5">
         <f t="shared" si="5"/>
         <v>170</v>
@@ -5091,7 +5101,7 @@
       </c>
       <c r="S105" s="4"/>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A106" s="5">
         <f t="shared" si="5"/>
         <v>173</v>
@@ -5129,7 +5139,7 @@
       </c>
       <c r="S106" s="4"/>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A107" s="5">
         <f t="shared" si="5"/>
         <v>176</v>
@@ -5165,7 +5175,7 @@
       <c r="O107" s="5"/>
       <c r="S107" s="4"/>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A108" s="5">
         <f t="shared" si="5"/>
         <v>179</v>
@@ -5201,7 +5211,7 @@
       <c r="O108" s="5"/>
       <c r="S108" s="4"/>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A109" s="5">
         <f t="shared" si="5"/>
         <v>182</v>
@@ -5237,7 +5247,7 @@
       <c r="O109" s="5"/>
       <c r="S109" s="4"/>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A110" s="5">
         <f t="shared" si="5"/>
         <v>185</v>
@@ -5275,19 +5285,19 @@
       </c>
       <c r="S110" s="4"/>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A111" s="35">
         <f t="shared" si="5"/>
         <v>188</v>
       </c>
-      <c r="B111" s="92">
+      <c r="B111" s="88">
         <f t="shared" si="6"/>
         <v>432</v>
       </c>
-      <c r="C111" s="93">
+      <c r="C111" s="89">
         <v>393</v>
       </c>
-      <c r="D111" s="90">
+      <c r="D111" s="86">
         <v>212</v>
       </c>
       <c r="E111" s="2">
@@ -5301,14 +5311,14 @@
         <f t="shared" si="7"/>
         <v>188</v>
       </c>
-      <c r="L111" s="92">
+      <c r="L111" s="88">
         <f t="shared" si="4"/>
         <v>465</v>
       </c>
-      <c r="M111" s="93">
+      <c r="M111" s="89">
         <v>426</v>
       </c>
-      <c r="N111" s="91">
+      <c r="N111" s="87">
         <v>259</v>
       </c>
       <c r="O111" s="2">
@@ -5316,7 +5326,7 @@
       </c>
       <c r="S111" s="4"/>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A112" s="5">
         <f t="shared" si="5"/>
         <v>191</v>
@@ -5357,19 +5367,19 @@
       </c>
       <c r="S112" s="4"/>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A113" s="98">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A113" s="94">
         <f t="shared" si="5"/>
         <v>194</v>
       </c>
-      <c r="B113" s="95">
+      <c r="B113" s="91">
         <f t="shared" si="6"/>
         <v>436</v>
       </c>
-      <c r="C113" s="96">
+      <c r="C113" s="92">
         <v>395</v>
       </c>
-      <c r="D113" s="97">
+      <c r="D113" s="93">
         <v>214</v>
       </c>
       <c r="E113" s="29">
@@ -5382,18 +5392,18 @@
       <c r="H113" s="30"/>
       <c r="I113" s="31"/>
       <c r="J113" s="30"/>
-      <c r="K113" s="98">
+      <c r="K113" s="94">
         <f t="shared" si="7"/>
         <v>194</v>
       </c>
-      <c r="L113" s="95">
+      <c r="L113" s="91">
         <f t="shared" si="4"/>
         <v>469</v>
       </c>
-      <c r="M113" s="96">
+      <c r="M113" s="92">
         <v>428</v>
       </c>
-      <c r="N113" s="102">
+      <c r="N113" s="98">
         <v>261</v>
       </c>
       <c r="O113" s="29">
@@ -5406,19 +5416,19 @@
       <c r="R113" s="30"/>
       <c r="S113" s="31"/>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A114" s="35">
         <f t="shared" si="5"/>
         <v>197</v>
       </c>
-      <c r="B114" s="92">
+      <c r="B114" s="88">
         <f t="shared" si="6"/>
         <v>438</v>
       </c>
-      <c r="C114" s="93">
+      <c r="C114" s="89">
         <v>396</v>
       </c>
-      <c r="D114" s="90">
+      <c r="D114" s="86">
         <v>215</v>
       </c>
       <c r="E114" s="2">
@@ -5429,14 +5439,14 @@
         <f t="shared" si="7"/>
         <v>197</v>
       </c>
-      <c r="L114" s="92">
+      <c r="L114" s="88">
         <f t="shared" si="4"/>
         <v>471</v>
       </c>
-      <c r="M114" s="93">
+      <c r="M114" s="89">
         <v>429</v>
       </c>
-      <c r="N114" s="91">
+      <c r="N114" s="87">
         <v>262</v>
       </c>
       <c r="O114" s="2">
@@ -5444,7 +5454,7 @@
       </c>
       <c r="S114" s="4"/>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A115" s="5">
         <f t="shared" si="5"/>
         <v>200</v>
@@ -5478,7 +5488,7 @@
       <c r="O115" s="5"/>
       <c r="S115" s="4"/>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A116" s="6">
         <f t="shared" si="5"/>
         <v>203</v>
@@ -5518,7 +5528,7 @@
       <c r="R116" s="7"/>
       <c r="S116" s="8"/>
     </row>
-    <row r="118" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A118" s="14" t="s">
         <v>0</v>
       </c>
@@ -5530,7 +5540,7 @@
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -5538,34 +5548,34 @@
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A120" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B120" s="40"/>
       <c r="C120" s="9"/>
-      <c r="E120" s="83" t="s">
+      <c r="E120" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="F120" s="84"/>
-      <c r="G120" s="84"/>
-      <c r="H120" s="84"/>
-      <c r="I120" s="84"/>
+      <c r="F120" s="105"/>
+      <c r="G120" s="105"/>
+      <c r="H120" s="105"/>
+      <c r="I120" s="105"/>
       <c r="K120" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L120" s="40"/>
       <c r="M120" s="9"/>
       <c r="N120" s="33"/>
-      <c r="O120" s="83" t="s">
+      <c r="O120" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="P120" s="84"/>
-      <c r="Q120" s="84"/>
-      <c r="R120" s="84"/>
-      <c r="S120" s="84"/>
-    </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P120" s="105"/>
+      <c r="Q120" s="105"/>
+      <c r="R120" s="105"/>
+      <c r="S120" s="105"/>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A121" s="9" t="s">
         <v>10</v>
       </c>
@@ -5621,7 +5631,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>110</v>
       </c>
@@ -5655,7 +5665,7 @@
       <c r="R122" s="30"/>
       <c r="S122" s="31"/>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>116</v>
       </c>
@@ -5685,7 +5695,7 @@
       <c r="O123" s="5"/>
       <c r="S123" s="4"/>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A124" s="32">
         <v>122</v>
       </c>
@@ -5731,17 +5741,17 @@
       <c r="R124" s="30"/>
       <c r="S124" s="31"/>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A125" s="90">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A125" s="86">
         <v>128</v>
       </c>
       <c r="B125" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C125" s="92">
+      <c r="C125" s="88">
         <v>405</v>
       </c>
-      <c r="D125" s="90">
+      <c r="D125" s="86">
         <v>223</v>
       </c>
       <c r="E125" s="2">
@@ -5757,10 +5767,10 @@
       <c r="L125" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="M125" s="93">
+      <c r="M125" s="89">
         <v>438</v>
       </c>
-      <c r="N125" s="90">
+      <c r="N125" s="86">
         <v>270</v>
       </c>
       <c r="O125" s="2">
@@ -5771,7 +5781,7 @@
       </c>
       <c r="S125" s="4"/>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>134</v>
       </c>
@@ -5811,17 +5821,17 @@
       </c>
       <c r="S126" s="4"/>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A127" s="103">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A127" s="99">
         <v>140</v>
       </c>
-      <c r="B127" s="101" t="s">
-        <v>25</v>
-      </c>
-      <c r="C127" s="95">
+      <c r="B127" s="97" t="s">
+        <v>25</v>
+      </c>
+      <c r="C127" s="91">
         <v>407</v>
       </c>
-      <c r="D127" s="97">
+      <c r="D127" s="93">
         <v>225</v>
       </c>
       <c r="E127" s="29">
@@ -5834,16 +5844,16 @@
       <c r="H127" s="30"/>
       <c r="I127" s="31"/>
       <c r="J127" s="30"/>
-      <c r="K127" s="98">
+      <c r="K127" s="94">
         <v>140</v>
       </c>
-      <c r="L127" s="101" t="s">
-        <v>25</v>
-      </c>
-      <c r="M127" s="96">
+      <c r="L127" s="97" t="s">
+        <v>25</v>
+      </c>
+      <c r="M127" s="92">
         <v>440</v>
       </c>
-      <c r="N127" s="97">
+      <c r="N127" s="93">
         <v>272</v>
       </c>
       <c r="O127" s="29">
@@ -5856,17 +5866,17 @@
       <c r="R127" s="30"/>
       <c r="S127" s="31"/>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A128" s="103">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A128" s="99">
         <v>146</v>
       </c>
-      <c r="B128" s="101" t="s">
-        <v>25</v>
-      </c>
-      <c r="C128" s="95">
+      <c r="B128" s="97" t="s">
+        <v>25</v>
+      </c>
+      <c r="C128" s="91">
         <v>408</v>
       </c>
-      <c r="D128" s="97">
+      <c r="D128" s="93">
         <v>226</v>
       </c>
       <c r="E128" s="29">
@@ -5878,16 +5888,16 @@
       <c r="G128" s="30"/>
       <c r="H128" s="30"/>
       <c r="I128" s="31"/>
-      <c r="K128" s="98">
+      <c r="K128" s="94">
         <v>146</v>
       </c>
-      <c r="L128" s="101" t="s">
-        <v>25</v>
-      </c>
-      <c r="M128" s="96">
+      <c r="L128" s="97" t="s">
+        <v>25</v>
+      </c>
+      <c r="M128" s="92">
         <v>441</v>
       </c>
-      <c r="N128" s="97">
+      <c r="N128" s="93">
         <v>273</v>
       </c>
       <c r="O128" s="29">
@@ -5900,7 +5910,7 @@
       <c r="R128" s="30"/>
       <c r="S128" s="31"/>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>152</v>
       </c>
@@ -5943,7 +5953,7 @@
       <c r="R129" s="30"/>
       <c r="S129" s="31"/>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A130" s="32">
         <v>158</v>
       </c>
@@ -5987,17 +5997,17 @@
       <c r="R130" s="30"/>
       <c r="S130" s="31"/>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A131" s="90">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A131" s="86">
         <v>164</v>
       </c>
       <c r="B131" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C131" s="92">
+      <c r="C131" s="88">
         <v>411</v>
       </c>
-      <c r="D131" s="90">
+      <c r="D131" s="86">
         <v>229</v>
       </c>
       <c r="E131" s="2">
@@ -6013,10 +6023,10 @@
       <c r="L131" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="M131" s="93">
+      <c r="M131" s="89">
         <v>444</v>
       </c>
-      <c r="N131" s="90">
+      <c r="N131" s="86">
         <v>276</v>
       </c>
       <c r="O131" s="2">
@@ -6027,7 +6037,7 @@
       </c>
       <c r="S131" s="4"/>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>170</v>
       </c>
@@ -6067,7 +6077,7 @@
       </c>
       <c r="S132" s="4"/>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>176</v>
       </c>
@@ -6113,7 +6123,7 @@
       </c>
       <c r="S133" s="4"/>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>182</v>
       </c>
@@ -6161,17 +6171,17 @@
       <c r="R134" s="56"/>
       <c r="S134" s="57"/>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A135" s="90">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A135" s="86">
         <v>188</v>
       </c>
       <c r="B135" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C135" s="92">
+      <c r="C135" s="88">
         <v>415</v>
       </c>
-      <c r="D135" s="90">
+      <c r="D135" s="86">
         <v>233</v>
       </c>
       <c r="E135" s="2">
@@ -6190,10 +6200,10 @@
       <c r="L135" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="M135" s="93">
+      <c r="M135" s="89">
         <v>448</v>
       </c>
-      <c r="N135" s="90">
+      <c r="N135" s="86">
         <v>280</v>
       </c>
       <c r="O135" s="2">
@@ -6207,17 +6217,17 @@
       </c>
       <c r="S135" s="4"/>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A136" s="103">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A136" s="99">
         <v>194</v>
       </c>
-      <c r="B136" s="101" t="s">
-        <v>25</v>
-      </c>
-      <c r="C136" s="95">
+      <c r="B136" s="97" t="s">
+        <v>25</v>
+      </c>
+      <c r="C136" s="91">
         <v>416</v>
       </c>
-      <c r="D136" s="97">
+      <c r="D136" s="93">
         <v>234</v>
       </c>
       <c r="E136" s="29">
@@ -6231,16 +6241,16 @@
       </c>
       <c r="H136" s="30"/>
       <c r="I136" s="31"/>
-      <c r="K136" s="98">
+      <c r="K136" s="94">
         <v>194</v>
       </c>
-      <c r="L136" s="101" t="s">
-        <v>25</v>
-      </c>
-      <c r="M136" s="96">
+      <c r="L136" s="97" t="s">
+        <v>25</v>
+      </c>
+      <c r="M136" s="92">
         <v>449</v>
       </c>
-      <c r="N136" s="97">
+      <c r="N136" s="93">
         <v>281</v>
       </c>
       <c r="O136" s="29">
@@ -6255,7 +6265,7 @@
       <c r="R136" s="30"/>
       <c r="S136" s="31"/>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>200</v>
       </c>
@@ -6285,7 +6295,7 @@
       <c r="O137" s="5"/>
       <c r="S137" s="4"/>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A138" s="7">
         <v>206</v>
       </c>

</xml_diff>

<commit_message>
MTP051 done with new COP rows; new spreadsheet made for tracking Phobos/Deimos observations
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA1DA92-9734-4038-89FF-001D3D8A03CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C591E7-0AE3-4C73-B75D-8017CF101975}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1337,26 +1337,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:I17"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.88671875" customWidth="1"/>
-    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.33203125" customWidth="1"/>
-    <col min="22" max="22" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.28515625" customWidth="1"/>
+    <col min="22" max="22" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1364,12 +1364,12 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="V2" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>12</v>
       </c>
@@ -1421,7 +1421,7 @@
       <c r="AC4" s="84"/>
       <c r="AD4" s="76"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
         <v>1</v>
       </c>
@@ -1472,7 +1472,7 @@
       <c r="AC5" s="81"/>
       <c r="AD5" s="4"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
         <v>2</v>
       </c>
@@ -1529,7 +1529,7 @@
       <c r="AC6" s="7"/>
       <c r="AD6" s="8"/>
     </row>
-    <row r="8" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C8"/>
       <c r="D8"/>
       <c r="E8"/>
@@ -1538,7 +1538,7 @@
       <c r="H8"/>
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:30" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" s="60" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>24</v>
       </c>
@@ -1546,7 +1546,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
         <v>12</v>
       </c>
@@ -1585,7 +1585,7 @@
       <c r="AC10" s="84"/>
       <c r="AD10" s="76"/>
     </row>
-    <row r="11" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="19" t="s">
         <v>34</v>
       </c>
@@ -1619,7 +1619,9 @@
       <c r="L11" s="15">
         <v>50</v>
       </c>
-      <c r="M11" s="16"/>
+      <c r="M11" s="15">
+        <v>51</v>
+      </c>
       <c r="N11" s="16"/>
       <c r="O11" s="16"/>
       <c r="P11" s="16"/>
@@ -1638,7 +1640,7 @@
       <c r="AC11" s="16"/>
       <c r="AD11" s="17"/>
     </row>
-    <row r="12" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="20" t="s">
         <v>36</v>
       </c>
@@ -1681,7 +1683,7 @@
       <c r="AC12" s="7"/>
       <c r="AD12" s="8"/>
     </row>
-    <row r="13" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>28</v>
       </c>
@@ -1693,14 +1695,14 @@
       <c r="H13"/>
       <c r="I13"/>
     </row>
-    <row r="14" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E14" s="59"/>
       <c r="F14" s="59"/>
       <c r="G14" s="59"/>
       <c r="H14" s="59"/>
       <c r="I14" s="59"/>
     </row>
-    <row r="15" spans="1:30" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>0</v>
       </c>
@@ -1714,12 +1716,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="AB16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>1</v>
       </c>
@@ -1747,7 +1749,7 @@
       <c r="R17" s="105"/>
       <c r="S17" s="105"/>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="39" t="s">
         <v>10</v>
       </c>
@@ -1822,7 +1824,7 @@
       </c>
       <c r="AD18" s="9"/>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="26">
         <v>105</v>
       </c>
@@ -1872,7 +1874,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="25">
         <v>107</v>
       </c>
@@ -1916,7 +1918,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="25">
         <v>120</v>
       </c>
@@ -1960,7 +1962,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="90">
         <v>126</v>
       </c>
@@ -2012,7 +2014,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="25">
         <v>130</v>
       </c>
@@ -2056,7 +2058,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="25">
         <v>134</v>
       </c>
@@ -2100,7 +2102,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="90">
         <v>141</v>
       </c>
@@ -2152,7 +2154,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="25">
         <v>142</v>
       </c>
@@ -2196,7 +2198,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="90">
         <v>146</v>
       </c>
@@ -2242,7 +2244,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="25">
         <v>151</v>
       </c>
@@ -2282,7 +2284,7 @@
       </c>
       <c r="Y28" s="61"/>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="25">
         <v>156</v>
       </c>
@@ -2320,7 +2322,7 @@
       <c r="X29" s="48"/>
       <c r="Y29" s="49"/>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="50">
         <v>162</v>
       </c>
@@ -2366,7 +2368,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="25">
         <v>164</v>
       </c>
@@ -2406,7 +2408,7 @@
       <c r="X31" s="48"/>
       <c r="Y31" s="49"/>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="88">
         <v>166</v>
       </c>
@@ -2446,7 +2448,7 @@
       <c r="X32" s="48"/>
       <c r="Y32" s="49"/>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="25">
         <v>167</v>
       </c>
@@ -2486,7 +2488,7 @@
       <c r="X33" s="48"/>
       <c r="Y33" s="49"/>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="88">
         <v>168</v>
       </c>
@@ -2526,7 +2528,7 @@
       <c r="X34" s="48"/>
       <c r="Y34" s="49"/>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="25">
         <v>169</v>
       </c>
@@ -2564,7 +2566,7 @@
       <c r="X35" s="48"/>
       <c r="Y35" s="49"/>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="25">
         <v>171</v>
       </c>
@@ -2602,7 +2604,7 @@
       <c r="X36" s="48"/>
       <c r="Y36" s="49"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="25">
         <v>172</v>
       </c>
@@ -2640,7 +2642,7 @@
       <c r="X37" s="48"/>
       <c r="Y37" s="49"/>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" s="25">
         <v>178</v>
       </c>
@@ -2678,7 +2680,7 @@
       <c r="X38" s="48"/>
       <c r="Y38" s="49"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" s="25">
         <v>180</v>
       </c>
@@ -2716,7 +2718,7 @@
       <c r="X39" s="48"/>
       <c r="Y39" s="49"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="25">
         <v>182</v>
       </c>
@@ -2754,7 +2756,7 @@
       <c r="X40" s="48"/>
       <c r="Y40" s="49"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="88">
         <v>188</v>
       </c>
@@ -2797,7 +2799,7 @@
       <c r="X41" s="48"/>
       <c r="Y41" s="49"/>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="25">
         <v>191</v>
       </c>
@@ -2842,7 +2844,7 @@
       <c r="X42" s="48"/>
       <c r="Y42" s="49"/>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="90">
         <v>194</v>
       </c>
@@ -2893,7 +2895,7 @@
       <c r="X43" s="48"/>
       <c r="Y43" s="49"/>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="25">
         <v>196</v>
       </c>
@@ -2935,7 +2937,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="88">
         <v>197</v>
       </c>
@@ -2973,7 +2975,7 @@
       <c r="X45" s="5"/>
       <c r="Y45" s="4"/>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="25">
         <v>199</v>
       </c>
@@ -3011,7 +3013,7 @@
       <c r="X46" s="5"/>
       <c r="Y46" s="4"/>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="25">
         <v>201</v>
       </c>
@@ -3047,7 +3049,7 @@
       <c r="X47" s="5"/>
       <c r="Y47" s="4"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" s="34">
         <v>210</v>
       </c>
@@ -3091,7 +3093,7 @@
       <c r="X48" s="5"/>
       <c r="Y48" s="4"/>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="V49" s="5">
         <v>4526.9799999999996</v>
       </c>
@@ -3101,7 +3103,7 @@
       <c r="X49" s="6"/>
       <c r="Y49" s="8"/>
     </row>
-    <row r="50" spans="1:25" ht="18" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A50" s="14" t="s">
         <v>0</v>
       </c>
@@ -3113,7 +3115,7 @@
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -3124,7 +3126,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>1</v>
       </c>
@@ -3152,7 +3154,7 @@
       <c r="R52" s="105"/>
       <c r="S52" s="105"/>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>10</v>
       </c>
@@ -3208,7 +3210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" s="65">
         <v>119</v>
       </c>
@@ -3242,7 +3244,7 @@
       </c>
       <c r="S54" s="4"/>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <f>A54+3</f>
         <v>122</v>
@@ -3276,7 +3278,7 @@
       <c r="O55" s="5"/>
       <c r="S55" s="4"/>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" s="29">
         <f t="shared" ref="A56:A82" si="0">A55+3</f>
         <v>125</v>
@@ -3325,7 +3327,7 @@
       <c r="R56" s="30"/>
       <c r="S56" s="31"/>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" s="35">
         <f t="shared" si="0"/>
         <v>128</v>
@@ -3359,7 +3361,7 @@
       <c r="O57" s="5"/>
       <c r="S57" s="4"/>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <f t="shared" si="0"/>
         <v>131</v>
@@ -3393,7 +3395,7 @@
       <c r="O58" s="5"/>
       <c r="S58" s="4"/>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59" s="65">
         <f t="shared" si="0"/>
         <v>134</v>
@@ -3431,7 +3433,7 @@
       </c>
       <c r="S59" s="4"/>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <f t="shared" si="0"/>
         <v>137</v>
@@ -3465,7 +3467,7 @@
       <c r="O60" s="5"/>
       <c r="S60" s="4"/>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" s="94">
         <f t="shared" si="0"/>
         <v>140</v>
@@ -3514,7 +3516,7 @@
       <c r="R61" s="30"/>
       <c r="S61" s="31"/>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <f t="shared" si="0"/>
         <v>143</v>
@@ -3548,7 +3550,7 @@
       <c r="O62" s="5"/>
       <c r="S62" s="4"/>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A63" s="94">
         <f t="shared" si="0"/>
         <v>146</v>
@@ -3597,7 +3599,7 @@
       <c r="R63" s="30"/>
       <c r="S63" s="31"/>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <f t="shared" si="0"/>
         <v>149</v>
@@ -3631,7 +3633,7 @@
       <c r="O64" s="5"/>
       <c r="S64" s="4"/>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <f t="shared" si="0"/>
         <v>152</v>
@@ -3665,7 +3667,7 @@
       <c r="O65" s="35"/>
       <c r="S65" s="4"/>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <f t="shared" si="0"/>
         <v>155</v>
@@ -3699,7 +3701,7 @@
       <c r="O66" s="5"/>
       <c r="S66" s="4"/>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <f t="shared" si="0"/>
         <v>158</v>
@@ -3733,7 +3735,7 @@
       <c r="O67" s="5"/>
       <c r="S67" s="4"/>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="29">
         <f t="shared" si="0"/>
         <v>161</v>
@@ -3782,7 +3784,7 @@
       <c r="R68" s="30"/>
       <c r="S68" s="31"/>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="95">
         <f t="shared" si="0"/>
         <v>164</v>
@@ -3826,7 +3828,7 @@
       </c>
       <c r="S69" s="4"/>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="95">
         <f t="shared" si="0"/>
         <v>167</v>
@@ -3864,7 +3866,7 @@
       </c>
       <c r="S70" s="4"/>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="65">
         <f t="shared" si="0"/>
         <v>170</v>
@@ -3898,7 +3900,7 @@
       <c r="O71" s="5"/>
       <c r="S71" s="4"/>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="65">
         <f t="shared" si="0"/>
         <v>173</v>
@@ -3932,7 +3934,7 @@
       <c r="O72" s="5"/>
       <c r="S72" s="4"/>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="65">
         <f t="shared" si="0"/>
         <v>176</v>
@@ -3966,7 +3968,7 @@
       <c r="O73" s="5"/>
       <c r="S73" s="4"/>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="65">
         <f t="shared" si="0"/>
         <v>179</v>
@@ -4000,7 +4002,7 @@
       <c r="O74" s="5"/>
       <c r="S74" s="4"/>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="65">
         <f t="shared" si="0"/>
         <v>182</v>
@@ -4034,7 +4036,7 @@
       <c r="O75" s="5"/>
       <c r="S75" s="4"/>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="65">
         <f t="shared" si="0"/>
         <v>185</v>
@@ -4072,7 +4074,7 @@
       </c>
       <c r="S76" s="4"/>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="95">
         <f t="shared" si="0"/>
         <v>188</v>
@@ -4113,7 +4115,7 @@
       </c>
       <c r="S77" s="4"/>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <f t="shared" si="0"/>
         <v>191</v>
@@ -4147,7 +4149,7 @@
       <c r="O78" s="5"/>
       <c r="S78" s="4"/>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="94">
         <f t="shared" si="0"/>
         <v>194</v>
@@ -4192,7 +4194,7 @@
       <c r="R79" s="30"/>
       <c r="S79" s="31"/>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="35">
         <f t="shared" si="0"/>
         <v>197</v>
@@ -4226,7 +4228,7 @@
       <c r="O80" s="5"/>
       <c r="S80" s="4"/>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <f t="shared" si="0"/>
         <v>200</v>
@@ -4260,7 +4262,7 @@
       <c r="O81" s="5"/>
       <c r="S81" s="4"/>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="6">
         <f t="shared" si="0"/>
         <v>203</v>
@@ -4300,7 +4302,7 @@
       <c r="R82" s="7"/>
       <c r="S82" s="8"/>
     </row>
-    <row r="84" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A84" s="14" t="s">
         <v>0</v>
       </c>
@@ -4314,7 +4316,7 @@
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -4322,7 +4324,7 @@
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>1</v>
       </c>
@@ -4350,7 +4352,7 @@
       <c r="R86" s="105"/>
       <c r="S86" s="105"/>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>10</v>
       </c>
@@ -4406,7 +4408,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>119</v>
       </c>
@@ -4436,7 +4438,7 @@
       <c r="O88" s="5"/>
       <c r="S88" s="4"/>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <f>A88+3</f>
         <v>122</v>
@@ -4474,7 +4476,7 @@
       </c>
       <c r="S89" s="4"/>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" s="29">
         <f t="shared" ref="A90:A116" si="5">A89+3</f>
         <v>125</v>
@@ -4519,7 +4521,7 @@
       <c r="R90" s="30"/>
       <c r="S90" s="31"/>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" s="35">
         <f t="shared" si="5"/>
         <v>128</v>
@@ -4553,7 +4555,7 @@
       <c r="O91" s="5"/>
       <c r="S91" s="4"/>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <f t="shared" si="5"/>
         <v>131</v>
@@ -4587,7 +4589,7 @@
       <c r="O92" s="5"/>
       <c r="S92" s="4"/>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <f t="shared" si="5"/>
         <v>134</v>
@@ -4621,7 +4623,7 @@
       <c r="O93" s="5"/>
       <c r="S93" s="4"/>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <f t="shared" si="5"/>
         <v>137</v>
@@ -4659,7 +4661,7 @@
       </c>
       <c r="S94" s="4"/>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" s="94">
         <f t="shared" si="5"/>
         <v>140</v>
@@ -4708,7 +4710,7 @@
       <c r="R95" s="30"/>
       <c r="S95" s="31"/>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <f t="shared" si="5"/>
         <v>143</v>
@@ -4744,7 +4746,7 @@
       </c>
       <c r="S96" s="4"/>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97" s="94">
         <f t="shared" si="5"/>
         <v>146</v>
@@ -4791,7 +4793,7 @@
       <c r="R97" s="30"/>
       <c r="S97" s="31"/>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98" s="29">
         <f t="shared" si="5"/>
         <v>149</v>
@@ -4833,7 +4835,7 @@
       <c r="R98" s="30"/>
       <c r="S98" s="31"/>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <f t="shared" si="5"/>
         <v>152</v>
@@ -4867,7 +4869,7 @@
       <c r="O99" s="35"/>
       <c r="S99" s="4"/>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <f t="shared" si="5"/>
         <v>155</v>
@@ -4901,7 +4903,7 @@
       <c r="O100" s="5"/>
       <c r="S100" s="4"/>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
         <f t="shared" si="5"/>
         <v>158</v>
@@ -4939,7 +4941,7 @@
       </c>
       <c r="S101" s="4"/>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A102" s="29">
         <f t="shared" si="5"/>
         <v>161</v>
@@ -4986,7 +4988,7 @@
       <c r="R102" s="30"/>
       <c r="S102" s="31"/>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A103" s="35">
         <f t="shared" si="5"/>
         <v>164</v>
@@ -5022,7 +5024,7 @@
       <c r="O103" s="5"/>
       <c r="S103" s="4"/>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104" s="97">
         <f t="shared" si="5"/>
         <v>167</v>
@@ -5063,7 +5065,7 @@
       </c>
       <c r="S104" s="4"/>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <f t="shared" si="5"/>
         <v>170</v>
@@ -5101,7 +5103,7 @@
       </c>
       <c r="S105" s="4"/>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
         <f t="shared" si="5"/>
         <v>173</v>
@@ -5139,7 +5141,7 @@
       </c>
       <c r="S106" s="4"/>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
         <f t="shared" si="5"/>
         <v>176</v>
@@ -5175,7 +5177,7 @@
       <c r="O107" s="5"/>
       <c r="S107" s="4"/>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <f t="shared" si="5"/>
         <v>179</v>
@@ -5211,7 +5213,7 @@
       <c r="O108" s="5"/>
       <c r="S108" s="4"/>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
         <f t="shared" si="5"/>
         <v>182</v>
@@ -5247,7 +5249,7 @@
       <c r="O109" s="5"/>
       <c r="S109" s="4"/>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
         <f t="shared" si="5"/>
         <v>185</v>
@@ -5285,7 +5287,7 @@
       </c>
       <c r="S110" s="4"/>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A111" s="35">
         <f t="shared" si="5"/>
         <v>188</v>
@@ -5326,7 +5328,7 @@
       </c>
       <c r="S111" s="4"/>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" s="5">
         <f t="shared" si="5"/>
         <v>191</v>
@@ -5367,7 +5369,7 @@
       </c>
       <c r="S112" s="4"/>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113" s="94">
         <f t="shared" si="5"/>
         <v>194</v>
@@ -5416,7 +5418,7 @@
       <c r="R113" s="30"/>
       <c r="S113" s="31"/>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" s="35">
         <f t="shared" si="5"/>
         <v>197</v>
@@ -5454,7 +5456,7 @@
       </c>
       <c r="S114" s="4"/>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115" s="5">
         <f t="shared" si="5"/>
         <v>200</v>
@@ -5488,7 +5490,7 @@
       <c r="O115" s="5"/>
       <c r="S115" s="4"/>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A116" s="6">
         <f t="shared" si="5"/>
         <v>203</v>
@@ -5528,7 +5530,7 @@
       <c r="R116" s="7"/>
       <c r="S116" s="8"/>
     </row>
-    <row r="118" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A118" s="14" t="s">
         <v>0</v>
       </c>
@@ -5540,7 +5542,7 @@
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -5548,7 +5550,7 @@
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
         <v>1</v>
       </c>
@@ -5575,7 +5577,7 @@
       <c r="R120" s="105"/>
       <c r="S120" s="105"/>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
         <v>10</v>
       </c>
@@ -5631,7 +5633,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>110</v>
       </c>
@@ -5665,7 +5667,7 @@
       <c r="R122" s="30"/>
       <c r="S122" s="31"/>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>116</v>
       </c>
@@ -5695,7 +5697,7 @@
       <c r="O123" s="5"/>
       <c r="S123" s="4"/>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124" s="32">
         <v>122</v>
       </c>
@@ -5741,7 +5743,7 @@
       <c r="R124" s="30"/>
       <c r="S124" s="31"/>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125" s="86">
         <v>128</v>
       </c>
@@ -5781,7 +5783,7 @@
       </c>
       <c r="S125" s="4"/>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>134</v>
       </c>
@@ -5821,7 +5823,7 @@
       </c>
       <c r="S126" s="4"/>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127" s="99">
         <v>140</v>
       </c>
@@ -5866,7 +5868,7 @@
       <c r="R127" s="30"/>
       <c r="S127" s="31"/>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A128" s="99">
         <v>146</v>
       </c>
@@ -5910,7 +5912,7 @@
       <c r="R128" s="30"/>
       <c r="S128" s="31"/>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>152</v>
       </c>
@@ -5928,6 +5930,9 @@
       </c>
       <c r="F129" s="63">
         <v>33</v>
+      </c>
+      <c r="G129" s="3">
+        <v>51</v>
       </c>
       <c r="I129" s="4"/>
       <c r="J129" s="30"/>
@@ -5953,7 +5958,7 @@
       <c r="R129" s="30"/>
       <c r="S129" s="31"/>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A130" s="32">
         <v>158</v>
       </c>
@@ -5972,7 +5977,9 @@
       <c r="F130" s="32">
         <v>12</v>
       </c>
-      <c r="G130" s="30"/>
+      <c r="G130" s="32">
+        <v>51</v>
+      </c>
       <c r="H130" s="30"/>
       <c r="I130" s="31"/>
       <c r="K130" s="29">
@@ -5997,7 +6004,7 @@
       <c r="R130" s="30"/>
       <c r="S130" s="31"/>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131" s="86">
         <v>164</v>
       </c>
@@ -6015,6 +6022,9 @@
       </c>
       <c r="F131" s="77">
         <v>28</v>
+      </c>
+      <c r="G131" s="98">
+        <v>51</v>
       </c>
       <c r="I131" s="4"/>
       <c r="K131" s="35">
@@ -6037,7 +6047,7 @@
       </c>
       <c r="S131" s="4"/>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>170</v>
       </c>
@@ -6055,6 +6065,9 @@
       </c>
       <c r="F132" s="77">
         <v>28</v>
+      </c>
+      <c r="G132" s="3">
+        <v>51</v>
       </c>
       <c r="I132" s="4"/>
       <c r="K132" s="5">
@@ -6077,7 +6090,7 @@
       </c>
       <c r="S132" s="4"/>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>176</v>
       </c>
@@ -6123,7 +6136,7 @@
       </c>
       <c r="S133" s="4"/>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>182</v>
       </c>
@@ -6142,7 +6155,7 @@
       <c r="F134" s="3">
         <v>28</v>
       </c>
-      <c r="G134">
+      <c r="G134" s="3">
         <v>42</v>
       </c>
       <c r="I134" s="4"/>
@@ -6165,13 +6178,13 @@
       <c r="P134" s="32">
         <v>31</v>
       </c>
-      <c r="Q134" s="56">
+      <c r="Q134" s="77">
         <v>42</v>
       </c>
       <c r="R134" s="56"/>
       <c r="S134" s="57"/>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A135" s="86">
         <v>188</v>
       </c>
@@ -6217,7 +6230,7 @@
       </c>
       <c r="S135" s="4"/>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A136" s="99">
         <v>194</v>
       </c>
@@ -6236,7 +6249,7 @@
       <c r="F136" s="32">
         <v>12</v>
       </c>
-      <c r="G136" s="30">
+      <c r="G136" s="32">
         <v>42</v>
       </c>
       <c r="H136" s="30"/>
@@ -6259,13 +6272,13 @@
       <c r="P136" s="32">
         <v>31</v>
       </c>
-      <c r="Q136" s="30">
+      <c r="Q136" s="32">
         <v>42</v>
       </c>
       <c r="R136" s="30"/>
       <c r="S136" s="31"/>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>200</v>
       </c>
@@ -6295,7 +6308,7 @@
       <c r="O137" s="5"/>
       <c r="S137" s="4"/>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A138" s="7">
         <v>206</v>
       </c>

</xml_diff>

<commit_message>
MTP053 done; UVIS observation names added from MTP040
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971A4DE5-CD7B-4650-A0A7-3636807F01E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADE3323-93C3-480B-927D-7B830B9369E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3105" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1358,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N132" sqref="N132"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R129" sqref="R129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5986,8 +5986,7 @@
       <c r="O123">
         <v>268</v>
       </c>
-      <c r="P123" s="5"/>
-      <c r="R123" s="3">
+      <c r="P123" s="3">
         <v>52</v>
       </c>
       <c r="T123" s="4"/>
@@ -6163,7 +6162,9 @@
       <c r="G127" s="32">
         <v>12</v>
       </c>
-      <c r="H127" s="30"/>
+      <c r="H127" s="32">
+        <v>53</v>
+      </c>
       <c r="I127" s="30"/>
       <c r="J127" s="31"/>
       <c r="K127" s="30"/>
@@ -6213,7 +6214,9 @@
       <c r="G128" s="63">
         <v>23</v>
       </c>
-      <c r="H128" s="30"/>
+      <c r="H128" s="32">
+        <v>53</v>
+      </c>
       <c r="I128" s="30"/>
       <c r="J128" s="31"/>
       <c r="L128" s="94">
@@ -6285,7 +6288,9 @@
       <c r="Q129" s="32">
         <v>29</v>
       </c>
-      <c r="R129" s="30"/>
+      <c r="R129" s="77">
+        <v>53</v>
+      </c>
       <c r="S129" s="30"/>
       <c r="T129" s="31"/>
     </row>
@@ -6334,7 +6339,9 @@
       <c r="Q130" s="32">
         <v>29</v>
       </c>
-      <c r="R130" s="30"/>
+      <c r="R130" s="32">
+        <v>53</v>
+      </c>
       <c r="S130" s="30"/>
       <c r="T130" s="31"/>
     </row>
@@ -6382,6 +6389,9 @@
       <c r="Q131" s="32">
         <v>29</v>
       </c>
+      <c r="R131" s="77">
+        <v>53</v>
+      </c>
       <c r="T131" s="4"/>
     </row>
     <row r="132" spans="1:20" x14ac:dyDescent="0.25">
@@ -6427,6 +6437,9 @@
       </c>
       <c r="Q132" s="32">
         <v>31</v>
+      </c>
+      <c r="R132" s="77">
+        <v>53</v>
       </c>
       <c r="T132" s="4"/>
     </row>

</xml_diff>

<commit_message>
MTP054 COP rows generated. Readme updated.
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADE3323-93C3-480B-927D-7B830B9369E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49642527-3A51-4711-8B48-A6BF1142AC09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1358,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R129" sqref="R129"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2064,7 +2064,9 @@
       <c r="E23" s="60">
         <v>58</v>
       </c>
-      <c r="F23" s="5"/>
+      <c r="F23" s="2">
+        <v>54</v>
+      </c>
       <c r="J23" s="4"/>
       <c r="L23" s="25">
         <v>130</v>
@@ -2111,7 +2113,9 @@
       <c r="E24" s="60">
         <v>59</v>
       </c>
-      <c r="F24" s="5"/>
+      <c r="F24" s="2">
+        <v>54</v>
+      </c>
       <c r="J24" s="4"/>
       <c r="L24" s="25">
         <v>134</v>
@@ -2213,7 +2217,9 @@
       <c r="E26" s="60">
         <v>61</v>
       </c>
-      <c r="F26" s="5"/>
+      <c r="F26" s="2">
+        <v>54</v>
+      </c>
       <c r="J26" s="4"/>
       <c r="L26" s="25">
         <v>142</v>
@@ -2309,7 +2315,9 @@
       <c r="E28" s="60">
         <v>63</v>
       </c>
-      <c r="F28" s="5"/>
+      <c r="F28" s="2">
+        <v>54</v>
+      </c>
       <c r="J28" s="4"/>
       <c r="L28" s="25">
         <v>151</v>

</xml_diff>

<commit_message>
MTP055 done, one merged occ changed to a grazing occ to match summary files
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49642527-3A51-4711-8B48-A6BF1142AC09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D60014-558E-4CB5-A364-315F74A693BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1359,7 +1359,7 @@
   <dimension ref="A1:AE147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1534,7 +1534,9 @@
       <c r="O6" s="18">
         <v>49</v>
       </c>
-      <c r="P6" s="7"/>
+      <c r="P6" s="18">
+        <v>55</v>
+      </c>
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
@@ -5276,7 +5278,9 @@
       <c r="O103" s="87">
         <v>251</v>
       </c>
-      <c r="P103" s="5"/>
+      <c r="P103" s="2">
+        <v>55</v>
+      </c>
       <c r="T103" s="4"/>
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.25">
@@ -5441,7 +5445,9 @@
       <c r="O107" s="59">
         <v>255</v>
       </c>
-      <c r="P107" s="5"/>
+      <c r="P107" s="2">
+        <v>55</v>
+      </c>
       <c r="T107" s="4"/>
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.25">
@@ -5480,7 +5486,9 @@
       <c r="O108" s="59">
         <v>256</v>
       </c>
-      <c r="P108" s="5"/>
+      <c r="P108" s="2">
+        <v>55</v>
+      </c>
       <c r="T108" s="4"/>
     </row>
     <row r="109" spans="1:20" x14ac:dyDescent="0.25">
@@ -5519,7 +5527,9 @@
       <c r="O109" s="59">
         <v>257</v>
       </c>
-      <c r="P109" s="5"/>
+      <c r="P109" s="2">
+        <v>55</v>
+      </c>
       <c r="T109" s="4"/>
     </row>
     <row r="110" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
MTP056 done; new Phobos obs added to spreadsheet
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D60014-558E-4CB5-A364-315F74A693BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204FF897-BC0C-4598-9C48-676219E6B4B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1358,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2468,7 +2468,9 @@
       <c r="O31" s="60">
         <v>113</v>
       </c>
-      <c r="P31" s="5"/>
+      <c r="P31" s="2">
+        <v>56</v>
+      </c>
       <c r="T31" s="4"/>
       <c r="W31" s="5">
         <v>3693.76</v>
@@ -2511,7 +2513,9 @@
       <c r="O32" s="86">
         <v>114</v>
       </c>
-      <c r="P32" s="5"/>
+      <c r="P32" s="2">
+        <v>56</v>
+      </c>
       <c r="T32" s="4"/>
       <c r="W32" s="5">
         <v>3752.1</v>
@@ -2554,7 +2558,9 @@
       <c r="O33" s="60">
         <v>115</v>
       </c>
-      <c r="P33" s="5"/>
+      <c r="P33" s="2">
+        <v>56</v>
+      </c>
       <c r="T33" s="4"/>
       <c r="W33" s="5">
         <v>3766.97</v>
@@ -2597,7 +2603,9 @@
       <c r="O34" s="86">
         <v>116</v>
       </c>
-      <c r="P34" s="5"/>
+      <c r="P34" s="2">
+        <v>56</v>
+      </c>
       <c r="T34" s="4"/>
       <c r="W34" s="5">
         <v>3784.4</v>

</xml_diff>

<commit_message>
MTP058 COP rows generated
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B79088-AB3E-431D-8706-F4E3CED9707A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB09E15-C497-49F7-AAB9-426867F51301}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -894,7 +894,7 @@
     <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -954,18 +954,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -982,13 +972,9 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -998,13 +984,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1016,10 +1000,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1032,7 +1013,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1358,13 +1339,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J104" sqref="J104"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O53" sqref="O53:O54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" style="60" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.140625" customWidth="1"/>
@@ -1414,40 +1395,40 @@
       <c r="E4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="58" t="s">
+      <c r="F4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="84"/>
-      <c r="L4" s="84"/>
-      <c r="M4" s="84"/>
-      <c r="N4" s="84"/>
-      <c r="O4" s="84"/>
-      <c r="P4" s="84"/>
-      <c r="Q4" s="84"/>
-      <c r="R4" s="84"/>
-      <c r="S4" s="84"/>
-      <c r="T4" s="84"/>
-      <c r="U4" s="84"/>
-      <c r="V4" s="84"/>
-      <c r="W4" s="84"/>
-      <c r="X4" s="84"/>
-      <c r="Y4" s="84"/>
-      <c r="Z4" s="84"/>
-      <c r="AA4" s="84"/>
-      <c r="AB4" s="84"/>
-      <c r="AC4" s="84"/>
-      <c r="AD4" s="84"/>
-      <c r="AE4" s="76"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="71"/>
+      <c r="M4" s="71"/>
+      <c r="N4" s="71"/>
+      <c r="O4" s="71"/>
+      <c r="P4" s="71"/>
+      <c r="Q4" s="71"/>
+      <c r="R4" s="71"/>
+      <c r="S4" s="71"/>
+      <c r="T4" s="71"/>
+      <c r="U4" s="71"/>
+      <c r="V4" s="71"/>
+      <c r="W4" s="71"/>
+      <c r="X4" s="71"/>
+      <c r="Y4" s="71"/>
+      <c r="Z4" s="71"/>
+      <c r="AA4" s="71"/>
+      <c r="AB4" s="71"/>
+      <c r="AC4" s="71"/>
+      <c r="AD4" s="71"/>
+      <c r="AE4" s="65"/>
     </row>
     <row r="5" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C5" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="78">
+      <c r="D5" s="66">
         <v>107</v>
       </c>
       <c r="E5" s="36" t="s">
@@ -1456,55 +1437,37 @@
       <c r="F5" s="2">
         <v>3</v>
       </c>
-      <c r="G5" s="64">
+      <c r="G5" s="3">
         <v>7</v>
       </c>
-      <c r="H5" s="64">
+      <c r="H5" s="3">
         <v>12</v>
       </c>
-      <c r="I5" s="64">
+      <c r="I5" s="3">
         <v>19</v>
       </c>
-      <c r="J5" s="64">
+      <c r="J5" s="3">
         <v>22</v>
       </c>
-      <c r="K5" s="64">
+      <c r="K5" s="3">
         <v>34</v>
       </c>
-      <c r="L5" s="64">
+      <c r="L5" s="3">
         <v>49</v>
       </c>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="81"/>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="81"/>
-      <c r="S5" s="81"/>
-      <c r="T5" s="81"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="81"/>
-      <c r="W5" s="81"/>
-      <c r="X5" s="81"/>
-      <c r="Y5" s="81"/>
-      <c r="Z5" s="81"/>
-      <c r="AA5" s="81"/>
-      <c r="AB5" s="81"/>
-      <c r="AC5" s="81"/>
-      <c r="AD5" s="81"/>
       <c r="AE5" s="4"/>
     </row>
     <row r="6" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="79">
+      <c r="D6" s="67">
         <v>57</v>
       </c>
       <c r="E6" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="82">
+      <c r="F6" s="69">
         <v>3</v>
       </c>
       <c r="G6" s="18">
@@ -1553,24 +1516,14 @@
       <c r="AD6" s="7"/>
       <c r="AE6" s="8"/>
     </row>
-    <row r="8" spans="2:31" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8"/>
-    </row>
-    <row r="9" spans="2:31" s="60" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:31" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C9"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="2:31" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
@@ -1580,46 +1533,46 @@
       <c r="E10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="102" t="s">
+      <c r="F10" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="103"/>
-      <c r="H10" s="103"/>
-      <c r="I10" s="103"/>
-      <c r="J10" s="103"/>
-      <c r="K10" s="84"/>
-      <c r="L10" s="84"/>
-      <c r="M10" s="84"/>
-      <c r="N10" s="84"/>
-      <c r="O10" s="84"/>
-      <c r="P10" s="84"/>
-      <c r="Q10" s="84"/>
-      <c r="R10" s="84"/>
-      <c r="S10" s="84"/>
-      <c r="T10" s="84"/>
-      <c r="U10" s="84"/>
-      <c r="V10" s="84"/>
-      <c r="W10" s="84"/>
-      <c r="X10" s="84"/>
-      <c r="Y10" s="84"/>
-      <c r="Z10" s="84"/>
-      <c r="AA10" s="84"/>
-      <c r="AB10" s="84"/>
-      <c r="AC10" s="84"/>
-      <c r="AD10" s="84"/>
-      <c r="AE10" s="76"/>
-    </row>
-    <row r="11" spans="2:31" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="86"/>
+      <c r="H10" s="86"/>
+      <c r="I10" s="86"/>
+      <c r="J10" s="86"/>
+      <c r="K10" s="71"/>
+      <c r="L10" s="71"/>
+      <c r="M10" s="71"/>
+      <c r="N10" s="71"/>
+      <c r="O10" s="71"/>
+      <c r="P10" s="71"/>
+      <c r="Q10" s="71"/>
+      <c r="R10" s="71"/>
+      <c r="S10" s="71"/>
+      <c r="T10" s="71"/>
+      <c r="U10" s="71"/>
+      <c r="V10" s="71"/>
+      <c r="W10" s="71"/>
+      <c r="X10" s="71"/>
+      <c r="Y10" s="71"/>
+      <c r="Z10" s="71"/>
+      <c r="AA10" s="71"/>
+      <c r="AB10" s="71"/>
+      <c r="AC10" s="71"/>
+      <c r="AD10" s="71"/>
+      <c r="AE10" s="65"/>
+    </row>
+    <row r="11" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C11" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="78">
+      <c r="D11" s="66">
         <v>3973</v>
       </c>
       <c r="E11" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="83">
+      <c r="F11" s="70">
         <v>5</v>
       </c>
       <c r="G11" s="15">
@@ -1664,17 +1617,17 @@
       <c r="AD11" s="16"/>
       <c r="AE11" s="17"/>
     </row>
-    <row r="12" spans="2:31" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C12" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="79">
+      <c r="D12" s="67">
         <v>674</v>
       </c>
-      <c r="E12" s="80" t="s">
+      <c r="E12" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="82">
+      <c r="F12" s="69">
         <v>15</v>
       </c>
       <c r="G12" s="18">
@@ -1683,7 +1636,9 @@
       <c r="H12" s="18">
         <v>44</v>
       </c>
-      <c r="I12" s="7"/>
+      <c r="I12" s="18">
+        <v>58</v>
+      </c>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
@@ -1707,24 +1662,10 @@
       <c r="AD12" s="7"/>
       <c r="AE12" s="8"/>
     </row>
-    <row r="13" spans="2:31" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>28</v>
       </c>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="J13"/>
-    </row>
-    <row r="14" spans="2:31" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="59"/>
     </row>
     <row r="15" spans="2:31" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B15" s="14" t="s">
@@ -1736,7 +1677,7 @@
       <c r="D15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="100" t="s">
+      <c r="F15" s="83" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1751,27 +1692,27 @@
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="104" t="s">
+      <c r="E17" s="9"/>
+      <c r="F17" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="105"/>
-      <c r="H17" s="105"/>
-      <c r="I17" s="105"/>
-      <c r="J17" s="105"/>
+      <c r="G17" s="88"/>
+      <c r="H17" s="88"/>
+      <c r="I17" s="88"/>
+      <c r="J17" s="88"/>
       <c r="L17" s="9" t="s">
         <v>2</v>
       </c>
       <c r="M17" s="13"/>
       <c r="N17" s="9"/>
-      <c r="O17" s="58"/>
-      <c r="P17" s="104" t="s">
+      <c r="O17" s="9"/>
+      <c r="P17" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="Q17" s="105"/>
-      <c r="R17" s="105"/>
-      <c r="S17" s="105"/>
-      <c r="T17" s="105"/>
+      <c r="Q17" s="88"/>
+      <c r="R17" s="88"/>
+      <c r="S17" s="88"/>
+      <c r="T17" s="88"/>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B18" s="39" t="s">
@@ -1780,7 +1721,7 @@
       <c r="C18" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="74" t="s">
+      <c r="D18" s="63" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="13" t="s">
@@ -1807,7 +1748,7 @@
       <c r="M18" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="N18" s="67" t="s">
+      <c r="N18" s="57" t="s">
         <v>21</v>
       </c>
       <c r="O18" s="13" t="s">
@@ -1849,7 +1790,7 @@
       <c r="AE18" s="9"/>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A19" s="60">
+      <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" s="26">
@@ -1858,7 +1799,7 @@
       <c r="C19" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="68">
+      <c r="D19" s="58">
         <v>295</v>
       </c>
       <c r="E19">
@@ -1875,7 +1816,7 @@
       <c r="M19" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="N19" s="68">
+      <c r="N19" s="58">
         <v>328</v>
       </c>
       <c r="O19">
@@ -1894,15 +1835,15 @@
       </c>
       <c r="Y19" s="5"/>
       <c r="Z19" s="4"/>
-      <c r="AC19" s="86">
+      <c r="AC19" s="73">
         <v>2927.1</v>
       </c>
-      <c r="AD19" s="86">
+      <c r="AD19" s="73">
         <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A20" s="60">
+      <c r="A20">
         <v>1</v>
       </c>
       <c r="B20" s="25">
@@ -1911,7 +1852,7 @@
       <c r="C20" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="69">
+      <c r="D20" s="59">
         <v>296</v>
       </c>
       <c r="E20">
@@ -1925,7 +1866,7 @@
       <c r="M20" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N20" s="69">
+      <c r="N20" s="59">
         <v>329</v>
       </c>
       <c r="O20">
@@ -1941,15 +1882,15 @@
       </c>
       <c r="Y20" s="5"/>
       <c r="Z20" s="4"/>
-      <c r="AC20" s="86">
+      <c r="AC20" s="73">
         <v>3172.9</v>
       </c>
-      <c r="AD20" s="86">
+      <c r="AD20" s="73">
         <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A21" s="60">
+      <c r="A21">
         <v>1</v>
       </c>
       <c r="B21" s="25">
@@ -1958,10 +1899,10 @@
       <c r="C21" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="69">
+      <c r="D21" s="59">
         <v>297</v>
       </c>
-      <c r="E21" s="60">
+      <c r="E21">
         <v>56</v>
       </c>
       <c r="F21" s="5"/>
@@ -1972,10 +1913,10 @@
       <c r="M21" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N21" s="69">
+      <c r="N21" s="59">
         <v>330</v>
       </c>
-      <c r="O21" s="60">
+      <c r="O21">
         <v>103</v>
       </c>
       <c r="P21" s="5"/>
@@ -1988,43 +1929,43 @@
       </c>
       <c r="Y21" s="5"/>
       <c r="Z21" s="4"/>
-      <c r="AC21" s="86">
+      <c r="AC21" s="73">
         <v>3289.6</v>
       </c>
-      <c r="AD21" s="86">
+      <c r="AD21" s="73">
         <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A22" s="60">
+      <c r="A22">
         <v>1</v>
       </c>
-      <c r="B22" s="90">
+      <c r="B22" s="76">
         <v>126</v>
       </c>
-      <c r="C22" s="91" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="92">
+      <c r="C22" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="78">
         <v>298</v>
       </c>
-      <c r="E22" s="93">
+      <c r="E22" s="79">
         <v>57</v>
       </c>
       <c r="F22" s="2">
         <v>11</v>
       </c>
       <c r="J22" s="4"/>
-      <c r="L22" s="90">
+      <c r="L22" s="76">
         <v>126</v>
       </c>
-      <c r="M22" s="91" t="s">
-        <v>25</v>
-      </c>
-      <c r="N22" s="92">
+      <c r="M22" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="N22" s="78">
         <v>331</v>
       </c>
-      <c r="O22" s="93">
+      <c r="O22" s="79">
         <v>104</v>
       </c>
       <c r="P22" s="2">
@@ -2043,15 +1984,15 @@
       <c r="Z22" s="49">
         <v>126</v>
       </c>
-      <c r="AC22" s="86">
+      <c r="AC22" s="73">
         <v>3750.1</v>
       </c>
-      <c r="AD22" s="87">
+      <c r="AD22" s="73">
         <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A23" s="60">
+      <c r="A23">
         <v>1</v>
       </c>
       <c r="B23" s="25">
@@ -2060,10 +2001,10 @@
       <c r="C23" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="69">
+      <c r="D23" s="59">
         <v>299</v>
       </c>
-      <c r="E23" s="60">
+      <c r="E23">
         <v>58</v>
       </c>
       <c r="F23" s="2">
@@ -2076,10 +2017,10 @@
       <c r="M23" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N23" s="69">
+      <c r="N23" s="59">
         <v>332</v>
       </c>
-      <c r="O23" s="60">
+      <c r="O23">
         <v>105</v>
       </c>
       <c r="P23" s="5"/>
@@ -2092,15 +2033,15 @@
       </c>
       <c r="Y23" s="48"/>
       <c r="Z23" s="49"/>
-      <c r="AC23" s="86">
+      <c r="AC23" s="73">
         <v>3787.9</v>
       </c>
-      <c r="AD23" s="87">
+      <c r="AD23" s="73">
         <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A24" s="60">
+      <c r="A24">
         <v>1</v>
       </c>
       <c r="B24" s="25">
@@ -2109,10 +2050,10 @@
       <c r="C24" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="69">
+      <c r="D24" s="59">
         <v>300</v>
       </c>
-      <c r="E24" s="60">
+      <c r="E24">
         <v>59</v>
       </c>
       <c r="F24" s="2">
@@ -2125,10 +2066,10 @@
       <c r="M24" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N24" s="69">
+      <c r="N24" s="59">
         <v>333</v>
       </c>
-      <c r="O24" s="60">
+      <c r="O24">
         <v>106</v>
       </c>
       <c r="P24" s="5"/>
@@ -2141,43 +2082,43 @@
       </c>
       <c r="Y24" s="48"/>
       <c r="Z24" s="49"/>
-      <c r="AC24" s="86">
+      <c r="AC24" s="73">
         <v>4276.1000000000004</v>
       </c>
-      <c r="AD24" s="87">
+      <c r="AD24" s="73">
         <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A25" s="60">
+      <c r="A25">
         <v>1</v>
       </c>
-      <c r="B25" s="90">
+      <c r="B25" s="76">
         <v>141</v>
       </c>
-      <c r="C25" s="91" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="92">
+      <c r="C25" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="78">
         <v>301</v>
       </c>
-      <c r="E25" s="93">
+      <c r="E25" s="79">
         <v>60</v>
       </c>
       <c r="F25" s="2">
         <v>11</v>
       </c>
       <c r="J25" s="4"/>
-      <c r="L25" s="90">
+      <c r="L25" s="76">
         <v>141</v>
       </c>
-      <c r="M25" s="91" t="s">
-        <v>25</v>
-      </c>
-      <c r="N25" s="92">
+      <c r="M25" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="N25" s="78">
         <v>334</v>
       </c>
-      <c r="O25" s="93">
+      <c r="O25" s="79">
         <v>107</v>
       </c>
       <c r="P25" s="2">
@@ -2196,15 +2137,15 @@
       <c r="Z25" s="49">
         <v>141</v>
       </c>
-      <c r="AC25" s="86">
+      <c r="AC25" s="73">
         <v>4383.5</v>
       </c>
-      <c r="AD25" s="87">
+      <c r="AD25" s="73">
         <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A26" s="60">
+      <c r="A26">
         <v>1</v>
       </c>
       <c r="B26" s="25">
@@ -2213,10 +2154,10 @@
       <c r="C26" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="69">
+      <c r="D26" s="59">
         <v>302</v>
       </c>
-      <c r="E26" s="60">
+      <c r="E26">
         <v>61</v>
       </c>
       <c r="F26" s="2">
@@ -2229,10 +2170,10 @@
       <c r="M26" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N26" s="69">
+      <c r="N26" s="59">
         <v>335</v>
       </c>
-      <c r="O26" s="60">
+      <c r="O26">
         <v>108</v>
       </c>
       <c r="P26" s="5"/>
@@ -2245,43 +2186,43 @@
       </c>
       <c r="Y26" s="48"/>
       <c r="Z26" s="49"/>
-      <c r="AC26" s="86">
+      <c r="AC26" s="73">
         <v>4448.5</v>
       </c>
-      <c r="AD26" s="87">
+      <c r="AD26" s="73">
         <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A27" s="60">
+      <c r="A27">
         <v>1</v>
       </c>
-      <c r="B27" s="90">
+      <c r="B27" s="76">
         <v>146</v>
       </c>
-      <c r="C27" s="91" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="92">
+      <c r="C27" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="78">
         <v>303</v>
       </c>
-      <c r="E27" s="93">
+      <c r="E27" s="79">
         <v>62</v>
       </c>
       <c r="F27" s="2">
         <v>11</v>
       </c>
       <c r="J27" s="4"/>
-      <c r="L27" s="90">
+      <c r="L27" s="76">
         <v>146</v>
       </c>
-      <c r="M27" s="91" t="s">
-        <v>25</v>
-      </c>
-      <c r="N27" s="92">
+      <c r="M27" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="N27" s="78">
         <v>336</v>
       </c>
-      <c r="O27" s="93">
+      <c r="O27" s="79">
         <v>109</v>
       </c>
       <c r="P27" s="2">
@@ -2302,7 +2243,7 @@
       </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A28" s="60">
+      <c r="A28">
         <v>1</v>
       </c>
       <c r="B28" s="25">
@@ -2311,10 +2252,10 @@
       <c r="C28" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="69">
+      <c r="D28" s="59">
         <v>304</v>
       </c>
-      <c r="E28" s="60">
+      <c r="E28">
         <v>63</v>
       </c>
       <c r="F28" s="2">
@@ -2327,27 +2268,27 @@
       <c r="M28" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N28" s="69">
+      <c r="N28" s="59">
         <v>337</v>
       </c>
-      <c r="O28" s="60">
+      <c r="O28">
         <v>110</v>
       </c>
       <c r="P28" s="5"/>
       <c r="T28" s="4"/>
-      <c r="W28" s="75">
+      <c r="W28" s="64">
         <v>3414.35</v>
       </c>
-      <c r="X28" s="101">
+      <c r="X28" s="84">
         <v>151</v>
       </c>
       <c r="Y28" t="s">
         <v>32</v>
       </c>
-      <c r="Z28" s="61"/>
+      <c r="Z28" s="55"/>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A29" s="60">
+      <c r="A29">
         <v>1</v>
       </c>
       <c r="B29" s="25">
@@ -2356,10 +2297,10 @@
       <c r="C29" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="69">
+      <c r="D29" s="59">
         <v>305</v>
       </c>
-      <c r="E29" s="60">
+      <c r="E29">
         <v>64</v>
       </c>
       <c r="F29" s="5"/>
@@ -2370,10 +2311,10 @@
       <c r="M29" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N29" s="69">
+      <c r="N29" s="59">
         <v>338</v>
       </c>
-      <c r="O29" s="60">
+      <c r="O29">
         <v>111</v>
       </c>
       <c r="P29" s="5"/>
@@ -2388,7 +2329,7 @@
       <c r="Z29" s="49"/>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A30" s="60">
+      <c r="A30">
         <v>1</v>
       </c>
       <c r="B30" s="50">
@@ -2397,7 +2338,7 @@
       <c r="C30" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="70">
+      <c r="D30" s="60">
         <v>306</v>
       </c>
       <c r="E30" s="3">
@@ -2413,7 +2354,7 @@
       <c r="M30" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="N30" s="70">
+      <c r="N30" s="60">
         <v>339</v>
       </c>
       <c r="O30" s="3">
@@ -2437,7 +2378,7 @@
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A31" s="60">
+      <c r="A31">
         <v>1</v>
       </c>
       <c r="B31" s="25">
@@ -2446,10 +2387,10 @@
       <c r="C31" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="69">
+      <c r="D31" s="59">
         <v>307</v>
       </c>
-      <c r="E31" s="60">
+      <c r="E31">
         <v>66</v>
       </c>
       <c r="F31" s="2">
@@ -2462,10 +2403,10 @@
       <c r="M31" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N31" s="69">
+      <c r="N31" s="59">
         <v>340</v>
       </c>
-      <c r="O31" s="60">
+      <c r="O31">
         <v>113</v>
       </c>
       <c r="P31" s="2">
@@ -2482,35 +2423,35 @@
       <c r="Z31" s="49"/>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A32" s="60">
+      <c r="A32">
         <v>1</v>
       </c>
-      <c r="B32" s="88">
+      <c r="B32" s="74">
         <v>166</v>
       </c>
-      <c r="C32" s="88" t="s">
-        <v>25</v>
-      </c>
-      <c r="D32" s="89">
+      <c r="C32" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="75">
         <v>308</v>
       </c>
-      <c r="E32" s="86">
+      <c r="E32" s="73">
         <v>67</v>
       </c>
       <c r="F32" s="2">
         <v>50</v>
       </c>
       <c r="J32" s="4"/>
-      <c r="L32" s="88">
+      <c r="L32" s="74">
         <v>166</v>
       </c>
-      <c r="M32" s="88" t="s">
-        <v>25</v>
-      </c>
-      <c r="N32" s="89">
+      <c r="M32" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="N32" s="75">
         <v>341</v>
       </c>
-      <c r="O32" s="86">
+      <c r="O32" s="73">
         <v>114</v>
       </c>
       <c r="P32" s="2">
@@ -2527,7 +2468,7 @@
       <c r="Z32" s="49"/>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A33" s="60">
+      <c r="A33">
         <v>1</v>
       </c>
       <c r="B33" s="25">
@@ -2536,10 +2477,10 @@
       <c r="C33" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="69">
+      <c r="D33" s="59">
         <v>309</v>
       </c>
-      <c r="E33" s="60">
+      <c r="E33">
         <v>68</v>
       </c>
       <c r="F33" s="2">
@@ -2552,10 +2493,10 @@
       <c r="M33" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N33" s="69">
+      <c r="N33" s="59">
         <v>342</v>
       </c>
-      <c r="O33" s="60">
+      <c r="O33">
         <v>115</v>
       </c>
       <c r="P33" s="2">
@@ -2572,35 +2513,35 @@
       <c r="Z33" s="49"/>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A34" s="60">
+      <c r="A34">
         <v>1</v>
       </c>
-      <c r="B34" s="88">
+      <c r="B34" s="74">
         <v>168</v>
       </c>
-      <c r="C34" s="88" t="s">
-        <v>25</v>
-      </c>
-      <c r="D34" s="89">
+      <c r="C34" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="75">
         <v>310</v>
       </c>
-      <c r="E34" s="86">
+      <c r="E34" s="73">
         <v>69</v>
       </c>
       <c r="F34" s="2">
         <v>50</v>
       </c>
       <c r="J34" s="4"/>
-      <c r="L34" s="88">
+      <c r="L34" s="74">
         <v>168</v>
       </c>
-      <c r="M34" s="88" t="s">
-        <v>25</v>
-      </c>
-      <c r="N34" s="89">
+      <c r="M34" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="N34" s="75">
         <v>343</v>
       </c>
-      <c r="O34" s="86">
+      <c r="O34" s="73">
         <v>116</v>
       </c>
       <c r="P34" s="2">
@@ -2617,7 +2558,7 @@
       <c r="Z34" s="49"/>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A35" s="60">
+      <c r="A35">
         <v>1</v>
       </c>
       <c r="B35" s="25">
@@ -2626,10 +2567,10 @@
       <c r="C35" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="69">
+      <c r="D35" s="59">
         <v>311</v>
       </c>
-      <c r="E35" s="60">
+      <c r="E35">
         <v>70</v>
       </c>
       <c r="F35" s="2">
@@ -2642,10 +2583,10 @@
       <c r="M35" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N35" s="69">
+      <c r="N35" s="59">
         <v>344</v>
       </c>
-      <c r="O35" s="60">
+      <c r="O35">
         <v>117</v>
       </c>
       <c r="P35" s="5"/>
@@ -2658,7 +2599,7 @@
       <c r="Z35" s="49"/>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A36" s="60">
+      <c r="A36">
         <v>1</v>
       </c>
       <c r="B36" s="25">
@@ -2667,13 +2608,15 @@
       <c r="C36" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="69">
+      <c r="D36" s="59">
         <v>312</v>
       </c>
-      <c r="E36" s="60">
+      <c r="E36">
         <v>71</v>
       </c>
-      <c r="F36" s="5"/>
+      <c r="F36" s="2">
+        <v>58</v>
+      </c>
       <c r="J36" s="4"/>
       <c r="L36" s="25">
         <v>171</v>
@@ -2681,10 +2624,10 @@
       <c r="M36" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N36" s="69">
+      <c r="N36" s="59">
         <v>345</v>
       </c>
-      <c r="O36" s="60">
+      <c r="O36">
         <v>118</v>
       </c>
       <c r="P36" s="5"/>
@@ -2699,7 +2642,7 @@
       <c r="Z36" s="49"/>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A37" s="60">
+      <c r="A37">
         <v>1</v>
       </c>
       <c r="B37" s="25">
@@ -2708,13 +2651,15 @@
       <c r="C37" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D37" s="69">
+      <c r="D37" s="59">
         <v>313</v>
       </c>
-      <c r="E37" s="60">
+      <c r="E37">
         <v>72</v>
       </c>
-      <c r="F37" s="5"/>
+      <c r="F37" s="2">
+        <v>58</v>
+      </c>
       <c r="J37" s="4"/>
       <c r="L37" s="25">
         <v>172</v>
@@ -2722,10 +2667,10 @@
       <c r="M37" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N37" s="69">
+      <c r="N37" s="59">
         <v>346</v>
       </c>
-      <c r="O37" s="60">
+      <c r="O37">
         <v>119</v>
       </c>
       <c r="P37" s="5"/>
@@ -2740,7 +2685,7 @@
       <c r="Z37" s="49"/>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A38" s="60">
+      <c r="A38">
         <v>1</v>
       </c>
       <c r="B38" s="25">
@@ -2749,10 +2694,10 @@
       <c r="C38" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="69">
+      <c r="D38" s="59">
         <v>314</v>
       </c>
-      <c r="E38" s="60">
+      <c r="E38">
         <v>73</v>
       </c>
       <c r="F38" s="5"/>
@@ -2763,10 +2708,10 @@
       <c r="M38" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N38" s="69">
+      <c r="N38" s="59">
         <v>347</v>
       </c>
-      <c r="O38" s="60">
+      <c r="O38">
         <v>120</v>
       </c>
       <c r="P38" s="5"/>
@@ -2781,7 +2726,7 @@
       <c r="Z38" s="49"/>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A39" s="60">
+      <c r="A39">
         <v>1</v>
       </c>
       <c r="B39" s="25">
@@ -2790,10 +2735,10 @@
       <c r="C39" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D39" s="69">
+      <c r="D39" s="59">
         <v>315</v>
       </c>
-      <c r="E39" s="60">
+      <c r="E39">
         <v>74</v>
       </c>
       <c r="F39" s="5"/>
@@ -2804,10 +2749,10 @@
       <c r="M39" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N39" s="69">
+      <c r="N39" s="59">
         <v>348</v>
       </c>
-      <c r="O39" s="60">
+      <c r="O39">
         <v>121</v>
       </c>
       <c r="P39" s="5"/>
@@ -2822,7 +2767,7 @@
       <c r="Z39" s="49"/>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A40" s="60">
+      <c r="A40">
         <v>1</v>
       </c>
       <c r="B40" s="25">
@@ -2831,10 +2776,10 @@
       <c r="C40" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D40" s="69">
+      <c r="D40" s="59">
         <v>316</v>
       </c>
-      <c r="E40" s="60">
+      <c r="E40">
         <v>75</v>
       </c>
       <c r="F40" s="5"/>
@@ -2845,10 +2790,10 @@
       <c r="M40" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N40" s="69">
+      <c r="N40" s="59">
         <v>349</v>
       </c>
-      <c r="O40" s="60">
+      <c r="O40">
         <v>122</v>
       </c>
       <c r="P40" s="5"/>
@@ -2863,38 +2808,38 @@
       <c r="Z40" s="49"/>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A41" s="60">
+      <c r="A41">
         <v>1</v>
       </c>
-      <c r="B41" s="88">
+      <c r="B41" s="74">
         <v>188</v>
       </c>
-      <c r="C41" s="88" t="s">
-        <v>25</v>
-      </c>
-      <c r="D41" s="89">
+      <c r="C41" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" s="75">
         <v>317</v>
       </c>
-      <c r="E41" s="86">
+      <c r="E41" s="73">
         <v>76</v>
       </c>
       <c r="F41" s="2">
         <v>45</v>
       </c>
-      <c r="G41" s="64">
+      <c r="G41" s="3">
         <v>49</v>
       </c>
       <c r="J41" s="4"/>
-      <c r="L41" s="88">
+      <c r="L41" s="74">
         <v>188</v>
       </c>
-      <c r="M41" s="88" t="s">
-        <v>25</v>
-      </c>
-      <c r="N41" s="89">
+      <c r="M41" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="N41" s="75">
         <v>350</v>
       </c>
-      <c r="O41" s="86">
+      <c r="O41" s="73">
         <v>123</v>
       </c>
       <c r="P41" s="5"/>
@@ -2909,7 +2854,7 @@
       <c r="Z41" s="49"/>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A42" s="60">
+      <c r="A42">
         <v>1</v>
       </c>
       <c r="B42" s="25">
@@ -2918,16 +2863,16 @@
       <c r="C42" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="69">
+      <c r="D42" s="59">
         <v>318</v>
       </c>
-      <c r="E42" s="60">
+      <c r="E42">
         <v>77</v>
       </c>
       <c r="F42" s="2">
         <v>43</v>
       </c>
-      <c r="G42" s="64">
+      <c r="G42" s="3">
         <v>49</v>
       </c>
       <c r="J42" s="4"/>
@@ -2937,10 +2882,10 @@
       <c r="M42" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N42" s="69">
+      <c r="N42" s="59">
         <v>351</v>
       </c>
-      <c r="O42" s="60">
+      <c r="O42">
         <v>124</v>
       </c>
       <c r="P42" s="2">
@@ -2957,19 +2902,19 @@
       <c r="Z42" s="49"/>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A43" s="60">
+      <c r="A43">
         <v>1</v>
       </c>
-      <c r="B43" s="90">
+      <c r="B43" s="76">
         <v>194</v>
       </c>
-      <c r="C43" s="91" t="s">
-        <v>25</v>
-      </c>
-      <c r="D43" s="92">
+      <c r="C43" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" s="78">
         <v>319</v>
       </c>
-      <c r="E43" s="93">
+      <c r="E43" s="79">
         <v>78</v>
       </c>
       <c r="F43" s="2">
@@ -2978,20 +2923,20 @@
       <c r="G43" s="3">
         <v>43</v>
       </c>
-      <c r="H43" s="64">
+      <c r="H43" s="3">
         <v>49</v>
       </c>
       <c r="J43" s="4"/>
-      <c r="L43" s="90">
+      <c r="L43" s="76">
         <v>194</v>
       </c>
-      <c r="M43" s="91" t="s">
-        <v>25</v>
-      </c>
-      <c r="N43" s="92">
+      <c r="M43" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="N43" s="78">
         <v>352</v>
       </c>
-      <c r="O43" s="93">
+      <c r="O43" s="79">
         <v>125</v>
       </c>
       <c r="P43" s="2">
@@ -3011,7 +2956,7 @@
       <c r="Z43" s="49"/>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A44" s="60">
+      <c r="A44">
         <v>1</v>
       </c>
       <c r="B44" s="25">
@@ -3020,10 +2965,10 @@
       <c r="C44" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D44" s="69">
+      <c r="D44" s="59">
         <v>320</v>
       </c>
-      <c r="E44" s="60">
+      <c r="E44">
         <v>79</v>
       </c>
       <c r="F44" s="5"/>
@@ -3034,10 +2979,10 @@
       <c r="M44" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N44" s="69">
+      <c r="N44" s="59">
         <v>353</v>
       </c>
-      <c r="O44" s="60">
+      <c r="O44">
         <v>126</v>
       </c>
       <c r="P44" s="5"/>
@@ -3056,33 +3001,33 @@
       </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A45" s="60">
+      <c r="A45">
         <v>1</v>
       </c>
-      <c r="B45" s="88">
+      <c r="B45" s="74">
         <v>197</v>
       </c>
-      <c r="C45" s="88" t="s">
-        <v>25</v>
-      </c>
-      <c r="D45" s="89">
+      <c r="C45" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" s="75">
         <v>321</v>
       </c>
-      <c r="E45" s="86">
+      <c r="E45" s="73">
         <v>80</v>
       </c>
       <c r="F45" s="5"/>
       <c r="J45" s="4"/>
-      <c r="L45" s="88">
+      <c r="L45" s="74">
         <v>197</v>
       </c>
-      <c r="M45" s="88" t="s">
-        <v>25</v>
-      </c>
-      <c r="N45" s="89">
+      <c r="M45" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="N45" s="75">
         <v>354</v>
       </c>
-      <c r="O45" s="86">
+      <c r="O45" s="73">
         <v>127</v>
       </c>
       <c r="P45" s="5"/>
@@ -3097,7 +3042,7 @@
       <c r="Z45" s="4"/>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A46" s="60">
+      <c r="A46">
         <v>1</v>
       </c>
       <c r="B46" s="25">
@@ -3106,10 +3051,10 @@
       <c r="C46" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D46" s="69">
+      <c r="D46" s="59">
         <v>322</v>
       </c>
-      <c r="E46" s="60">
+      <c r="E46">
         <v>81</v>
       </c>
       <c r="F46" s="5"/>
@@ -3120,10 +3065,10 @@
       <c r="M46" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N46" s="69">
+      <c r="N46" s="59">
         <v>355</v>
       </c>
-      <c r="O46" s="60">
+      <c r="O46">
         <v>128</v>
       </c>
       <c r="P46" s="5"/>
@@ -3138,7 +3083,7 @@
       <c r="Z46" s="4"/>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A47" s="60">
+      <c r="A47">
         <v>1</v>
       </c>
       <c r="B47" s="25">
@@ -3147,10 +3092,10 @@
       <c r="C47" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D47" s="69">
+      <c r="D47" s="59">
         <v>323</v>
       </c>
-      <c r="E47" s="60">
+      <c r="E47">
         <v>82</v>
       </c>
       <c r="F47" s="5"/>
@@ -3161,10 +3106,10 @@
       <c r="M47" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N47" s="69">
+      <c r="N47" s="59">
         <v>356</v>
       </c>
-      <c r="O47" s="60">
+      <c r="O47">
         <v>129</v>
       </c>
       <c r="P47" s="5"/>
@@ -3177,7 +3122,7 @@
       <c r="Z47" s="4"/>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A48" s="60">
+      <c r="A48">
         <v>1</v>
       </c>
       <c r="B48" s="34">
@@ -3186,10 +3131,10 @@
       <c r="C48" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="D48" s="71">
+      <c r="D48" s="61">
         <v>324</v>
       </c>
-      <c r="E48" s="60">
+      <c r="E48">
         <v>83</v>
       </c>
       <c r="F48" s="6"/>
@@ -3203,10 +3148,10 @@
       <c r="M48" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="N48" s="71">
+      <c r="N48" s="61">
         <v>357</v>
       </c>
-      <c r="O48" s="60">
+      <c r="O48">
         <v>130</v>
       </c>
       <c r="P48" s="6"/>
@@ -3262,27 +3207,27 @@
       </c>
       <c r="C52" s="13"/>
       <c r="D52" s="9"/>
-      <c r="E52" s="58"/>
-      <c r="F52" s="104" t="s">
+      <c r="E52" s="9"/>
+      <c r="F52" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="G52" s="105"/>
-      <c r="H52" s="105"/>
-      <c r="I52" s="105"/>
-      <c r="J52" s="105"/>
+      <c r="G52" s="88"/>
+      <c r="H52" s="88"/>
+      <c r="I52" s="88"/>
+      <c r="J52" s="88"/>
       <c r="L52" s="9" t="s">
         <v>2</v>
       </c>
       <c r="M52" s="13"/>
       <c r="N52" s="9"/>
-      <c r="O52" s="58"/>
-      <c r="P52" s="104" t="s">
+      <c r="O52" s="9"/>
+      <c r="P52" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="Q52" s="105"/>
-      <c r="R52" s="105"/>
-      <c r="S52" s="105"/>
-      <c r="T52" s="105"/>
+      <c r="Q52" s="88"/>
+      <c r="R52" s="88"/>
+      <c r="S52" s="88"/>
+      <c r="T52" s="88"/>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B53" s="9" t="s">
@@ -3291,7 +3236,7 @@
       <c r="C53" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="D53" s="67" t="s">
+      <c r="D53" s="57" t="s">
         <v>21</v>
       </c>
       <c r="E53" s="13" t="s">
@@ -3318,7 +3263,7 @@
       <c r="M53" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="N53" s="67" t="s">
+      <c r="N53" s="57" t="s">
         <v>21</v>
       </c>
       <c r="O53" s="13" t="s">
@@ -3341,16 +3286,16 @@
       </c>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A54" s="60">
+      <c r="A54">
         <v>2</v>
       </c>
-      <c r="B54" s="65">
+      <c r="B54" s="5">
         <v>119</v>
       </c>
-      <c r="C54" s="66">
+      <c r="C54" s="42">
         <v>310</v>
       </c>
-      <c r="D54" s="68">
+      <c r="D54" s="58">
         <v>332</v>
       </c>
       <c r="E54">
@@ -3360,13 +3305,13 @@
         <v>4</v>
       </c>
       <c r="J54" s="4"/>
-      <c r="L54" s="65">
+      <c r="L54" s="5">
         <v>119</v>
       </c>
-      <c r="M54" s="66">
+      <c r="M54" s="42">
         <v>343</v>
       </c>
-      <c r="N54" s="72">
+      <c r="N54" s="62">
         <v>365</v>
       </c>
       <c r="O54">
@@ -3378,7 +3323,7 @@
       <c r="T54" s="4"/>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A55" s="60">
+      <c r="A55">
         <v>2</v>
       </c>
       <c r="B55" s="5">
@@ -3389,7 +3334,7 @@
         <f>C54+2</f>
         <v>312</v>
       </c>
-      <c r="D55" s="69">
+      <c r="D55" s="59">
         <v>333</v>
       </c>
       <c r="E55">
@@ -3397,15 +3342,15 @@
       </c>
       <c r="F55" s="5"/>
       <c r="J55" s="4"/>
-      <c r="L55" s="65">
+      <c r="L55" s="5">
         <f>L54+3</f>
         <v>122</v>
       </c>
-      <c r="M55" s="66">
+      <c r="M55" s="42">
         <f>M54+2</f>
         <v>345</v>
       </c>
-      <c r="N55" s="69">
+      <c r="N55" s="59">
         <v>366</v>
       </c>
       <c r="O55">
@@ -3415,7 +3360,7 @@
       <c r="T55" s="4"/>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A56" s="60">
+      <c r="A56">
         <v>2</v>
       </c>
       <c r="B56" s="29">
@@ -3426,7 +3371,7 @@
         <f t="shared" ref="C56:C82" si="1">C55+2</f>
         <v>314</v>
       </c>
-      <c r="D56" s="70">
+      <c r="D56" s="60">
         <v>334</v>
       </c>
       <c r="E56" s="3">
@@ -3450,7 +3395,7 @@
         <f t="shared" ref="M56:M82" si="3">M55+2</f>
         <v>347</v>
       </c>
-      <c r="N56" s="70">
+      <c r="N56" s="60">
         <v>367</v>
       </c>
       <c r="O56" s="3">
@@ -3467,44 +3412,44 @@
       <c r="T56" s="31"/>
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A57" s="60">
+      <c r="A57">
         <v>2</v>
       </c>
       <c r="B57" s="35">
         <f t="shared" si="0"/>
         <v>128</v>
       </c>
-      <c r="C57" s="88">
+      <c r="C57" s="74">
         <f t="shared" si="1"/>
         <v>316</v>
       </c>
-      <c r="D57" s="89">
+      <c r="D57" s="75">
         <v>335</v>
       </c>
-      <c r="E57" s="86">
+      <c r="E57" s="73">
         <v>90</v>
       </c>
       <c r="F57" s="5"/>
       <c r="J57" s="4"/>
-      <c r="L57" s="95">
+      <c r="L57" s="35">
         <f t="shared" si="2"/>
         <v>128</v>
       </c>
-      <c r="M57" s="96">
+      <c r="M57" s="74">
         <f t="shared" si="3"/>
         <v>349</v>
       </c>
-      <c r="N57" s="89">
+      <c r="N57" s="75">
         <v>368</v>
       </c>
-      <c r="O57" s="86">
+      <c r="O57" s="73">
         <v>137</v>
       </c>
       <c r="P57" s="5"/>
       <c r="T57" s="4"/>
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A58" s="60">
+      <c r="A58">
         <v>2</v>
       </c>
       <c r="B58" s="5">
@@ -3515,65 +3460,65 @@
         <f t="shared" si="1"/>
         <v>318</v>
       </c>
-      <c r="D58" s="69">
+      <c r="D58" s="59">
         <v>336</v>
       </c>
-      <c r="E58" s="60">
+      <c r="E58">
         <v>91</v>
       </c>
       <c r="F58" s="5"/>
       <c r="J58" s="4"/>
-      <c r="L58" s="65">
+      <c r="L58" s="5">
         <f t="shared" si="2"/>
         <v>131</v>
       </c>
-      <c r="M58" s="66">
+      <c r="M58" s="42">
         <f t="shared" si="3"/>
         <v>351</v>
       </c>
-      <c r="N58" s="69">
+      <c r="N58" s="59">
         <v>369</v>
       </c>
-      <c r="O58" s="60">
+      <c r="O58">
         <v>138</v>
       </c>
       <c r="P58" s="5"/>
       <c r="T58" s="4"/>
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A59" s="60">
+      <c r="A59">
         <v>2</v>
       </c>
-      <c r="B59" s="65">
+      <c r="B59" s="5">
         <f t="shared" si="0"/>
         <v>134</v>
       </c>
-      <c r="C59" s="66">
+      <c r="C59" s="42">
         <f t="shared" si="1"/>
         <v>320</v>
       </c>
-      <c r="D59" s="69">
+      <c r="D59" s="59">
         <v>337</v>
       </c>
-      <c r="E59" s="60">
+      <c r="E59">
         <v>92</v>
       </c>
       <c r="F59" s="2">
         <v>6</v>
       </c>
       <c r="J59" s="4"/>
-      <c r="L59" s="65">
+      <c r="L59" s="5">
         <f t="shared" si="2"/>
         <v>134</v>
       </c>
-      <c r="M59" s="66">
+      <c r="M59" s="42">
         <f t="shared" si="3"/>
         <v>353</v>
       </c>
-      <c r="N59" s="69">
+      <c r="N59" s="59">
         <v>370</v>
       </c>
-      <c r="O59" s="60">
+      <c r="O59">
         <v>139</v>
       </c>
       <c r="P59" s="2">
@@ -3582,7 +3527,7 @@
       <c r="T59" s="4"/>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A60" s="60">
+      <c r="A60">
         <v>2</v>
       </c>
       <c r="B60" s="5">
@@ -3593,10 +3538,10 @@
         <f t="shared" si="1"/>
         <v>322</v>
       </c>
-      <c r="D60" s="69">
+      <c r="D60" s="59">
         <v>338</v>
       </c>
-      <c r="E60" s="60">
+      <c r="E60">
         <v>93</v>
       </c>
       <c r="F60" s="5"/>
@@ -3609,31 +3554,31 @@
         <f t="shared" si="3"/>
         <v>355</v>
       </c>
-      <c r="N60" s="69">
+      <c r="N60" s="59">
         <v>371</v>
       </c>
-      <c r="O60" s="60">
+      <c r="O60">
         <v>140</v>
       </c>
       <c r="P60" s="5"/>
       <c r="T60" s="4"/>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A61" s="60">
+      <c r="A61">
         <v>2</v>
       </c>
-      <c r="B61" s="94">
+      <c r="B61" s="80">
         <f t="shared" si="0"/>
         <v>140</v>
       </c>
-      <c r="C61" s="91">
+      <c r="C61" s="77">
         <f t="shared" si="1"/>
         <v>324</v>
       </c>
-      <c r="D61" s="92">
+      <c r="D61" s="78">
         <v>339</v>
       </c>
-      <c r="E61" s="93">
+      <c r="E61" s="79">
         <v>94</v>
       </c>
       <c r="F61" s="29">
@@ -3646,18 +3591,18 @@
       <c r="I61" s="30"/>
       <c r="J61" s="31"/>
       <c r="K61" s="30"/>
-      <c r="L61" s="94">
+      <c r="L61" s="80">
         <f t="shared" si="2"/>
         <v>140</v>
       </c>
-      <c r="M61" s="91">
+      <c r="M61" s="77">
         <f t="shared" si="3"/>
         <v>357</v>
       </c>
-      <c r="N61" s="92">
+      <c r="N61" s="78">
         <v>372</v>
       </c>
-      <c r="O61" s="93">
+      <c r="O61" s="79">
         <v>141</v>
       </c>
       <c r="P61" s="29">
@@ -3671,7 +3616,7 @@
       <c r="T61" s="31"/>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A62" s="60">
+      <c r="A62">
         <v>2</v>
       </c>
       <c r="B62" s="5">
@@ -3682,10 +3627,10 @@
         <f t="shared" si="1"/>
         <v>326</v>
       </c>
-      <c r="D62" s="69">
+      <c r="D62" s="59">
         <v>340</v>
       </c>
-      <c r="E62" s="60">
+      <c r="E62">
         <v>95</v>
       </c>
       <c r="F62" s="5"/>
@@ -3698,31 +3643,31 @@
         <f t="shared" si="3"/>
         <v>359</v>
       </c>
-      <c r="N62" s="69">
+      <c r="N62" s="59">
         <v>373</v>
       </c>
-      <c r="O62" s="60">
+      <c r="O62">
         <v>142</v>
       </c>
       <c r="P62" s="5"/>
       <c r="T62" s="4"/>
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A63" s="60">
+      <c r="A63">
         <v>2</v>
       </c>
-      <c r="B63" s="94">
+      <c r="B63" s="80">
         <f t="shared" si="0"/>
         <v>146</v>
       </c>
-      <c r="C63" s="91">
+      <c r="C63" s="77">
         <f t="shared" si="1"/>
         <v>328</v>
       </c>
-      <c r="D63" s="92">
+      <c r="D63" s="78">
         <v>341</v>
       </c>
-      <c r="E63" s="93">
+      <c r="E63" s="79">
         <v>96</v>
       </c>
       <c r="F63" s="29">
@@ -3735,18 +3680,18 @@
       <c r="I63" s="30"/>
       <c r="J63" s="31"/>
       <c r="K63" s="30"/>
-      <c r="L63" s="94">
+      <c r="L63" s="80">
         <f t="shared" si="2"/>
         <v>146</v>
       </c>
-      <c r="M63" s="91">
+      <c r="M63" s="77">
         <f t="shared" si="3"/>
         <v>361</v>
       </c>
-      <c r="N63" s="92">
+      <c r="N63" s="78">
         <v>374</v>
       </c>
-      <c r="O63" s="93">
+      <c r="O63" s="79">
         <v>143</v>
       </c>
       <c r="P63" s="29">
@@ -3760,7 +3705,7 @@
       <c r="T63" s="31"/>
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A64" s="60">
+      <c r="A64">
         <v>2</v>
       </c>
       <c r="B64" s="5">
@@ -3771,10 +3716,10 @@
         <f t="shared" si="1"/>
         <v>330</v>
       </c>
-      <c r="D64" s="69">
+      <c r="D64" s="59">
         <v>342</v>
       </c>
-      <c r="E64" s="60">
+      <c r="E64">
         <v>97</v>
       </c>
       <c r="F64" s="5"/>
@@ -3787,17 +3732,17 @@
         <f t="shared" si="3"/>
         <v>363</v>
       </c>
-      <c r="N64" s="69">
+      <c r="N64" s="59">
         <v>375</v>
       </c>
-      <c r="O64" s="60">
+      <c r="O64">
         <v>144</v>
       </c>
       <c r="P64" s="5"/>
       <c r="T64" s="4"/>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A65" s="60">
+      <c r="A65">
         <v>2</v>
       </c>
       <c r="B65" s="5">
@@ -3808,10 +3753,10 @@
         <f t="shared" si="1"/>
         <v>332</v>
       </c>
-      <c r="D65" s="69">
+      <c r="D65" s="59">
         <v>343</v>
       </c>
-      <c r="E65" s="60">
+      <c r="E65">
         <v>98</v>
       </c>
       <c r="F65" s="35"/>
@@ -3824,17 +3769,17 @@
         <f t="shared" si="3"/>
         <v>365</v>
       </c>
-      <c r="N65" s="69">
+      <c r="N65" s="59">
         <v>376</v>
       </c>
-      <c r="O65" s="60">
+      <c r="O65">
         <v>145</v>
       </c>
       <c r="P65" s="35"/>
       <c r="T65" s="4"/>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A66" s="60">
+      <c r="A66">
         <v>2</v>
       </c>
       <c r="B66" s="5">
@@ -3845,10 +3790,10 @@
         <f t="shared" si="1"/>
         <v>334</v>
       </c>
-      <c r="D66" s="69">
+      <c r="D66" s="59">
         <v>344</v>
       </c>
-      <c r="E66" s="60">
+      <c r="E66">
         <v>99</v>
       </c>
       <c r="F66" s="5"/>
@@ -3861,17 +3806,17 @@
         <f t="shared" si="3"/>
         <v>367</v>
       </c>
-      <c r="N66" s="69">
+      <c r="N66" s="59">
         <v>377</v>
       </c>
-      <c r="O66" s="60">
+      <c r="O66">
         <v>146</v>
       </c>
       <c r="P66" s="5"/>
       <c r="T66" s="4"/>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A67" s="60">
+      <c r="A67">
         <v>2</v>
       </c>
       <c r="B67" s="5">
@@ -3882,10 +3827,10 @@
         <f t="shared" si="1"/>
         <v>336</v>
       </c>
-      <c r="D67" s="69">
+      <c r="D67" s="59">
         <v>345</v>
       </c>
-      <c r="E67" s="60">
+      <c r="E67">
         <v>100</v>
       </c>
       <c r="F67" s="5"/>
@@ -3898,17 +3843,17 @@
         <f t="shared" si="3"/>
         <v>369</v>
       </c>
-      <c r="N67" s="69">
+      <c r="N67" s="59">
         <v>378</v>
       </c>
-      <c r="O67" s="60">
+      <c r="O67">
         <v>147</v>
       </c>
       <c r="P67" s="5"/>
       <c r="T67" s="4"/>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A68" s="60">
+      <c r="A68">
         <v>2</v>
       </c>
       <c r="B68" s="29">
@@ -3919,7 +3864,7 @@
         <f t="shared" si="1"/>
         <v>338</v>
       </c>
-      <c r="D68" s="70">
+      <c r="D68" s="60">
         <v>346</v>
       </c>
       <c r="E68" s="3">
@@ -3943,7 +3888,7 @@
         <f t="shared" si="3"/>
         <v>371</v>
       </c>
-      <c r="N68" s="70">
+      <c r="N68" s="60">
         <v>379</v>
       </c>
       <c r="O68" s="3">
@@ -3960,21 +3905,21 @@
       <c r="T68" s="31"/>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A69" s="60">
+      <c r="A69">
         <v>2</v>
       </c>
-      <c r="B69" s="95">
+      <c r="B69" s="35">
         <f t="shared" si="0"/>
         <v>164</v>
       </c>
-      <c r="C69" s="96">
+      <c r="C69" s="74">
         <f t="shared" si="1"/>
         <v>340</v>
       </c>
-      <c r="D69" s="89">
+      <c r="D69" s="75">
         <v>347</v>
       </c>
-      <c r="E69" s="86">
+      <c r="E69" s="73">
         <v>102</v>
       </c>
       <c r="F69" s="2">
@@ -3984,18 +3929,18 @@
         <v>7</v>
       </c>
       <c r="J69" s="4"/>
-      <c r="L69" s="95">
+      <c r="L69" s="35">
         <f t="shared" si="2"/>
         <v>164</v>
       </c>
-      <c r="M69" s="96">
+      <c r="M69" s="74">
         <f t="shared" si="3"/>
         <v>373</v>
       </c>
-      <c r="N69" s="89">
+      <c r="N69" s="75">
         <v>380</v>
       </c>
-      <c r="O69" s="86">
+      <c r="O69" s="73">
         <v>149</v>
       </c>
       <c r="P69" s="2">
@@ -4007,39 +3952,39 @@
       <c r="T69" s="4"/>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A70" s="60">
+      <c r="A70">
         <v>2</v>
       </c>
-      <c r="B70" s="95">
+      <c r="B70" s="35">
         <f t="shared" si="0"/>
         <v>167</v>
       </c>
-      <c r="C70" s="96">
+      <c r="C70" s="74">
         <f t="shared" si="1"/>
         <v>342</v>
       </c>
-      <c r="D70" s="89">
+      <c r="D70" s="75">
         <v>348</v>
       </c>
-      <c r="E70" s="86">
+      <c r="E70" s="73">
         <v>103</v>
       </c>
       <c r="F70" s="2">
         <v>4</v>
       </c>
       <c r="J70" s="4"/>
-      <c r="L70" s="95">
+      <c r="L70" s="35">
         <f t="shared" si="2"/>
         <v>167</v>
       </c>
-      <c r="M70" s="96">
+      <c r="M70" s="74">
         <f t="shared" si="3"/>
         <v>375</v>
       </c>
-      <c r="N70" s="89">
+      <c r="N70" s="75">
         <v>381</v>
       </c>
-      <c r="O70" s="86">
+      <c r="O70" s="73">
         <v>150</v>
       </c>
       <c r="P70" s="2">
@@ -4048,224 +3993,224 @@
       <c r="T70" s="4"/>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A71" s="60">
+      <c r="A71">
         <v>2</v>
       </c>
-      <c r="B71" s="65">
+      <c r="B71" s="5">
         <f t="shared" si="0"/>
         <v>170</v>
       </c>
-      <c r="C71" s="66">
+      <c r="C71" s="42">
         <f t="shared" si="1"/>
         <v>344</v>
       </c>
-      <c r="D71" s="69">
+      <c r="D71" s="59">
         <v>349</v>
       </c>
-      <c r="E71" s="60">
+      <c r="E71">
         <v>104</v>
       </c>
       <c r="F71" s="5"/>
       <c r="J71" s="4"/>
-      <c r="L71" s="65">
+      <c r="L71" s="5">
         <f t="shared" si="2"/>
         <v>170</v>
       </c>
-      <c r="M71" s="66">
+      <c r="M71" s="42">
         <f t="shared" si="3"/>
         <v>377</v>
       </c>
-      <c r="N71" s="69">
+      <c r="N71" s="59">
         <v>382</v>
       </c>
-      <c r="O71" s="60">
+      <c r="O71">
         <v>151</v>
       </c>
       <c r="P71" s="5"/>
       <c r="T71" s="4"/>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A72" s="60">
+      <c r="A72">
         <v>2</v>
       </c>
-      <c r="B72" s="65">
+      <c r="B72" s="5">
         <f t="shared" si="0"/>
         <v>173</v>
       </c>
-      <c r="C72" s="66">
+      <c r="C72" s="42">
         <f t="shared" si="1"/>
         <v>346</v>
       </c>
-      <c r="D72" s="69">
+      <c r="D72" s="59">
         <v>350</v>
       </c>
-      <c r="E72" s="60">
+      <c r="E72">
         <v>105</v>
       </c>
       <c r="F72" s="5"/>
       <c r="J72" s="4"/>
-      <c r="L72" s="65">
+      <c r="L72" s="5">
         <f t="shared" si="2"/>
         <v>173</v>
       </c>
-      <c r="M72" s="66">
+      <c r="M72" s="42">
         <f t="shared" si="3"/>
         <v>379</v>
       </c>
-      <c r="N72" s="69">
+      <c r="N72" s="59">
         <v>383</v>
       </c>
-      <c r="O72" s="60">
+      <c r="O72">
         <v>152</v>
       </c>
       <c r="P72" s="5"/>
       <c r="T72" s="4"/>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A73" s="60">
+      <c r="A73">
         <v>2</v>
       </c>
-      <c r="B73" s="65">
+      <c r="B73" s="5">
         <f t="shared" si="0"/>
         <v>176</v>
       </c>
-      <c r="C73" s="66">
+      <c r="C73" s="42">
         <f t="shared" si="1"/>
         <v>348</v>
       </c>
-      <c r="D73" s="69">
+      <c r="D73" s="59">
         <v>351</v>
       </c>
-      <c r="E73" s="60">
+      <c r="E73">
         <v>106</v>
       </c>
       <c r="F73" s="5"/>
       <c r="J73" s="4"/>
-      <c r="L73" s="65">
+      <c r="L73" s="5">
         <f t="shared" si="2"/>
         <v>176</v>
       </c>
-      <c r="M73" s="66">
+      <c r="M73" s="42">
         <f t="shared" si="3"/>
         <v>381</v>
       </c>
-      <c r="N73" s="69">
+      <c r="N73" s="59">
         <v>384</v>
       </c>
-      <c r="O73" s="60">
+      <c r="O73">
         <v>153</v>
       </c>
       <c r="P73" s="5"/>
       <c r="T73" s="4"/>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A74" s="60">
+      <c r="A74">
         <v>2</v>
       </c>
-      <c r="B74" s="65">
+      <c r="B74" s="5">
         <f t="shared" si="0"/>
         <v>179</v>
       </c>
-      <c r="C74" s="66">
+      <c r="C74" s="42">
         <f t="shared" si="1"/>
         <v>350</v>
       </c>
-      <c r="D74" s="69">
+      <c r="D74" s="59">
         <v>352</v>
       </c>
-      <c r="E74" s="60">
+      <c r="E74">
         <v>107</v>
       </c>
       <c r="F74" s="5"/>
       <c r="J74" s="4"/>
-      <c r="L74" s="65">
+      <c r="L74" s="5">
         <f t="shared" si="2"/>
         <v>179</v>
       </c>
-      <c r="M74" s="66">
+      <c r="M74" s="42">
         <f t="shared" si="3"/>
         <v>383</v>
       </c>
-      <c r="N74" s="69">
+      <c r="N74" s="59">
         <v>385</v>
       </c>
-      <c r="O74" s="60">
+      <c r="O74">
         <v>154</v>
       </c>
       <c r="P74" s="5"/>
       <c r="T74" s="4"/>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A75" s="60">
+      <c r="A75">
         <v>2</v>
       </c>
-      <c r="B75" s="65">
+      <c r="B75" s="5">
         <f t="shared" si="0"/>
         <v>182</v>
       </c>
-      <c r="C75" s="66">
+      <c r="C75" s="42">
         <f t="shared" si="1"/>
         <v>352</v>
       </c>
-      <c r="D75" s="69">
+      <c r="D75" s="59">
         <v>353</v>
       </c>
-      <c r="E75" s="60">
+      <c r="E75">
         <v>108</v>
       </c>
       <c r="F75" s="5"/>
       <c r="J75" s="4"/>
-      <c r="L75" s="65">
+      <c r="L75" s="5">
         <f t="shared" si="2"/>
         <v>182</v>
       </c>
-      <c r="M75" s="66">
+      <c r="M75" s="42">
         <f t="shared" si="3"/>
         <v>385</v>
       </c>
-      <c r="N75" s="69">
+      <c r="N75" s="59">
         <v>386</v>
       </c>
-      <c r="O75" s="60">
+      <c r="O75">
         <v>155</v>
       </c>
       <c r="P75" s="5"/>
       <c r="T75" s="4"/>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A76" s="60">
+      <c r="A76">
         <v>2</v>
       </c>
-      <c r="B76" s="65">
+      <c r="B76" s="5">
         <f t="shared" si="0"/>
         <v>185</v>
       </c>
-      <c r="C76" s="66">
+      <c r="C76" s="42">
         <f t="shared" si="1"/>
         <v>354</v>
       </c>
-      <c r="D76" s="69">
+      <c r="D76" s="59">
         <v>354</v>
       </c>
-      <c r="E76" s="60">
+      <c r="E76">
         <v>109</v>
       </c>
       <c r="F76" s="2">
         <v>6</v>
       </c>
       <c r="J76" s="4"/>
-      <c r="L76" s="65">
+      <c r="L76" s="5">
         <f t="shared" si="2"/>
         <v>185</v>
       </c>
-      <c r="M76" s="66">
+      <c r="M76" s="42">
         <f t="shared" si="3"/>
         <v>387</v>
       </c>
-      <c r="N76" s="69">
+      <c r="N76" s="59">
         <v>387</v>
       </c>
-      <c r="O76" s="60">
+      <c r="O76">
         <v>156</v>
       </c>
       <c r="P76" s="2">
@@ -4274,21 +4219,21 @@
       <c r="T76" s="4"/>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A77" s="60">
+      <c r="A77">
         <v>2</v>
       </c>
-      <c r="B77" s="95">
+      <c r="B77" s="35">
         <f t="shared" si="0"/>
         <v>188</v>
       </c>
-      <c r="C77" s="96">
+      <c r="C77" s="74">
         <f t="shared" si="1"/>
         <v>356</v>
       </c>
-      <c r="D77" s="89">
+      <c r="D77" s="75">
         <v>355</v>
       </c>
-      <c r="E77" s="86">
+      <c r="E77" s="73">
         <v>110</v>
       </c>
       <c r="F77" s="2">
@@ -4298,18 +4243,18 @@
         <v>45</v>
       </c>
       <c r="J77" s="4"/>
-      <c r="L77" s="95">
+      <c r="L77" s="35">
         <f t="shared" si="2"/>
         <v>188</v>
       </c>
-      <c r="M77" s="96">
+      <c r="M77" s="74">
         <f t="shared" si="3"/>
         <v>389</v>
       </c>
-      <c r="N77" s="89">
+      <c r="N77" s="75">
         <v>388</v>
       </c>
-      <c r="O77" s="86">
+      <c r="O77" s="73">
         <v>157</v>
       </c>
       <c r="P77" s="2">
@@ -4318,7 +4263,7 @@
       <c r="T77" s="4"/>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A78" s="60">
+      <c r="A78">
         <v>2</v>
       </c>
       <c r="B78" s="5">
@@ -4329,10 +4274,10 @@
         <f t="shared" si="1"/>
         <v>358</v>
       </c>
-      <c r="D78" s="69">
+      <c r="D78" s="59">
         <v>356</v>
       </c>
-      <c r="E78" s="60">
+      <c r="E78">
         <v>111</v>
       </c>
       <c r="F78" s="5"/>
@@ -4345,31 +4290,31 @@
         <f t="shared" si="3"/>
         <v>391</v>
       </c>
-      <c r="N78" s="69">
+      <c r="N78" s="59">
         <v>389</v>
       </c>
-      <c r="O78" s="60">
+      <c r="O78">
         <v>158</v>
       </c>
       <c r="P78" s="5"/>
       <c r="T78" s="4"/>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A79" s="60">
+      <c r="A79">
         <v>2</v>
       </c>
-      <c r="B79" s="94">
+      <c r="B79" s="80">
         <f t="shared" si="0"/>
         <v>194</v>
       </c>
-      <c r="C79" s="91">
+      <c r="C79" s="77">
         <f t="shared" si="1"/>
         <v>360</v>
       </c>
-      <c r="D79" s="92">
+      <c r="D79" s="78">
         <v>357</v>
       </c>
-      <c r="E79" s="93">
+      <c r="E79" s="79">
         <v>112</v>
       </c>
       <c r="F79" s="29">
@@ -4380,18 +4325,18 @@
       <c r="I79" s="30"/>
       <c r="J79" s="31"/>
       <c r="K79" s="30"/>
-      <c r="L79" s="94">
+      <c r="L79" s="80">
         <f t="shared" si="2"/>
         <v>194</v>
       </c>
-      <c r="M79" s="91">
+      <c r="M79" s="77">
         <f t="shared" si="3"/>
         <v>393</v>
       </c>
-      <c r="N79" s="92">
+      <c r="N79" s="78">
         <v>390</v>
       </c>
-      <c r="O79" s="93">
+      <c r="O79" s="79">
         <v>159</v>
       </c>
       <c r="P79" s="29">
@@ -4403,21 +4348,21 @@
       <c r="T79" s="31"/>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A80" s="60">
+      <c r="A80">
         <v>2</v>
       </c>
       <c r="B80" s="35">
         <f t="shared" si="0"/>
         <v>197</v>
       </c>
-      <c r="C80" s="88">
+      <c r="C80" s="74">
         <f t="shared" si="1"/>
         <v>362</v>
       </c>
-      <c r="D80" s="89">
+      <c r="D80" s="75">
         <v>358</v>
       </c>
-      <c r="E80" s="86">
+      <c r="E80" s="73">
         <v>113</v>
       </c>
       <c r="F80" s="5"/>
@@ -4426,21 +4371,21 @@
         <f t="shared" si="2"/>
         <v>197</v>
       </c>
-      <c r="M80" s="88">
+      <c r="M80" s="74">
         <f t="shared" si="3"/>
         <v>395</v>
       </c>
-      <c r="N80" s="89">
+      <c r="N80" s="75">
         <v>391</v>
       </c>
-      <c r="O80" s="86">
+      <c r="O80" s="73">
         <v>160</v>
       </c>
       <c r="P80" s="5"/>
       <c r="T80" s="4"/>
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A81" s="60">
+      <c r="A81">
         <v>2</v>
       </c>
       <c r="B81" s="5">
@@ -4451,10 +4396,10 @@
         <f t="shared" si="1"/>
         <v>364</v>
       </c>
-      <c r="D81" s="69">
+      <c r="D81" s="59">
         <v>359</v>
       </c>
-      <c r="E81" s="60">
+      <c r="E81">
         <v>114</v>
       </c>
       <c r="F81" s="5"/>
@@ -4467,17 +4412,17 @@
         <f t="shared" si="3"/>
         <v>397</v>
       </c>
-      <c r="N81" s="69">
+      <c r="N81" s="59">
         <v>392</v>
       </c>
-      <c r="O81" s="60">
+      <c r="O81">
         <v>161</v>
       </c>
       <c r="P81" s="5"/>
       <c r="T81" s="4"/>
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A82" s="60">
+      <c r="A82">
         <v>2</v>
       </c>
       <c r="B82" s="6">
@@ -4488,10 +4433,10 @@
         <f t="shared" si="1"/>
         <v>366</v>
       </c>
-      <c r="D82" s="71">
+      <c r="D82" s="61">
         <v>360</v>
       </c>
-      <c r="E82" s="60">
+      <c r="E82">
         <v>115</v>
       </c>
       <c r="F82" s="6"/>
@@ -4507,10 +4452,10 @@
         <f t="shared" si="3"/>
         <v>399</v>
       </c>
-      <c r="N82" s="71">
+      <c r="N82" s="61">
         <v>393</v>
       </c>
-      <c r="O82" s="60">
+      <c r="O82">
         <v>162</v>
       </c>
       <c r="P82" s="6"/>
@@ -4548,26 +4493,26 @@
       <c r="C86" s="13"/>
       <c r="D86" s="9"/>
       <c r="E86" s="33"/>
-      <c r="F86" s="104" t="s">
+      <c r="F86" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="G86" s="105"/>
-      <c r="H86" s="105"/>
-      <c r="I86" s="105"/>
-      <c r="J86" s="105"/>
+      <c r="G86" s="88"/>
+      <c r="H86" s="88"/>
+      <c r="I86" s="88"/>
+      <c r="J86" s="88"/>
       <c r="L86" s="9" t="s">
         <v>2</v>
       </c>
       <c r="M86" s="13"/>
       <c r="N86" s="9"/>
       <c r="O86" s="33"/>
-      <c r="P86" s="104" t="s">
+      <c r="P86" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="Q86" s="105"/>
-      <c r="R86" s="105"/>
-      <c r="S86" s="105"/>
-      <c r="T86" s="105"/>
+      <c r="Q86" s="88"/>
+      <c r="R86" s="88"/>
+      <c r="S86" s="88"/>
+      <c r="T86" s="88"/>
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B87" s="9" t="s">
@@ -4576,7 +4521,7 @@
       <c r="C87" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="D87" s="67" t="s">
+      <c r="D87" s="57" t="s">
         <v>21</v>
       </c>
       <c r="E87" s="13" t="s">
@@ -4603,7 +4548,7 @@
       <c r="M87" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="N87" s="67" t="s">
+      <c r="N87" s="57" t="s">
         <v>21</v>
       </c>
       <c r="O87" s="13" t="s">
@@ -4626,7 +4571,7 @@
       </c>
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A88" s="60">
+      <c r="A88">
         <v>4</v>
       </c>
       <c r="B88" s="5">
@@ -4635,7 +4580,7 @@
       <c r="C88" s="44">
         <v>386</v>
       </c>
-      <c r="D88" s="68">
+      <c r="D88" s="58">
         <v>370</v>
       </c>
       <c r="E88">
@@ -4649,17 +4594,17 @@
       <c r="M88" s="42">
         <v>419</v>
       </c>
-      <c r="N88" s="73">
+      <c r="N88" s="58">
         <v>403</v>
       </c>
-      <c r="O88" s="59">
+      <c r="O88">
         <v>236</v>
       </c>
       <c r="P88" s="5"/>
       <c r="T88" s="4"/>
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A89" s="60">
+      <c r="A89">
         <v>4</v>
       </c>
       <c r="B89" s="5">
@@ -4670,7 +4615,7 @@
         <f>C88+2</f>
         <v>388</v>
       </c>
-      <c r="D89" s="69">
+      <c r="D89" s="59">
         <v>371</v>
       </c>
       <c r="E89">
@@ -4688,10 +4633,10 @@
         <f t="shared" ref="M89:M116" si="4">M88+2</f>
         <v>421</v>
       </c>
-      <c r="N89" s="69">
+      <c r="N89" s="59">
         <v>404</v>
       </c>
-      <c r="O89" s="59">
+      <c r="O89">
         <v>237</v>
       </c>
       <c r="P89" s="2">
@@ -4700,7 +4645,7 @@
       <c r="T89" s="4"/>
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A90" s="60">
+      <c r="A90">
         <v>4</v>
       </c>
       <c r="B90" s="29">
@@ -4711,7 +4656,7 @@
         <f t="shared" ref="C90:C116" si="6">C89+2</f>
         <v>390</v>
       </c>
-      <c r="D90" s="70">
+      <c r="D90" s="60">
         <v>372</v>
       </c>
       <c r="E90" s="3">
@@ -4735,10 +4680,10 @@
         <f t="shared" si="4"/>
         <v>423</v>
       </c>
-      <c r="N90" s="70">
+      <c r="N90" s="60">
         <v>405</v>
       </c>
-      <c r="O90" s="64">
+      <c r="O90" s="3">
         <v>238</v>
       </c>
       <c r="P90" s="29">
@@ -4750,21 +4695,21 @@
       <c r="T90" s="31"/>
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A91" s="60">
+      <c r="A91">
         <v>4</v>
       </c>
       <c r="B91" s="35">
         <f t="shared" si="5"/>
         <v>128</v>
       </c>
-      <c r="C91" s="88">
+      <c r="C91" s="74">
         <f t="shared" si="6"/>
         <v>392</v>
       </c>
-      <c r="D91" s="89">
+      <c r="D91" s="75">
         <v>373</v>
       </c>
-      <c r="E91" s="86">
+      <c r="E91" s="73">
         <v>192</v>
       </c>
       <c r="F91" s="2">
@@ -4775,21 +4720,21 @@
         <f t="shared" si="7"/>
         <v>128</v>
       </c>
-      <c r="M91" s="88">
+      <c r="M91" s="74">
         <f t="shared" si="4"/>
         <v>425</v>
       </c>
-      <c r="N91" s="89">
+      <c r="N91" s="75">
         <v>406</v>
       </c>
-      <c r="O91" s="87">
+      <c r="O91" s="73">
         <v>239</v>
       </c>
       <c r="P91" s="5"/>
       <c r="T91" s="4"/>
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A92" s="60">
+      <c r="A92">
         <v>4</v>
       </c>
       <c r="B92" s="5">
@@ -4800,10 +4745,10 @@
         <f t="shared" si="6"/>
         <v>394</v>
       </c>
-      <c r="D92" s="69">
+      <c r="D92" s="59">
         <v>374</v>
       </c>
-      <c r="E92" s="60">
+      <c r="E92">
         <v>193</v>
       </c>
       <c r="F92" s="5"/>
@@ -4816,17 +4761,17 @@
         <f t="shared" si="4"/>
         <v>427</v>
       </c>
-      <c r="N92" s="69">
+      <c r="N92" s="59">
         <v>407</v>
       </c>
-      <c r="O92" s="59">
+      <c r="O92">
         <v>240</v>
       </c>
       <c r="P92" s="5"/>
       <c r="T92" s="4"/>
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A93" s="60">
+      <c r="A93">
         <v>4</v>
       </c>
       <c r="B93" s="5">
@@ -4837,10 +4782,10 @@
         <f t="shared" si="6"/>
         <v>396</v>
       </c>
-      <c r="D93" s="69">
+      <c r="D93" s="59">
         <v>375</v>
       </c>
-      <c r="E93" s="60">
+      <c r="E93">
         <v>194</v>
       </c>
       <c r="F93" s="5"/>
@@ -4853,17 +4798,17 @@
         <f t="shared" si="4"/>
         <v>429</v>
       </c>
-      <c r="N93" s="69">
+      <c r="N93" s="59">
         <v>408</v>
       </c>
-      <c r="O93" s="59">
+      <c r="O93">
         <v>241</v>
       </c>
       <c r="P93" s="5"/>
       <c r="T93" s="4"/>
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A94" s="60">
+      <c r="A94">
         <v>4</v>
       </c>
       <c r="B94" s="5">
@@ -4874,10 +4819,10 @@
         <f t="shared" si="6"/>
         <v>398</v>
       </c>
-      <c r="D94" s="69">
+      <c r="D94" s="59">
         <v>376</v>
       </c>
-      <c r="E94" s="60">
+      <c r="E94">
         <v>195</v>
       </c>
       <c r="F94" s="2">
@@ -4892,10 +4837,10 @@
         <f t="shared" si="4"/>
         <v>431</v>
       </c>
-      <c r="N94" s="69">
+      <c r="N94" s="59">
         <v>409</v>
       </c>
-      <c r="O94" s="59">
+      <c r="O94">
         <v>242</v>
       </c>
       <c r="P94" s="2">
@@ -4904,21 +4849,21 @@
       <c r="T94" s="4"/>
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A95" s="60">
+      <c r="A95">
         <v>4</v>
       </c>
-      <c r="B95" s="94">
+      <c r="B95" s="80">
         <f t="shared" si="5"/>
         <v>140</v>
       </c>
-      <c r="C95" s="91">
+      <c r="C95" s="77">
         <f t="shared" si="6"/>
         <v>400</v>
       </c>
-      <c r="D95" s="92">
+      <c r="D95" s="78">
         <v>377</v>
       </c>
-      <c r="E95" s="93">
+      <c r="E95" s="79">
         <v>196</v>
       </c>
       <c r="F95" s="29">
@@ -4931,18 +4876,18 @@
       <c r="I95" s="30"/>
       <c r="J95" s="31"/>
       <c r="K95" s="30"/>
-      <c r="L95" s="94">
+      <c r="L95" s="80">
         <f t="shared" si="7"/>
         <v>140</v>
       </c>
-      <c r="M95" s="91">
+      <c r="M95" s="77">
         <f t="shared" si="4"/>
         <v>433</v>
       </c>
-      <c r="N95" s="92">
+      <c r="N95" s="78">
         <v>410</v>
       </c>
-      <c r="O95" s="98">
+      <c r="O95" s="79">
         <v>243</v>
       </c>
       <c r="P95" s="29">
@@ -4956,7 +4901,7 @@
       <c r="T95" s="31"/>
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A96" s="60">
+      <c r="A96">
         <v>4</v>
       </c>
       <c r="B96" s="5">
@@ -4967,10 +4912,10 @@
         <f t="shared" si="6"/>
         <v>402</v>
       </c>
-      <c r="D96" s="69">
+      <c r="D96" s="59">
         <v>378</v>
       </c>
-      <c r="E96" s="60">
+      <c r="E96">
         <v>197</v>
       </c>
       <c r="F96" s="5"/>
@@ -4983,10 +4928,10 @@
         <f t="shared" si="4"/>
         <v>435</v>
       </c>
-      <c r="N96" s="69">
+      <c r="N96" s="59">
         <v>411</v>
       </c>
-      <c r="O96" s="59">
+      <c r="O96">
         <v>244</v>
       </c>
       <c r="P96" s="2">
@@ -4995,21 +4940,21 @@
       <c r="T96" s="4"/>
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A97" s="60">
+      <c r="A97">
         <v>4</v>
       </c>
-      <c r="B97" s="94">
+      <c r="B97" s="80">
         <f t="shared" si="5"/>
         <v>146</v>
       </c>
-      <c r="C97" s="91">
+      <c r="C97" s="77">
         <f t="shared" si="6"/>
         <v>404</v>
       </c>
-      <c r="D97" s="92">
+      <c r="D97" s="78">
         <v>379</v>
       </c>
-      <c r="E97" s="93">
+      <c r="E97" s="79">
         <v>198</v>
       </c>
       <c r="F97" s="29">
@@ -5022,18 +4967,18 @@
       <c r="I97" s="30"/>
       <c r="J97" s="31"/>
       <c r="K97" s="30"/>
-      <c r="L97" s="94">
+      <c r="L97" s="80">
         <f t="shared" si="7"/>
         <v>146</v>
       </c>
-      <c r="M97" s="91">
+      <c r="M97" s="77">
         <f t="shared" si="4"/>
         <v>437</v>
       </c>
-      <c r="N97" s="92">
+      <c r="N97" s="78">
         <v>412</v>
       </c>
-      <c r="O97" s="98">
+      <c r="O97" s="79">
         <v>245</v>
       </c>
       <c r="P97" s="29">
@@ -5045,7 +4990,7 @@
       <c r="T97" s="31"/>
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A98" s="60">
+      <c r="A98">
         <v>4</v>
       </c>
       <c r="B98" s="29">
@@ -5056,7 +5001,7 @@
         <f t="shared" si="6"/>
         <v>406</v>
       </c>
-      <c r="D98" s="70">
+      <c r="D98" s="60">
         <v>380</v>
       </c>
       <c r="E98" s="3">
@@ -5077,10 +5022,10 @@
         <f t="shared" si="4"/>
         <v>439</v>
       </c>
-      <c r="N98" s="70">
+      <c r="N98" s="60">
         <v>413</v>
       </c>
-      <c r="O98" s="64">
+      <c r="O98" s="3">
         <v>246</v>
       </c>
       <c r="P98" s="28"/>
@@ -5090,7 +5035,7 @@
       <c r="T98" s="31"/>
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A99" s="60">
+      <c r="A99">
         <v>4</v>
       </c>
       <c r="B99" s="5">
@@ -5101,13 +5046,13 @@
         <f t="shared" si="6"/>
         <v>408</v>
       </c>
-      <c r="D99" s="69">
+      <c r="D99" s="59">
         <v>381</v>
       </c>
-      <c r="E99" s="60">
+      <c r="E99">
         <v>200</v>
       </c>
-      <c r="F99" s="75"/>
+      <c r="F99" s="64"/>
       <c r="J99" s="4"/>
       <c r="L99" s="5">
         <f t="shared" si="7"/>
@@ -5117,17 +5062,17 @@
         <f t="shared" si="4"/>
         <v>441</v>
       </c>
-      <c r="N99" s="69">
+      <c r="N99" s="59">
         <v>414</v>
       </c>
-      <c r="O99" s="59">
+      <c r="O99">
         <v>247</v>
       </c>
       <c r="P99" s="35"/>
       <c r="T99" s="4"/>
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A100" s="60">
+      <c r="A100">
         <v>4</v>
       </c>
       <c r="B100" s="5">
@@ -5138,10 +5083,10 @@
         <f t="shared" si="6"/>
         <v>410</v>
       </c>
-      <c r="D100" s="69">
+      <c r="D100" s="59">
         <v>382</v>
       </c>
-      <c r="E100" s="60">
+      <c r="E100">
         <v>201</v>
       </c>
       <c r="F100" s="5"/>
@@ -5154,17 +5099,17 @@
         <f t="shared" si="4"/>
         <v>443</v>
       </c>
-      <c r="N100" s="69">
+      <c r="N100" s="59">
         <v>415</v>
       </c>
-      <c r="O100" s="59">
+      <c r="O100">
         <v>248</v>
       </c>
       <c r="P100" s="5"/>
       <c r="T100" s="4"/>
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A101" s="60">
+      <c r="A101">
         <v>4</v>
       </c>
       <c r="B101" s="5">
@@ -5175,10 +5120,10 @@
         <f t="shared" si="6"/>
         <v>412</v>
       </c>
-      <c r="D101" s="69">
+      <c r="D101" s="59">
         <v>383</v>
       </c>
-      <c r="E101" s="60">
+      <c r="E101">
         <v>202</v>
       </c>
       <c r="F101" s="2">
@@ -5193,10 +5138,10 @@
         <f t="shared" si="4"/>
         <v>445</v>
       </c>
-      <c r="N101" s="69">
+      <c r="N101" s="59">
         <v>416</v>
       </c>
-      <c r="O101" s="59">
+      <c r="O101">
         <v>249</v>
       </c>
       <c r="P101" s="2">
@@ -5205,7 +5150,7 @@
       <c r="T101" s="4"/>
     </row>
     <row r="102" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A102" s="60">
+      <c r="A102">
         <v>4</v>
       </c>
       <c r="B102" s="29">
@@ -5216,7 +5161,7 @@
         <f t="shared" si="6"/>
         <v>414</v>
       </c>
-      <c r="D102" s="70">
+      <c r="D102" s="60">
         <v>384</v>
       </c>
       <c r="E102" s="3">
@@ -5240,10 +5185,10 @@
         <f t="shared" si="4"/>
         <v>447</v>
       </c>
-      <c r="N102" s="70">
+      <c r="N102" s="60">
         <v>417</v>
       </c>
-      <c r="O102" s="64">
+      <c r="O102" s="3">
         <v>250</v>
       </c>
       <c r="P102" s="29">
@@ -5255,21 +5200,21 @@
       <c r="T102" s="31"/>
     </row>
     <row r="103" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A103" s="60">
+      <c r="A103">
         <v>4</v>
       </c>
       <c r="B103" s="35">
         <f t="shared" si="5"/>
         <v>164</v>
       </c>
-      <c r="C103" s="88">
+      <c r="C103" s="74">
         <f t="shared" si="6"/>
         <v>416</v>
       </c>
-      <c r="D103" s="89">
+      <c r="D103" s="75">
         <v>385</v>
       </c>
-      <c r="E103" s="86">
+      <c r="E103" s="73">
         <v>204</v>
       </c>
       <c r="F103" s="2">
@@ -5280,14 +5225,14 @@
         <f t="shared" si="7"/>
         <v>164</v>
       </c>
-      <c r="M103" s="88">
+      <c r="M103" s="74">
         <f t="shared" si="4"/>
         <v>449</v>
       </c>
-      <c r="N103" s="89">
+      <c r="N103" s="75">
         <v>418</v>
       </c>
-      <c r="O103" s="87">
+      <c r="O103" s="73">
         <v>251</v>
       </c>
       <c r="P103" s="2">
@@ -5296,21 +5241,21 @@
       <c r="T103" s="4"/>
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A104" s="60">
+      <c r="A104">
         <v>4</v>
       </c>
-      <c r="B104" s="97">
+      <c r="B104" s="81">
         <f t="shared" si="5"/>
         <v>167</v>
       </c>
-      <c r="C104" s="91">
+      <c r="C104" s="77">
         <f t="shared" si="6"/>
         <v>418</v>
       </c>
-      <c r="D104" s="89">
+      <c r="D104" s="75">
         <v>386</v>
       </c>
-      <c r="E104" s="86">
+      <c r="E104" s="73">
         <v>205</v>
       </c>
       <c r="F104" s="2">
@@ -5320,18 +5265,18 @@
         <v>47</v>
       </c>
       <c r="J104" s="4"/>
-      <c r="L104" s="97">
+      <c r="L104" s="81">
         <f t="shared" si="7"/>
         <v>167</v>
       </c>
-      <c r="M104" s="91">
+      <c r="M104" s="77">
         <f t="shared" si="4"/>
         <v>451</v>
       </c>
-      <c r="N104" s="92">
+      <c r="N104" s="78">
         <v>419</v>
       </c>
-      <c r="O104" s="87">
+      <c r="O104" s="73">
         <v>252</v>
       </c>
       <c r="P104" s="2">
@@ -5340,7 +5285,7 @@
       <c r="T104" s="4"/>
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A105" s="60">
+      <c r="A105">
         <v>4</v>
       </c>
       <c r="B105" s="5">
@@ -5351,10 +5296,10 @@
         <f t="shared" si="6"/>
         <v>420</v>
       </c>
-      <c r="D105" s="69">
+      <c r="D105" s="59">
         <v>387</v>
       </c>
-      <c r="E105" s="60">
+      <c r="E105">
         <v>206</v>
       </c>
       <c r="F105" s="2">
@@ -5372,10 +5317,10 @@
         <f t="shared" si="4"/>
         <v>453</v>
       </c>
-      <c r="N105" s="69">
+      <c r="N105" s="59">
         <v>420</v>
       </c>
-      <c r="O105" s="59">
+      <c r="O105">
         <v>253</v>
       </c>
       <c r="P105" s="2">
@@ -5384,7 +5329,7 @@
       <c r="T105" s="4"/>
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A106" s="60">
+      <c r="A106">
         <v>4</v>
       </c>
       <c r="B106" s="5">
@@ -5395,10 +5340,10 @@
         <f t="shared" si="6"/>
         <v>422</v>
       </c>
-      <c r="D106" s="69">
+      <c r="D106" s="59">
         <v>388</v>
       </c>
-      <c r="E106" s="60">
+      <c r="E106">
         <v>207</v>
       </c>
       <c r="F106" s="2">
@@ -5416,10 +5361,10 @@
         <f t="shared" si="4"/>
         <v>455</v>
       </c>
-      <c r="N106" s="69">
+      <c r="N106" s="59">
         <v>421</v>
       </c>
-      <c r="O106" s="59">
+      <c r="O106">
         <v>254</v>
       </c>
       <c r="P106" s="2">
@@ -5428,7 +5373,7 @@
       <c r="T106" s="4"/>
     </row>
     <row r="107" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A107" s="60">
+      <c r="A107">
         <v>4</v>
       </c>
       <c r="B107" s="5">
@@ -5439,10 +5384,10 @@
         <f t="shared" si="6"/>
         <v>424</v>
       </c>
-      <c r="D107" s="69">
+      <c r="D107" s="59">
         <v>389</v>
       </c>
-      <c r="E107" s="60">
+      <c r="E107">
         <v>208</v>
       </c>
       <c r="F107" s="2">
@@ -5457,10 +5402,10 @@
         <f t="shared" si="4"/>
         <v>457</v>
       </c>
-      <c r="N107" s="69">
+      <c r="N107" s="59">
         <v>422</v>
       </c>
-      <c r="O107" s="59">
+      <c r="O107">
         <v>255</v>
       </c>
       <c r="P107" s="2">
@@ -5469,7 +5414,7 @@
       <c r="T107" s="4"/>
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A108" s="60">
+      <c r="A108">
         <v>4</v>
       </c>
       <c r="B108" s="5">
@@ -5480,10 +5425,10 @@
         <f t="shared" si="6"/>
         <v>426</v>
       </c>
-      <c r="D108" s="69">
+      <c r="D108" s="59">
         <v>390</v>
       </c>
-      <c r="E108" s="60">
+      <c r="E108">
         <v>209</v>
       </c>
       <c r="F108" s="2">
@@ -5498,10 +5443,10 @@
         <f t="shared" si="4"/>
         <v>459</v>
       </c>
-      <c r="N108" s="69">
+      <c r="N108" s="59">
         <v>423</v>
       </c>
-      <c r="O108" s="59">
+      <c r="O108">
         <v>256</v>
       </c>
       <c r="P108" s="2">
@@ -5510,7 +5455,7 @@
       <c r="T108" s="4"/>
     </row>
     <row r="109" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A109" s="60">
+      <c r="A109">
         <v>4</v>
       </c>
       <c r="B109" s="5">
@@ -5521,10 +5466,10 @@
         <f t="shared" si="6"/>
         <v>428</v>
       </c>
-      <c r="D109" s="69">
+      <c r="D109" s="59">
         <v>391</v>
       </c>
-      <c r="E109" s="60">
+      <c r="E109">
         <v>210</v>
       </c>
       <c r="F109" s="2">
@@ -5539,10 +5484,10 @@
         <f t="shared" si="4"/>
         <v>461</v>
       </c>
-      <c r="N109" s="69">
+      <c r="N109" s="59">
         <v>424</v>
       </c>
-      <c r="O109" s="59">
+      <c r="O109">
         <v>257</v>
       </c>
       <c r="P109" s="2">
@@ -5551,7 +5496,7 @@
       <c r="T109" s="4"/>
     </row>
     <row r="110" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A110" s="60">
+      <c r="A110">
         <v>4</v>
       </c>
       <c r="B110" s="5">
@@ -5562,10 +5507,10 @@
         <f t="shared" si="6"/>
         <v>430</v>
       </c>
-      <c r="D110" s="69">
+      <c r="D110" s="59">
         <v>392</v>
       </c>
-      <c r="E110" s="60">
+      <c r="E110">
         <v>211</v>
       </c>
       <c r="F110" s="2">
@@ -5580,10 +5525,10 @@
         <f t="shared" si="4"/>
         <v>463</v>
       </c>
-      <c r="N110" s="69">
+      <c r="N110" s="59">
         <v>425</v>
       </c>
-      <c r="O110" s="59">
+      <c r="O110">
         <v>258</v>
       </c>
       <c r="P110" s="2">
@@ -5592,21 +5537,21 @@
       <c r="T110" s="4"/>
     </row>
     <row r="111" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A111" s="60">
+      <c r="A111">
         <v>4</v>
       </c>
       <c r="B111" s="35">
         <f t="shared" si="5"/>
         <v>188</v>
       </c>
-      <c r="C111" s="88">
+      <c r="C111" s="74">
         <f t="shared" si="6"/>
         <v>432</v>
       </c>
-      <c r="D111" s="89">
+      <c r="D111" s="75">
         <v>393</v>
       </c>
-      <c r="E111" s="86">
+      <c r="E111" s="73">
         <v>212</v>
       </c>
       <c r="F111" s="2">
@@ -5620,14 +5565,14 @@
         <f t="shared" si="7"/>
         <v>188</v>
       </c>
-      <c r="M111" s="88">
+      <c r="M111" s="74">
         <f t="shared" si="4"/>
         <v>465</v>
       </c>
-      <c r="N111" s="89">
+      <c r="N111" s="75">
         <v>426</v>
       </c>
-      <c r="O111" s="87">
+      <c r="O111" s="73">
         <v>259</v>
       </c>
       <c r="P111" s="2">
@@ -5636,7 +5581,7 @@
       <c r="T111" s="4"/>
     </row>
     <row r="112" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A112" s="60">
+      <c r="A112">
         <v>4</v>
       </c>
       <c r="B112" s="5">
@@ -5647,10 +5592,10 @@
         <f t="shared" si="6"/>
         <v>434</v>
       </c>
-      <c r="D112" s="69">
+      <c r="D112" s="59">
         <v>394</v>
       </c>
-      <c r="E112" s="60">
+      <c r="E112">
         <v>213</v>
       </c>
       <c r="F112" s="2">
@@ -5668,10 +5613,10 @@
         <f t="shared" si="4"/>
         <v>467</v>
       </c>
-      <c r="N112" s="69">
+      <c r="N112" s="59">
         <v>427</v>
       </c>
-      <c r="O112" s="59">
+      <c r="O112">
         <v>260</v>
       </c>
       <c r="P112" s="2">
@@ -5680,21 +5625,21 @@
       <c r="T112" s="4"/>
     </row>
     <row r="113" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A113" s="60">
+      <c r="A113">
         <v>4</v>
       </c>
-      <c r="B113" s="94">
+      <c r="B113" s="80">
         <f t="shared" si="5"/>
         <v>194</v>
       </c>
-      <c r="C113" s="91">
+      <c r="C113" s="77">
         <f t="shared" si="6"/>
         <v>436</v>
       </c>
-      <c r="D113" s="92">
+      <c r="D113" s="78">
         <v>395</v>
       </c>
-      <c r="E113" s="93">
+      <c r="E113" s="79">
         <v>214</v>
       </c>
       <c r="F113" s="29">
@@ -5707,18 +5652,18 @@
       <c r="I113" s="30"/>
       <c r="J113" s="31"/>
       <c r="K113" s="30"/>
-      <c r="L113" s="94">
+      <c r="L113" s="80">
         <f t="shared" si="7"/>
         <v>194</v>
       </c>
-      <c r="M113" s="91">
+      <c r="M113" s="77">
         <f t="shared" si="4"/>
         <v>469</v>
       </c>
-      <c r="N113" s="92">
+      <c r="N113" s="78">
         <v>428</v>
       </c>
-      <c r="O113" s="98">
+      <c r="O113" s="79">
         <v>261</v>
       </c>
       <c r="P113" s="29">
@@ -5732,21 +5677,21 @@
       <c r="T113" s="31"/>
     </row>
     <row r="114" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A114" s="60">
+      <c r="A114">
         <v>4</v>
       </c>
       <c r="B114" s="35">
         <f t="shared" si="5"/>
         <v>197</v>
       </c>
-      <c r="C114" s="88">
+      <c r="C114" s="74">
         <f t="shared" si="6"/>
         <v>438</v>
       </c>
-      <c r="D114" s="89">
+      <c r="D114" s="75">
         <v>396</v>
       </c>
-      <c r="E114" s="86">
+      <c r="E114" s="73">
         <v>215</v>
       </c>
       <c r="F114" s="2">
@@ -5757,14 +5702,14 @@
         <f t="shared" si="7"/>
         <v>197</v>
       </c>
-      <c r="M114" s="88">
+      <c r="M114" s="74">
         <f t="shared" si="4"/>
         <v>471</v>
       </c>
-      <c r="N114" s="89">
+      <c r="N114" s="75">
         <v>429</v>
       </c>
-      <c r="O114" s="87">
+      <c r="O114" s="73">
         <v>262</v>
       </c>
       <c r="P114" s="2">
@@ -5773,7 +5718,7 @@
       <c r="T114" s="4"/>
     </row>
     <row r="115" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A115" s="60">
+      <c r="A115">
         <v>4</v>
       </c>
       <c r="B115" s="5">
@@ -5784,10 +5729,10 @@
         <f t="shared" si="6"/>
         <v>440</v>
       </c>
-      <c r="D115" s="69">
+      <c r="D115" s="59">
         <v>397</v>
       </c>
-      <c r="E115" s="60">
+      <c r="E115">
         <v>216</v>
       </c>
       <c r="F115" s="5"/>
@@ -5800,17 +5745,17 @@
         <f t="shared" si="4"/>
         <v>473</v>
       </c>
-      <c r="N115" s="69">
+      <c r="N115" s="59">
         <v>430</v>
       </c>
-      <c r="O115" s="59">
+      <c r="O115">
         <v>263</v>
       </c>
       <c r="P115" s="5"/>
       <c r="T115" s="4"/>
     </row>
     <row r="116" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A116" s="60">
+      <c r="A116">
         <v>4</v>
       </c>
       <c r="B116" s="6">
@@ -5821,10 +5766,10 @@
         <f t="shared" si="6"/>
         <v>442</v>
       </c>
-      <c r="D116" s="71">
+      <c r="D116" s="61">
         <v>398</v>
       </c>
-      <c r="E116" s="60">
+      <c r="E116">
         <v>217</v>
       </c>
       <c r="F116" s="6"/>
@@ -5840,10 +5785,10 @@
         <f t="shared" si="4"/>
         <v>475</v>
       </c>
-      <c r="N116" s="71">
+      <c r="N116" s="61">
         <v>431</v>
       </c>
-      <c r="O116" s="59">
+      <c r="O116">
         <v>264</v>
       </c>
       <c r="P116" s="6"/>
@@ -5878,26 +5823,26 @@
       </c>
       <c r="C120" s="40"/>
       <c r="D120" s="9"/>
-      <c r="F120" s="104" t="s">
+      <c r="F120" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="G120" s="105"/>
-      <c r="H120" s="105"/>
-      <c r="I120" s="105"/>
-      <c r="J120" s="105"/>
+      <c r="G120" s="88"/>
+      <c r="H120" s="88"/>
+      <c r="I120" s="88"/>
+      <c r="J120" s="88"/>
       <c r="L120" s="9" t="s">
         <v>2</v>
       </c>
       <c r="M120" s="40"/>
       <c r="N120" s="9"/>
       <c r="O120" s="33"/>
-      <c r="P120" s="104" t="s">
+      <c r="P120" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="Q120" s="105"/>
-      <c r="R120" s="105"/>
-      <c r="S120" s="105"/>
-      <c r="T120" s="105"/>
+      <c r="Q120" s="88"/>
+      <c r="R120" s="88"/>
+      <c r="S120" s="88"/>
+      <c r="T120" s="88"/>
     </row>
     <row r="121" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B121" s="9" t="s">
@@ -5906,7 +5851,7 @@
       <c r="C121" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D121" s="74" t="s">
+      <c r="D121" s="63" t="s">
         <v>21</v>
       </c>
       <c r="E121" s="13" t="s">
@@ -5933,7 +5878,7 @@
       <c r="M121" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="N121" s="67" t="s">
+      <c r="N121" s="57" t="s">
         <v>21</v>
       </c>
       <c r="O121" s="13" t="s">
@@ -5956,7 +5901,7 @@
       </c>
     </row>
     <row r="122" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A122" s="60">
+      <c r="A122">
         <v>8</v>
       </c>
       <c r="B122">
@@ -5980,7 +5925,7 @@
       <c r="M122" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="N122" s="69">
+      <c r="N122" s="59">
         <v>435</v>
       </c>
       <c r="O122">
@@ -5993,7 +5938,7 @@
       <c r="T122" s="31"/>
     </row>
     <row r="123" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A123" s="60">
+      <c r="A123">
         <v>8</v>
       </c>
       <c r="B123">
@@ -6016,7 +5961,7 @@
       <c r="M123" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="N123" s="69">
+      <c r="N123" s="59">
         <v>436</v>
       </c>
       <c r="O123">
@@ -6028,13 +5973,13 @@
       <c r="T123" s="4"/>
     </row>
     <row r="124" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A124" s="60">
+      <c r="A124">
         <v>8</v>
       </c>
       <c r="B124" s="32">
         <v>122</v>
       </c>
-      <c r="C124" s="62" t="s">
+      <c r="C124" s="56" t="s">
         <v>25</v>
       </c>
       <c r="D124" s="53">
@@ -6057,10 +6002,10 @@
       <c r="L124" s="29">
         <v>122</v>
       </c>
-      <c r="M124" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="N124" s="70">
+      <c r="M124" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="N124" s="60">
         <v>437</v>
       </c>
       <c r="O124" s="3">
@@ -6079,28 +6024,28 @@
       <c r="T124" s="31"/>
     </row>
     <row r="125" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A125" s="60">
+      <c r="A125">
         <v>8</v>
       </c>
-      <c r="B125" s="86">
+      <c r="B125" s="73">
         <v>128</v>
       </c>
       <c r="C125" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="D125" s="88">
+      <c r="D125" s="74">
         <v>405</v>
       </c>
-      <c r="E125" s="86">
+      <c r="E125" s="73">
         <v>223</v>
       </c>
       <c r="F125" s="2">
         <v>14</v>
       </c>
-      <c r="G125" s="64">
+      <c r="G125" s="3">
         <v>32</v>
       </c>
-      <c r="H125" s="98">
+      <c r="H125" s="79">
         <v>52</v>
       </c>
       <c r="J125" s="4"/>
@@ -6110,10 +6055,10 @@
       <c r="M125" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="N125" s="89">
+      <c r="N125" s="75">
         <v>438</v>
       </c>
-      <c r="O125" s="86">
+      <c r="O125" s="73">
         <v>270</v>
       </c>
       <c r="P125" s="2">
@@ -6128,7 +6073,7 @@
       <c r="T125" s="4"/>
     </row>
     <row r="126" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A126" s="60">
+      <c r="A126">
         <v>8</v>
       </c>
       <c r="B126">
@@ -6140,13 +6085,13 @@
       <c r="D126" s="52">
         <v>406</v>
       </c>
-      <c r="E126" s="60">
+      <c r="E126">
         <v>224</v>
       </c>
       <c r="F126" s="2">
         <v>14</v>
       </c>
-      <c r="G126" s="64">
+      <c r="G126" s="3">
         <v>32</v>
       </c>
       <c r="H126" s="3">
@@ -6159,10 +6104,10 @@
       <c r="M126" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="N126" s="69">
+      <c r="N126" s="59">
         <v>439</v>
       </c>
-      <c r="O126" s="60">
+      <c r="O126">
         <v>271</v>
       </c>
       <c r="P126" s="2">
@@ -6177,19 +6122,19 @@
       <c r="T126" s="4"/>
     </row>
     <row r="127" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A127" s="60">
+      <c r="A127">
         <v>8</v>
       </c>
-      <c r="B127" s="99">
+      <c r="B127" s="82">
         <v>140</v>
       </c>
-      <c r="C127" s="97" t="s">
-        <v>25</v>
-      </c>
-      <c r="D127" s="91">
+      <c r="C127" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="D127" s="77">
         <v>407</v>
       </c>
-      <c r="E127" s="93">
+      <c r="E127" s="79">
         <v>225</v>
       </c>
       <c r="F127" s="29">
@@ -6204,16 +6149,16 @@
       <c r="I127" s="30"/>
       <c r="J127" s="31"/>
       <c r="K127" s="30"/>
-      <c r="L127" s="94">
+      <c r="L127" s="80">
         <v>140</v>
       </c>
-      <c r="M127" s="97" t="s">
-        <v>25</v>
-      </c>
-      <c r="N127" s="92">
+      <c r="M127" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="N127" s="78">
         <v>440</v>
       </c>
-      <c r="O127" s="93">
+      <c r="O127" s="79">
         <v>272</v>
       </c>
       <c r="P127" s="29">
@@ -6229,25 +6174,25 @@
       <c r="T127" s="31"/>
     </row>
     <row r="128" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A128" s="60">
+      <c r="A128">
         <v>8</v>
       </c>
-      <c r="B128" s="99">
+      <c r="B128" s="82">
         <v>146</v>
       </c>
-      <c r="C128" s="97" t="s">
-        <v>25</v>
-      </c>
-      <c r="D128" s="91">
+      <c r="C128" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="D128" s="77">
         <v>408</v>
       </c>
-      <c r="E128" s="93">
+      <c r="E128" s="79">
         <v>226</v>
       </c>
       <c r="F128" s="29">
         <v>14</v>
       </c>
-      <c r="G128" s="63">
+      <c r="G128" s="32">
         <v>23</v>
       </c>
       <c r="H128" s="32">
@@ -6255,16 +6200,16 @@
       </c>
       <c r="I128" s="30"/>
       <c r="J128" s="31"/>
-      <c r="L128" s="94">
+      <c r="L128" s="80">
         <v>146</v>
       </c>
-      <c r="M128" s="97" t="s">
-        <v>25</v>
-      </c>
-      <c r="N128" s="92">
+      <c r="M128" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="N128" s="78">
         <v>441</v>
       </c>
-      <c r="O128" s="93">
+      <c r="O128" s="79">
         <v>273</v>
       </c>
       <c r="P128" s="29">
@@ -6280,7 +6225,7 @@
       <c r="T128" s="31"/>
     </row>
     <row r="129" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A129" s="60">
+      <c r="A129">
         <v>8</v>
       </c>
       <c r="B129">
@@ -6292,13 +6237,13 @@
       <c r="D129" s="52">
         <v>409</v>
       </c>
-      <c r="E129" s="60">
+      <c r="E129">
         <v>227</v>
       </c>
       <c r="F129" s="2">
         <v>14</v>
       </c>
-      <c r="G129" s="63">
+      <c r="G129" s="32">
         <v>33</v>
       </c>
       <c r="H129" s="3">
@@ -6312,32 +6257,32 @@
       <c r="M129" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="N129" s="69">
+      <c r="N129" s="59">
         <v>442</v>
       </c>
-      <c r="O129" s="60">
+      <c r="O129">
         <v>274</v>
       </c>
-      <c r="P129" s="55">
+      <c r="P129" s="2">
         <v>17</v>
       </c>
       <c r="Q129" s="32">
         <v>29</v>
       </c>
-      <c r="R129" s="77">
+      <c r="R129" s="3">
         <v>53</v>
       </c>
       <c r="S129" s="30"/>
       <c r="T129" s="31"/>
     </row>
     <row r="130" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A130" s="60">
+      <c r="A130">
         <v>8</v>
       </c>
       <c r="B130" s="32">
         <v>158</v>
       </c>
-      <c r="C130" s="62" t="s">
+      <c r="C130" s="56" t="s">
         <v>25</v>
       </c>
       <c r="D130" s="53">
@@ -6360,10 +6305,10 @@
       <c r="L130" s="29">
         <v>158</v>
       </c>
-      <c r="M130" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="N130" s="70">
+      <c r="M130" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="N130" s="60">
         <v>443</v>
       </c>
       <c r="O130" s="3">
@@ -6382,28 +6327,28 @@
       <c r="T130" s="31"/>
     </row>
     <row r="131" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A131" s="60">
+      <c r="A131">
         <v>8</v>
       </c>
-      <c r="B131" s="86">
+      <c r="B131" s="73">
         <v>164</v>
       </c>
       <c r="C131" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="D131" s="88">
+      <c r="D131" s="74">
         <v>411</v>
       </c>
-      <c r="E131" s="86">
+      <c r="E131" s="73">
         <v>229</v>
       </c>
       <c r="F131" s="2">
         <v>18</v>
       </c>
-      <c r="G131" s="77">
+      <c r="G131" s="3">
         <v>28</v>
       </c>
-      <c r="H131" s="98">
+      <c r="H131" s="79">
         <v>51</v>
       </c>
       <c r="J131" s="4"/>
@@ -6413,10 +6358,10 @@
       <c r="M131" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="N131" s="89">
+      <c r="N131" s="75">
         <v>444</v>
       </c>
-      <c r="O131" s="86">
+      <c r="O131" s="73">
         <v>276</v>
       </c>
       <c r="P131" s="2">
@@ -6425,13 +6370,13 @@
       <c r="Q131" s="32">
         <v>29</v>
       </c>
-      <c r="R131" s="77">
+      <c r="R131" s="3">
         <v>53</v>
       </c>
       <c r="T131" s="4"/>
     </row>
     <row r="132" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A132" s="60">
+      <c r="A132">
         <v>8</v>
       </c>
       <c r="B132">
@@ -6443,13 +6388,13 @@
       <c r="D132" s="52">
         <v>412</v>
       </c>
-      <c r="E132" s="60">
+      <c r="E132">
         <v>230</v>
       </c>
       <c r="F132" s="2">
         <v>18</v>
       </c>
-      <c r="G132" s="77">
+      <c r="G132" s="3">
         <v>28</v>
       </c>
       <c r="H132" s="3">
@@ -6462,10 +6407,10 @@
       <c r="M132" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="N132" s="69">
+      <c r="N132" s="59">
         <v>445</v>
       </c>
-      <c r="O132" s="60">
+      <c r="O132">
         <v>277</v>
       </c>
       <c r="P132" s="2">
@@ -6474,13 +6419,13 @@
       <c r="Q132" s="32">
         <v>31</v>
       </c>
-      <c r="R132" s="77">
+      <c r="R132" s="3">
         <v>53</v>
       </c>
       <c r="T132" s="4"/>
     </row>
     <row r="133" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A133" s="60">
+      <c r="A133">
         <v>8</v>
       </c>
       <c r="B133">
@@ -6492,7 +6437,7 @@
       <c r="D133" s="52">
         <v>413</v>
       </c>
-      <c r="E133" s="60">
+      <c r="E133">
         <v>231</v>
       </c>
       <c r="F133" s="2">
@@ -6511,10 +6456,10 @@
       <c r="M133" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="N133" s="69">
+      <c r="N133" s="59">
         <v>446</v>
       </c>
-      <c r="O133" s="60">
+      <c r="O133">
         <v>278</v>
       </c>
       <c r="P133" s="2">
@@ -6529,7 +6474,7 @@
       <c r="T133" s="4"/>
     </row>
     <row r="134" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A134" s="60">
+      <c r="A134">
         <v>8</v>
       </c>
       <c r="B134">
@@ -6541,7 +6486,7 @@
       <c r="D134" s="52">
         <v>414</v>
       </c>
-      <c r="E134" s="60">
+      <c r="E134">
         <v>232</v>
       </c>
       <c r="F134" s="2">
@@ -6561,38 +6506,37 @@
       <c r="M134" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="N134" s="69">
+      <c r="N134" s="59">
         <v>447</v>
       </c>
-      <c r="O134" s="60">
+      <c r="O134">
         <v>279</v>
       </c>
-      <c r="P134" s="55">
+      <c r="P134" s="2">
         <v>19</v>
       </c>
       <c r="Q134" s="32">
         <v>31</v>
       </c>
-      <c r="R134" s="77">
+      <c r="R134" s="3">
         <v>42</v>
       </c>
-      <c r="S134" s="56"/>
-      <c r="T134" s="57"/>
+      <c r="T134" s="4"/>
     </row>
     <row r="135" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A135" s="60">
+      <c r="A135">
         <v>8</v>
       </c>
-      <c r="B135" s="86">
+      <c r="B135" s="73">
         <v>188</v>
       </c>
       <c r="C135" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="D135" s="88">
+      <c r="D135" s="74">
         <v>415</v>
       </c>
-      <c r="E135" s="86">
+      <c r="E135" s="73">
         <v>233</v>
       </c>
       <c r="F135" s="2">
@@ -6611,10 +6555,10 @@
       <c r="M135" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="N135" s="89">
+      <c r="N135" s="75">
         <v>448</v>
       </c>
-      <c r="O135" s="86">
+      <c r="O135" s="73">
         <v>280</v>
       </c>
       <c r="P135" s="2">
@@ -6629,19 +6573,19 @@
       <c r="T135" s="4"/>
     </row>
     <row r="136" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A136" s="60">
+      <c r="A136">
         <v>8</v>
       </c>
-      <c r="B136" s="99">
+      <c r="B136" s="82">
         <v>194</v>
       </c>
-      <c r="C136" s="97" t="s">
-        <v>25</v>
-      </c>
-      <c r="D136" s="91">
+      <c r="C136" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="D136" s="77">
         <v>416</v>
       </c>
-      <c r="E136" s="93">
+      <c r="E136" s="79">
         <v>234</v>
       </c>
       <c r="F136" s="29">
@@ -6655,16 +6599,16 @@
       </c>
       <c r="I136" s="30"/>
       <c r="J136" s="31"/>
-      <c r="L136" s="94">
+      <c r="L136" s="80">
         <v>194</v>
       </c>
-      <c r="M136" s="97" t="s">
-        <v>25</v>
-      </c>
-      <c r="N136" s="92">
+      <c r="M136" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="N136" s="78">
         <v>449</v>
       </c>
-      <c r="O136" s="93">
+      <c r="O136" s="79">
         <v>281</v>
       </c>
       <c r="P136" s="29">
@@ -6680,7 +6624,7 @@
       <c r="T136" s="31"/>
     </row>
     <row r="137" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A137" s="60">
+      <c r="A137">
         <v>8</v>
       </c>
       <c r="B137">
@@ -6692,7 +6636,7 @@
       <c r="D137" s="52">
         <v>417</v>
       </c>
-      <c r="E137" s="60">
+      <c r="E137">
         <v>235</v>
       </c>
       <c r="F137" s="5"/>
@@ -6703,17 +6647,17 @@
       <c r="M137" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="N137" s="69">
+      <c r="N137" s="59">
         <v>450</v>
       </c>
-      <c r="O137" s="60">
+      <c r="O137">
         <v>282</v>
       </c>
       <c r="P137" s="5"/>
       <c r="T137" s="4"/>
     </row>
     <row r="138" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A138" s="60">
+      <c r="A138">
         <v>8</v>
       </c>
       <c r="B138" s="7">
@@ -6725,7 +6669,7 @@
       <c r="D138" s="54">
         <v>418</v>
       </c>
-      <c r="E138" s="60">
+      <c r="E138">
         <v>236</v>
       </c>
       <c r="F138" s="6"/>
@@ -6739,10 +6683,10 @@
       <c r="M138" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="N138" s="71">
+      <c r="N138" s="61">
         <v>451</v>
       </c>
-      <c r="O138" s="60">
+      <c r="O138">
         <v>283</v>
       </c>
       <c r="P138" s="6"/>
@@ -6761,7 +6705,7 @@
       <c r="D141" t="s">
         <v>43</v>
       </c>
-      <c r="L141" s="60" t="s">
+      <c r="L141" t="s">
         <v>2</v>
       </c>
       <c r="M141" t="s">
@@ -6775,7 +6719,7 @@
       <c r="B142" t="s">
         <v>41</v>
       </c>
-      <c r="L142" s="60" t="s">
+      <c r="L142" t="s">
         <v>41</v>
       </c>
     </row>
@@ -6783,7 +6727,7 @@
       <c r="B143">
         <v>125</v>
       </c>
-      <c r="L143" s="60">
+      <c r="L143">
         <v>127</v>
       </c>
     </row>
@@ -6791,18 +6735,15 @@
       <c r="B144">
         <v>126</v>
       </c>
-      <c r="L144" s="60">
+      <c r="L144">
         <v>128</v>
       </c>
-    </row>
-    <row r="145" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L145" s="60"/>
     </row>
     <row r="146" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>42</v>
       </c>
-      <c r="L146" s="60" t="s">
+      <c r="L146" t="s">
         <v>42</v>
       </c>
     </row>
@@ -6811,7 +6752,7 @@
         <f ca="1">"3,1,"&amp;INDIRECT(D141&amp;B143)&amp;","&amp;INDIRECT(D141&amp;B144)&amp;",0,-1,NONE,NONE,SO MINISCAN "&amp;A138&amp;"KHZ STARTING ORDER "&amp;INDIRECT(C141&amp;B143)&amp;" &amp; "&amp;INDIRECT(C141&amp;B144)</f>
         <v>3,1,223,224,0,-1,NONE,NONE,SO MINISCAN 8KHZ STARTING ORDER 128 &amp; 134</v>
       </c>
-      <c r="L147" s="60" t="str">
+      <c r="L147" t="str">
         <f ca="1">"3,1,"&amp;INDIRECT(N141&amp;L143)&amp;","&amp;INDIRECT(N141&amp;L144)&amp;",1,-1,NONE,NONE,LNO MINISCAN "&amp;A138&amp;"KHZ STARTING ORDER "&amp;INDIRECT(M141&amp;L143)&amp;" &amp; "&amp;INDIRECT(M141&amp;L144)</f>
         <v>3,1,272,273,1,-1,NONE,NONE,LNO MINISCAN 8KHZ STARTING ORDER 140 &amp; 146</v>
       </c>

</xml_diff>

<commit_message>
MTP059 COP rows generated
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB09E15-C497-49F7-AAB9-426867F51301}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2054C092-DA23-4A69-95DB-A4F53543EF0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -894,7 +894,7 @@
     <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1016,6 +1016,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -1339,8 +1340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O53" sqref="O53:O54"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E133" sqref="E133:E136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1455,6 +1456,9 @@
       <c r="L5" s="3">
         <v>49</v>
       </c>
+      <c r="M5" s="3">
+        <v>59</v>
+      </c>
       <c r="AE5" s="4"/>
     </row>
     <row r="6" spans="2:31" x14ac:dyDescent="0.25">
@@ -6449,6 +6453,9 @@
       <c r="H133" s="3">
         <v>41</v>
       </c>
+      <c r="I133" s="89">
+        <v>59</v>
+      </c>
       <c r="J133" s="4"/>
       <c r="L133" s="5">
         <v>176</v>
@@ -6497,6 +6504,9 @@
       </c>
       <c r="H134" s="3">
         <v>42</v>
+      </c>
+      <c r="I134" s="89">
+        <v>59</v>
       </c>
       <c r="J134" s="4"/>
       <c r="K134" s="30"/>
@@ -6548,6 +6558,9 @@
       <c r="H135" s="3">
         <v>41</v>
       </c>
+      <c r="I135" s="89">
+        <v>59</v>
+      </c>
       <c r="J135" s="4"/>
       <c r="L135" s="35">
         <v>188</v>
@@ -6597,7 +6610,9 @@
       <c r="H136" s="32">
         <v>42</v>
       </c>
-      <c r="I136" s="30"/>
+      <c r="I136" s="32">
+        <v>59</v>
+      </c>
       <c r="J136" s="31"/>
       <c r="L136" s="80">
         <v>194</v>

</xml_diff>

<commit_message>
MTP065 COP rows automatically generated
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24675858-D2D1-4C91-946A-9F89ECC6E964}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01552E63-3282-4B16-BC52-48DD3C67A315}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1340,7 +1340,7 @@
   <dimension ref="A1:AE147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,7 +1503,9 @@
       <c r="P6" s="18">
         <v>55</v>
       </c>
-      <c r="Q6" s="7"/>
+      <c r="Q6" s="18">
+        <v>64</v>
+      </c>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
@@ -2755,6 +2757,9 @@
       <c r="F39" s="2">
         <v>61</v>
       </c>
+      <c r="G39" s="3">
+        <v>64</v>
+      </c>
       <c r="J39" s="4"/>
       <c r="L39" s="25">
         <v>180</v>
@@ -2795,7 +2800,9 @@
       <c r="E40">
         <v>75</v>
       </c>
-      <c r="F40" s="5"/>
+      <c r="F40" s="2">
+        <v>64</v>
+      </c>
       <c r="J40" s="4"/>
       <c r="L40" s="25">
         <v>182</v>
@@ -2842,6 +2849,9 @@
       <c r="G41" s="3">
         <v>49</v>
       </c>
+      <c r="H41" s="3">
+        <v>64</v>
+      </c>
       <c r="J41" s="4"/>
       <c r="L41" s="74">
         <v>188</v>
@@ -2887,6 +2897,9 @@
       </c>
       <c r="G42" s="3">
         <v>49</v>
+      </c>
+      <c r="H42" s="3">
+        <v>64</v>
       </c>
       <c r="J42" s="4"/>
       <c r="L42" s="25">

</xml_diff>

<commit_message>
MTP075 done and UVIS COP rows added to previous MTPs
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6186DA5A-E870-4698-8AE7-293B934C36DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52135466-701D-42AC-A026-6678CC86D66F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="30960" windowHeight="12264" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -897,7 +897,7 @@
     <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1020,6 +1020,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -1343,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F88" sqref="F88"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1462,6 +1464,9 @@
       <c r="M5" s="3">
         <v>59</v>
       </c>
+      <c r="N5" s="3">
+        <v>75</v>
+      </c>
       <c r="AE5" s="4"/>
     </row>
     <row r="6" spans="2:31" x14ac:dyDescent="0.3">
@@ -1510,7 +1515,9 @@
       <c r="Q6" s="18">
         <v>64</v>
       </c>
-      <c r="R6" s="7"/>
+      <c r="R6" s="18">
+        <v>75</v>
+      </c>
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
       <c r="U6" s="7"/>
@@ -6646,7 +6653,9 @@
       <c r="I135" s="3">
         <v>59</v>
       </c>
-      <c r="J135" s="4"/>
+      <c r="J135" s="90">
+        <v>75</v>
+      </c>
       <c r="L135" s="35">
         <v>188</v>
       </c>
@@ -6698,7 +6707,9 @@
       <c r="I136" s="32">
         <v>59</v>
       </c>
-      <c r="J136" s="31"/>
+      <c r="J136" s="91">
+        <v>75</v>
+      </c>
       <c r="L136" s="80">
         <v>194</v>
       </c>

</xml_diff>

<commit_message>
MTP078 done; MTP079 inputs added; code upgraded to work with py3.11 (floats and ints)
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DEDA6B-22E2-43D0-AAE1-29220845E51D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83A0044-DBA5-4C5E-A2AF-303F73F16F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="20832" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -897,7 +908,7 @@
     <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1023,6 +1034,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -1346,27 +1358,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E129" sqref="E129"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G101" sqref="G101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" customWidth="1"/>
-    <col min="12" max="12" width="16.88671875" customWidth="1"/>
-    <col min="13" max="13" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="21" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.33203125" customWidth="1"/>
-    <col min="23" max="23" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.28515625" customWidth="1"/>
+    <col min="23" max="23" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1374,12 +1386,12 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="2:31" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:31" ht="18.75" x14ac:dyDescent="0.3">
       <c r="W2" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:31" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:31" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="14" t="s">
         <v>3</v>
       </c>
@@ -1392,7 +1404,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C4" s="13" t="s">
         <v>12</v>
       </c>
@@ -1431,7 +1443,7 @@
       <c r="AD4" s="71"/>
       <c r="AE4" s="65"/>
     </row>
-    <row r="5" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C5" s="19" t="s">
         <v>1</v>
       </c>
@@ -1470,7 +1482,7 @@
       </c>
       <c r="AE5" s="4"/>
     </row>
-    <row r="6" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C6" s="20" t="s">
         <v>2</v>
       </c>
@@ -1533,14 +1545,14 @@
       <c r="AD6" s="7"/>
       <c r="AE6" s="8"/>
     </row>
-    <row r="9" spans="2:31" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:31" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
@@ -1579,7 +1591,7 @@
       <c r="AD10" s="71"/>
       <c r="AE10" s="65"/>
     </row>
-    <row r="11" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C11" s="19" t="s">
         <v>34</v>
       </c>
@@ -1636,7 +1648,7 @@
       <c r="AD11" s="16"/>
       <c r="AE11" s="17"/>
     </row>
-    <row r="12" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C12" s="20" t="s">
         <v>36</v>
       </c>
@@ -1681,12 +1693,12 @@
       <c r="AD12" s="7"/>
       <c r="AE12" s="8"/>
     </row>
-    <row r="13" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:31" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:31" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B15" s="14" t="s">
         <v>0</v>
       </c>
@@ -1700,12 +1712,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:31" x14ac:dyDescent="0.25">
       <c r="AC16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
         <v>1</v>
       </c>
@@ -1733,7 +1745,7 @@
       <c r="S17" s="91"/>
       <c r="T17" s="91"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B18" s="39" t="s">
         <v>10</v>
       </c>
@@ -1808,7 +1820,7 @@
       </c>
       <c r="AE18" s="9"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1861,7 +1873,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1908,7 +1920,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1955,7 +1967,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2019,7 +2031,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2068,7 +2080,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2117,7 +2129,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -2177,7 +2189,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -2226,7 +2238,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -2278,7 +2290,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2323,7 +2335,7 @@
       </c>
       <c r="Z28" s="55"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2366,7 +2378,7 @@
       <c r="Y29" s="48"/>
       <c r="Z29" s="49"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -2415,7 +2427,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -2460,7 +2472,7 @@
       <c r="Y31" s="48"/>
       <c r="Z31" s="49"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2510,7 +2522,7 @@
       <c r="Y32" s="48"/>
       <c r="Z32" s="49"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -2555,7 +2567,7 @@
       <c r="Y33" s="48"/>
       <c r="Z33" s="49"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -2601,7 +2613,7 @@
       <c r="Y34" s="48"/>
       <c r="Z34" s="49"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
@@ -2644,7 +2656,7 @@
       <c r="Y35" s="48"/>
       <c r="Z35" s="49"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -2689,7 +2701,7 @@
       <c r="Y36" s="48"/>
       <c r="Z36" s="49"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -2732,7 +2744,7 @@
       <c r="Y37" s="48"/>
       <c r="Z37" s="49"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
@@ -2775,7 +2787,7 @@
       <c r="Y38" s="48"/>
       <c r="Z38" s="49"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1</v>
       </c>
@@ -2821,7 +2833,7 @@
       <c r="Y39" s="48"/>
       <c r="Z39" s="49"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1</v>
       </c>
@@ -2864,7 +2876,7 @@
       <c r="Y40" s="48"/>
       <c r="Z40" s="49"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1</v>
       </c>
@@ -2914,7 +2926,7 @@
       <c r="Y41" s="48"/>
       <c r="Z41" s="49"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1</v>
       </c>
@@ -2965,7 +2977,7 @@
       <c r="Y42" s="48"/>
       <c r="Z42" s="49"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
@@ -3020,7 +3032,7 @@
       <c r="Y43" s="48"/>
       <c r="Z43" s="49"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1</v>
       </c>
@@ -3067,7 +3079,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1</v>
       </c>
@@ -3113,7 +3125,7 @@
       <c r="Y45" s="5"/>
       <c r="Z45" s="4"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1</v>
       </c>
@@ -3154,7 +3166,7 @@
       <c r="Y46" s="5"/>
       <c r="Z46" s="4"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1</v>
       </c>
@@ -3193,7 +3205,7 @@
       <c r="Y47" s="5"/>
       <c r="Z47" s="4"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1</v>
       </c>
@@ -3240,7 +3252,7 @@
       <c r="Y48" s="5"/>
       <c r="Z48" s="4"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="W49" s="5">
         <v>4526.9799999999996</v>
       </c>
@@ -3250,7 +3262,7 @@
       <c r="Y49" s="6"/>
       <c r="Z49" s="8"/>
     </row>
-    <row r="50" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B50" s="14" t="s">
         <v>0</v>
       </c>
@@ -3262,7 +3274,7 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -3273,7 +3285,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B52" s="9" t="s">
         <v>1</v>
       </c>
@@ -3301,7 +3313,7 @@
       <c r="S52" s="91"/>
       <c r="T52" s="91"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B53" s="9" t="s">
         <v>10</v>
       </c>
@@ -3357,7 +3369,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2</v>
       </c>
@@ -3394,7 +3406,7 @@
       </c>
       <c r="T54" s="4"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2</v>
       </c>
@@ -3431,7 +3443,7 @@
       <c r="P55" s="5"/>
       <c r="T55" s="4"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2</v>
       </c>
@@ -3483,7 +3495,7 @@
       <c r="S56" s="30"/>
       <c r="T56" s="31"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2</v>
       </c>
@@ -3520,7 +3532,7 @@
       <c r="P57" s="5"/>
       <c r="T57" s="4"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2</v>
       </c>
@@ -3557,7 +3569,7 @@
       <c r="P58" s="5"/>
       <c r="T58" s="4"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2</v>
       </c>
@@ -3598,7 +3610,7 @@
       </c>
       <c r="T59" s="4"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2</v>
       </c>
@@ -3635,7 +3647,7 @@
       <c r="P60" s="5"/>
       <c r="T60" s="4"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2</v>
       </c>
@@ -3687,7 +3699,7 @@
       <c r="S61" s="30"/>
       <c r="T61" s="31"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2</v>
       </c>
@@ -3724,7 +3736,7 @@
       <c r="P62" s="5"/>
       <c r="T62" s="4"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2</v>
       </c>
@@ -3776,7 +3788,7 @@
       <c r="S63" s="30"/>
       <c r="T63" s="31"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2</v>
       </c>
@@ -3813,7 +3825,7 @@
       <c r="P64" s="5"/>
       <c r="T64" s="4"/>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2</v>
       </c>
@@ -3850,7 +3862,7 @@
       <c r="P65" s="35"/>
       <c r="T65" s="4"/>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2</v>
       </c>
@@ -3887,7 +3899,7 @@
       <c r="P66" s="5"/>
       <c r="T66" s="4"/>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2</v>
       </c>
@@ -3924,7 +3936,7 @@
       <c r="P67" s="5"/>
       <c r="T67" s="4"/>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2</v>
       </c>
@@ -3976,7 +3988,7 @@
       <c r="S68" s="30"/>
       <c r="T68" s="31"/>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2</v>
       </c>
@@ -4023,7 +4035,7 @@
       </c>
       <c r="T69" s="4"/>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2</v>
       </c>
@@ -4064,7 +4076,7 @@
       </c>
       <c r="T70" s="4"/>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2</v>
       </c>
@@ -4101,7 +4113,7 @@
       <c r="P71" s="5"/>
       <c r="T71" s="4"/>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2</v>
       </c>
@@ -4138,7 +4150,7 @@
       <c r="P72" s="5"/>
       <c r="T72" s="4"/>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2</v>
       </c>
@@ -4175,7 +4187,7 @@
       <c r="P73" s="5"/>
       <c r="T73" s="4"/>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2</v>
       </c>
@@ -4212,7 +4224,7 @@
       <c r="P74" s="5"/>
       <c r="T74" s="4"/>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2</v>
       </c>
@@ -4249,7 +4261,7 @@
       <c r="P75" s="5"/>
       <c r="T75" s="4"/>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2</v>
       </c>
@@ -4290,7 +4302,7 @@
       </c>
       <c r="T76" s="4"/>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2</v>
       </c>
@@ -4334,7 +4346,7 @@
       </c>
       <c r="T77" s="4"/>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2</v>
       </c>
@@ -4371,7 +4383,7 @@
       <c r="P78" s="5"/>
       <c r="T78" s="4"/>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2</v>
       </c>
@@ -4419,7 +4431,7 @@
       <c r="S79" s="30"/>
       <c r="T79" s="31"/>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2</v>
       </c>
@@ -4456,7 +4468,7 @@
       <c r="P80" s="5"/>
       <c r="T80" s="4"/>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2</v>
       </c>
@@ -4493,7 +4505,7 @@
       <c r="P81" s="5"/>
       <c r="T81" s="4"/>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2</v>
       </c>
@@ -4536,7 +4548,7 @@
       <c r="S82" s="7"/>
       <c r="T82" s="8"/>
     </row>
-    <row r="84" spans="1:20" ht="18" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B84" s="14" t="s">
         <v>0</v>
       </c>
@@ -4550,7 +4562,7 @@
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
@@ -4558,7 +4570,7 @@
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B86" s="9" t="s">
         <v>1</v>
       </c>
@@ -4586,7 +4598,7 @@
       <c r="S86" s="91"/>
       <c r="T86" s="91"/>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B87" s="9" t="s">
         <v>10</v>
       </c>
@@ -4642,7 +4654,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>4</v>
       </c>
@@ -4677,7 +4689,7 @@
       <c r="P88" s="5"/>
       <c r="T88" s="4"/>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>4</v>
       </c>
@@ -4718,7 +4730,7 @@
       </c>
       <c r="T89" s="4"/>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>4</v>
       </c>
@@ -4768,7 +4780,7 @@
       <c r="S90" s="30"/>
       <c r="T90" s="31"/>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>4</v>
       </c>
@@ -4809,7 +4821,7 @@
       </c>
       <c r="T91" s="4"/>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>4</v>
       </c>
@@ -4846,7 +4858,7 @@
       <c r="P92" s="5"/>
       <c r="T92" s="4"/>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>4</v>
       </c>
@@ -4883,7 +4895,7 @@
       <c r="P93" s="5"/>
       <c r="T93" s="4"/>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>4</v>
       </c>
@@ -4924,7 +4936,7 @@
       </c>
       <c r="T94" s="4"/>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>4</v>
       </c>
@@ -4976,7 +4988,7 @@
       <c r="S95" s="30"/>
       <c r="T95" s="31"/>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>4</v>
       </c>
@@ -5015,7 +5027,7 @@
       </c>
       <c r="T96" s="4"/>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>4</v>
       </c>
@@ -5065,7 +5077,7 @@
       <c r="S97" s="30"/>
       <c r="T97" s="31"/>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>4</v>
       </c>
@@ -5112,7 +5124,7 @@
       <c r="S98" s="30"/>
       <c r="T98" s="31"/>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>4</v>
       </c>
@@ -5151,7 +5163,7 @@
       </c>
       <c r="T99" s="4"/>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>4</v>
       </c>
@@ -5190,7 +5202,7 @@
       </c>
       <c r="T100" s="4"/>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>4</v>
       </c>
@@ -5231,7 +5243,7 @@
       </c>
       <c r="T101" s="4"/>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>4</v>
       </c>
@@ -5281,7 +5293,7 @@
       <c r="S102" s="30"/>
       <c r="T102" s="31"/>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>4</v>
       </c>
@@ -5322,7 +5334,7 @@
       </c>
       <c r="T103" s="4"/>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>4</v>
       </c>
@@ -5366,7 +5378,7 @@
       </c>
       <c r="T104" s="4"/>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>4</v>
       </c>
@@ -5410,7 +5422,7 @@
       </c>
       <c r="T105" s="4"/>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>4</v>
       </c>
@@ -5454,7 +5466,7 @@
       </c>
       <c r="T106" s="4"/>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>4</v>
       </c>
@@ -5495,7 +5507,7 @@
       </c>
       <c r="T107" s="4"/>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>4</v>
       </c>
@@ -5536,7 +5548,7 @@
       </c>
       <c r="T108" s="4"/>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>4</v>
       </c>
@@ -5577,7 +5589,7 @@
       </c>
       <c r="T109" s="4"/>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>4</v>
       </c>
@@ -5618,7 +5630,7 @@
       </c>
       <c r="T110" s="4"/>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>4</v>
       </c>
@@ -5644,6 +5656,9 @@
       </c>
       <c r="H111" s="3">
         <v>62</v>
+      </c>
+      <c r="I111" s="92">
+        <v>78</v>
       </c>
       <c r="J111" s="4"/>
       <c r="L111" s="35">
@@ -5666,7 +5681,7 @@
       <c r="Q111" s="73"/>
       <c r="T111" s="4"/>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>4</v>
       </c>
@@ -5692,6 +5707,9 @@
       </c>
       <c r="H112" s="3">
         <v>62</v>
+      </c>
+      <c r="I112" s="92">
+        <v>78</v>
       </c>
       <c r="J112" s="4"/>
       <c r="L112" s="5">
@@ -5713,7 +5731,7 @@
       </c>
       <c r="T112" s="4"/>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>4</v>
       </c>
@@ -5737,7 +5755,9 @@
       <c r="G113" s="32">
         <v>13</v>
       </c>
-      <c r="H113" s="30"/>
+      <c r="H113" s="32">
+        <v>78</v>
+      </c>
       <c r="I113" s="30"/>
       <c r="J113" s="31"/>
       <c r="K113" s="30"/>
@@ -5765,7 +5785,7 @@
       <c r="S113" s="30"/>
       <c r="T113" s="31"/>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>4</v>
       </c>
@@ -5785,6 +5805,9 @@
       </c>
       <c r="F114" s="2">
         <v>8</v>
+      </c>
+      <c r="G114" s="93">
+        <v>78</v>
       </c>
       <c r="J114" s="4"/>
       <c r="L114" s="35">
@@ -5806,7 +5829,7 @@
       </c>
       <c r="T114" s="4"/>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>4</v>
       </c>
@@ -5843,7 +5866,7 @@
       <c r="P115" s="5"/>
       <c r="T115" s="4"/>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>4</v>
       </c>
@@ -5886,7 +5909,7 @@
       <c r="S116" s="7"/>
       <c r="T116" s="8"/>
     </row>
-    <row r="118" spans="1:20" ht="18" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B118" s="14" t="s">
         <v>0</v>
       </c>
@@ -5898,7 +5921,7 @@
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
@@ -5906,7 +5929,7 @@
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B120" s="9" t="s">
         <v>1</v>
       </c>
@@ -5933,7 +5956,7 @@
       <c r="S120" s="91"/>
       <c r="T120" s="91"/>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B121" s="9" t="s">
         <v>10</v>
       </c>
@@ -5989,7 +6012,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>8</v>
       </c>
@@ -6028,7 +6051,7 @@
       <c r="S122" s="30"/>
       <c r="T122" s="31"/>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>8</v>
       </c>
@@ -6063,7 +6086,7 @@
       </c>
       <c r="T123" s="4"/>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>8</v>
       </c>
@@ -6116,7 +6139,7 @@
       <c r="S124" s="30"/>
       <c r="T124" s="31"/>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>8</v>
       </c>
@@ -6168,7 +6191,7 @@
       </c>
       <c r="T125" s="4"/>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>8</v>
       </c>
@@ -6193,7 +6216,7 @@
       <c r="H126" s="3">
         <v>52</v>
       </c>
-      <c r="I126" s="92">
+      <c r="I126" s="3">
         <v>76</v>
       </c>
       <c r="J126" s="4"/>
@@ -6220,7 +6243,7 @@
       </c>
       <c r="T126" s="4"/>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>8</v>
       </c>
@@ -6274,7 +6297,7 @@
       <c r="S127" s="30"/>
       <c r="T127" s="31"/>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>8</v>
       </c>
@@ -6327,7 +6350,7 @@
       <c r="S128" s="30"/>
       <c r="T128" s="31"/>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>8</v>
       </c>
@@ -6381,7 +6404,7 @@
       <c r="S129" s="30"/>
       <c r="T129" s="31"/>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>8</v>
       </c>
@@ -6432,7 +6455,7 @@
       <c r="S130" s="30"/>
       <c r="T130" s="31"/>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>8</v>
       </c>
@@ -6484,7 +6507,7 @@
       </c>
       <c r="T131" s="4"/>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>8</v>
       </c>
@@ -6536,7 +6559,7 @@
       </c>
       <c r="T132" s="4"/>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>8</v>
       </c>
@@ -6588,7 +6611,7 @@
       </c>
       <c r="T133" s="4"/>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>8</v>
       </c>
@@ -6641,7 +6664,7 @@
       </c>
       <c r="T134" s="4"/>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>8</v>
       </c>
@@ -6695,7 +6718,7 @@
       </c>
       <c r="T135" s="4"/>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>8</v>
       </c>
@@ -6750,7 +6773,7 @@
       <c r="S136" s="30"/>
       <c r="T136" s="31"/>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>8</v>
       </c>
@@ -6783,7 +6806,7 @@
       <c r="P137" s="5"/>
       <c r="T137" s="4"/>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>8</v>
       </c>
@@ -6822,7 +6845,7 @@
       <c r="S138" s="7"/>
       <c r="T138" s="8"/>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>40</v>
       </c>
@@ -6842,7 +6865,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>41</v>
       </c>
@@ -6850,7 +6873,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B143">
         <v>125</v>
       </c>
@@ -6858,7 +6881,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B144">
         <v>126</v>
       </c>
@@ -6866,7 +6889,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="146" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>42</v>
       </c>
@@ -6874,7 +6897,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="147" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B147" t="str">
         <f ca="1">"3,1,"&amp;INDIRECT(D141&amp;B143)&amp;","&amp;INDIRECT(D141&amp;B144)&amp;",0,-1,NONE,NONE,SO MINISCAN "&amp;A138&amp;"KHZ STARTING ORDER "&amp;INDIRECT(C141&amp;B143)&amp;" &amp; "&amp;INDIRECT(C141&amp;B144)</f>
         <v>3,1,223,224,0,-1,NONE,NONE,SO MINISCAN 8KHZ STARTING ORDER 128 &amp; 134</v>

</xml_diff>

<commit_message>
MTP084 done and advanced planning updated
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A773503E-7A7A-4F54-9AA4-9C5062F9D503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9EE5CD-7BCC-4408-A500-E92736BCAAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -908,7 +908,7 @@
     <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1033,6 +1033,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -1356,8 +1357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U97" sqref="U97"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q111" sqref="O111:Q112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5305,7 +5306,9 @@
       <c r="P102" s="29">
         <v>8</v>
       </c>
-      <c r="Q102" s="30"/>
+      <c r="Q102" s="30">
+        <v>84</v>
+      </c>
       <c r="R102" s="30"/>
       <c r="S102" s="30"/>
       <c r="T102" s="31"/>
@@ -5695,7 +5698,9 @@
       <c r="P111" s="2">
         <v>38</v>
       </c>
-      <c r="Q111" s="73"/>
+      <c r="Q111" s="79">
+        <v>84</v>
+      </c>
       <c r="T111" s="4"/>
     </row>
     <row r="112" spans="1:20" x14ac:dyDescent="0.3">
@@ -5745,6 +5750,9 @@
       </c>
       <c r="P112" s="2">
         <v>9</v>
+      </c>
+      <c r="Q112" s="3">
+        <v>84</v>
       </c>
       <c r="T112" s="4"/>
     </row>
@@ -5844,6 +5852,7 @@
       <c r="P114" s="2">
         <v>8</v>
       </c>
+      <c r="Q114" s="92"/>
       <c r="T114" s="4"/>
     </row>
     <row r="115" spans="1:20" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
All MTPs reprocessed to correct UVIS COP table bug. MTP085 COP rows generated
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9EE5CD-7BCC-4408-A500-E92736BCAAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8951F16E-9A13-4A82-A02B-F0ACAB3E3D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1033,7 +1033,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -1358,7 +1358,7 @@
   <dimension ref="A1:AE147"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A83" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q111" sqref="O111:Q112"/>
+      <selection activeCell="V111" sqref="V111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5306,8 +5306,8 @@
       <c r="P102" s="29">
         <v>8</v>
       </c>
-      <c r="Q102" s="30">
-        <v>84</v>
+      <c r="Q102" s="32">
+        <v>85</v>
       </c>
       <c r="R102" s="30"/>
       <c r="S102" s="30"/>
@@ -5351,6 +5351,9 @@
       </c>
       <c r="P103" s="2">
         <v>55</v>
+      </c>
+      <c r="Q103" s="92">
+        <v>85</v>
       </c>
       <c r="T103" s="4"/>
     </row>
@@ -5852,7 +5855,7 @@
       <c r="P114" s="2">
         <v>8</v>
       </c>
-      <c r="Q114" s="92"/>
+      <c r="Q114" s="73"/>
       <c r="T114" s="4"/>
     </row>
     <row r="115" spans="1:20" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
MTP092 done; 2025 patches started
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D32958-A825-4976-AFA1-70B8D61500F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4A8FBD-5D40-42C3-A50E-D094CD4BB8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1360,7 +1360,7 @@
   <dimension ref="A1:AE147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1481,6 +1481,9 @@
       <c r="N5" s="3">
         <v>75</v>
       </c>
+      <c r="O5" s="3">
+        <v>92</v>
+      </c>
       <c r="AE5" s="4"/>
     </row>
     <row r="6" spans="2:31" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Planning code changed to generate more accurate distribution of high/medium/low priority observations; MTP096 generated
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57622501-5317-4AE2-B259-049FB36EC26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCD8F26-62BF-4C46-82CD-33D4B153802D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1359,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F122" sqref="F122:F123"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F93" sqref="F93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4904,7 +4904,9 @@
       <c r="E93">
         <v>194</v>
       </c>
-      <c r="F93" s="5"/>
+      <c r="F93" s="5">
+        <v>96</v>
+      </c>
       <c r="J93" s="4"/>
       <c r="L93" s="5">
         <f t="shared" si="7"/>
@@ -5181,7 +5183,9 @@
       <c r="E99">
         <v>200</v>
       </c>
-      <c r="F99" s="64"/>
+      <c r="F99" s="64">
+        <v>96</v>
+      </c>
       <c r="J99" s="4"/>
       <c r="L99" s="5">
         <f t="shared" si="7"/>
@@ -5220,7 +5224,9 @@
       <c r="E100">
         <v>201</v>
       </c>
-      <c r="F100" s="5"/>
+      <c r="F100" s="5">
+        <v>96</v>
+      </c>
       <c r="J100" s="4"/>
       <c r="L100" s="5">
         <f t="shared" si="7"/>
@@ -5355,6 +5361,9 @@
       <c r="F103" s="2">
         <v>47</v>
       </c>
+      <c r="G103" s="79">
+        <v>95</v>
+      </c>
       <c r="J103" s="4"/>
       <c r="L103" s="35">
         <f t="shared" si="7"/>
@@ -5619,6 +5628,9 @@
       <c r="F109" s="2">
         <v>27</v>
       </c>
+      <c r="G109" s="3">
+        <v>96</v>
+      </c>
       <c r="J109" s="4"/>
       <c r="L109" s="5">
         <f t="shared" si="7"/>
@@ -5660,7 +5672,9 @@
       <c r="F110" s="2">
         <v>38</v>
       </c>
-      <c r="G110" s="3"/>
+      <c r="G110" s="3">
+        <v>95</v>
+      </c>
       <c r="J110" s="4"/>
       <c r="L110" s="5">
         <f t="shared" si="7"/>

</xml_diff>

<commit_message>
MTP096 and MTP097 done
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21D78EC-7B3D-4EF6-B885-26A6232C6863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33EA8E6B-1B49-4034-A15A-0DFC2B1D6D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -911,7 +911,7 @@
     <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1036,7 +1036,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -1360,27 +1362,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H93" sqref="H93"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H103" sqref="H103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" customWidth="1"/>
-    <col min="12" max="12" width="16.88671875" customWidth="1"/>
-    <col min="13" max="13" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="21" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.33203125" customWidth="1"/>
-    <col min="23" max="23" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.28515625" customWidth="1"/>
+    <col min="23" max="23" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1388,12 +1390,12 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="2:31" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:31" ht="18.75" x14ac:dyDescent="0.3">
       <c r="W2" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:31" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:31" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="14" t="s">
         <v>3</v>
       </c>
@@ -1406,7 +1408,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C4" s="13" t="s">
         <v>12</v>
       </c>
@@ -1445,7 +1447,7 @@
       <c r="AD4" s="71"/>
       <c r="AE4" s="65"/>
     </row>
-    <row r="5" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C5" s="19" t="s">
         <v>1</v>
       </c>
@@ -1487,7 +1489,7 @@
       </c>
       <c r="AE5" s="4"/>
     </row>
-    <row r="6" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C6" s="20" t="s">
         <v>2</v>
       </c>
@@ -1552,14 +1554,14 @@
       <c r="AD6" s="7"/>
       <c r="AE6" s="8"/>
     </row>
-    <row r="9" spans="2:31" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:31" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
@@ -1598,7 +1600,7 @@
       <c r="AD10" s="71"/>
       <c r="AE10" s="65"/>
     </row>
-    <row r="11" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C11" s="19" t="s">
         <v>34</v>
       </c>
@@ -1655,7 +1657,7 @@
       <c r="AD11" s="16"/>
       <c r="AE11" s="17"/>
     </row>
-    <row r="12" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C12" s="20" t="s">
         <v>36</v>
       </c>
@@ -1700,12 +1702,12 @@
       <c r="AD12" s="7"/>
       <c r="AE12" s="8"/>
     </row>
-    <row r="13" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:31" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:31" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B15" s="14" t="s">
         <v>0</v>
       </c>
@@ -1719,12 +1721,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:31" x14ac:dyDescent="0.25">
       <c r="AC16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
         <v>1</v>
       </c>
@@ -1752,7 +1754,7 @@
       <c r="S17" s="91"/>
       <c r="T17" s="91"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B18" s="39" t="s">
         <v>10</v>
       </c>
@@ -1827,7 +1829,7 @@
       </c>
       <c r="AE18" s="9"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1882,7 +1884,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1931,7 +1933,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1978,7 +1980,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2042,7 +2044,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2091,7 +2093,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2140,7 +2142,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -2200,7 +2202,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -2249,7 +2251,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -2301,7 +2303,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2346,7 +2348,7 @@
       </c>
       <c r="Z28" s="55"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2389,7 +2391,7 @@
       <c r="Y29" s="48"/>
       <c r="Z29" s="49"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -2438,7 +2440,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -2483,7 +2485,7 @@
       <c r="Y31" s="48"/>
       <c r="Z31" s="49"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2533,7 +2535,7 @@
       <c r="Y32" s="48"/>
       <c r="Z32" s="49"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -2578,7 +2580,7 @@
       <c r="Y33" s="48"/>
       <c r="Z33" s="49"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -2626,7 +2628,7 @@
       <c r="Y34" s="48"/>
       <c r="Z34" s="49"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
@@ -2672,7 +2674,7 @@
       <c r="Y35" s="48"/>
       <c r="Z35" s="49"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -2717,7 +2719,7 @@
       <c r="Y36" s="48"/>
       <c r="Z36" s="49"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -2760,7 +2762,7 @@
       <c r="Y37" s="48"/>
       <c r="Z37" s="49"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
@@ -2803,7 +2805,7 @@
       <c r="Y38" s="48"/>
       <c r="Z38" s="49"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1</v>
       </c>
@@ -2849,7 +2851,7 @@
       <c r="Y39" s="48"/>
       <c r="Z39" s="49"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1</v>
       </c>
@@ -2892,7 +2894,7 @@
       <c r="Y40" s="48"/>
       <c r="Z40" s="49"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1</v>
       </c>
@@ -2942,7 +2944,7 @@
       <c r="Y41" s="48"/>
       <c r="Z41" s="49"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1</v>
       </c>
@@ -2993,7 +2995,7 @@
       <c r="Y42" s="48"/>
       <c r="Z42" s="49"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
@@ -3048,7 +3050,7 @@
       <c r="Y43" s="48"/>
       <c r="Z43" s="49"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1</v>
       </c>
@@ -3095,7 +3097,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1</v>
       </c>
@@ -3141,7 +3143,7 @@
       <c r="Y45" s="5"/>
       <c r="Z45" s="4"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1</v>
       </c>
@@ -3182,7 +3184,7 @@
       <c r="Y46" s="5"/>
       <c r="Z46" s="4"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1</v>
       </c>
@@ -3221,7 +3223,7 @@
       <c r="Y47" s="5"/>
       <c r="Z47" s="4"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1</v>
       </c>
@@ -3268,7 +3270,7 @@
       <c r="Y48" s="5"/>
       <c r="Z48" s="4"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="W49" s="5">
         <v>4526.9799999999996</v>
       </c>
@@ -3278,7 +3280,7 @@
       <c r="Y49" s="6"/>
       <c r="Z49" s="8"/>
     </row>
-    <row r="50" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B50" s="14" t="s">
         <v>0</v>
       </c>
@@ -3290,7 +3292,7 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -3301,7 +3303,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B52" s="9" t="s">
         <v>1</v>
       </c>
@@ -3329,7 +3331,7 @@
       <c r="S52" s="91"/>
       <c r="T52" s="91"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B53" s="9" t="s">
         <v>10</v>
       </c>
@@ -3385,7 +3387,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2</v>
       </c>
@@ -3422,7 +3424,7 @@
       </c>
       <c r="T54" s="4"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2</v>
       </c>
@@ -3459,7 +3461,7 @@
       <c r="P55" s="5"/>
       <c r="T55" s="4"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2</v>
       </c>
@@ -3511,7 +3513,7 @@
       <c r="S56" s="30"/>
       <c r="T56" s="31"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2</v>
       </c>
@@ -3548,7 +3550,7 @@
       <c r="P57" s="5"/>
       <c r="T57" s="4"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2</v>
       </c>
@@ -3585,7 +3587,7 @@
       <c r="P58" s="5"/>
       <c r="T58" s="4"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2</v>
       </c>
@@ -3626,7 +3628,7 @@
       </c>
       <c r="T59" s="4"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2</v>
       </c>
@@ -3663,7 +3665,7 @@
       <c r="P60" s="5"/>
       <c r="T60" s="4"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2</v>
       </c>
@@ -3715,7 +3717,7 @@
       <c r="S61" s="30"/>
       <c r="T61" s="31"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2</v>
       </c>
@@ -3752,7 +3754,7 @@
       <c r="P62" s="5"/>
       <c r="T62" s="4"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2</v>
       </c>
@@ -3804,7 +3806,7 @@
       <c r="S63" s="30"/>
       <c r="T63" s="31"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2</v>
       </c>
@@ -3841,7 +3843,7 @@
       <c r="P64" s="5"/>
       <c r="T64" s="4"/>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2</v>
       </c>
@@ -3878,7 +3880,7 @@
       <c r="P65" s="35"/>
       <c r="T65" s="4"/>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2</v>
       </c>
@@ -3915,7 +3917,7 @@
       <c r="P66" s="5"/>
       <c r="T66" s="4"/>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2</v>
       </c>
@@ -3952,7 +3954,7 @@
       <c r="P67" s="5"/>
       <c r="T67" s="4"/>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2</v>
       </c>
@@ -4004,7 +4006,7 @@
       <c r="S68" s="30"/>
       <c r="T68" s="31"/>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2</v>
       </c>
@@ -4051,7 +4053,7 @@
       </c>
       <c r="T69" s="4"/>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2</v>
       </c>
@@ -4092,7 +4094,7 @@
       </c>
       <c r="T70" s="4"/>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2</v>
       </c>
@@ -4129,7 +4131,7 @@
       <c r="P71" s="5"/>
       <c r="T71" s="4"/>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2</v>
       </c>
@@ -4166,7 +4168,7 @@
       <c r="P72" s="5"/>
       <c r="T72" s="4"/>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2</v>
       </c>
@@ -4203,7 +4205,7 @@
       <c r="P73" s="5"/>
       <c r="T73" s="4"/>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2</v>
       </c>
@@ -4240,7 +4242,7 @@
       <c r="P74" s="5"/>
       <c r="T74" s="4"/>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2</v>
       </c>
@@ -4277,7 +4279,7 @@
       <c r="P75" s="5"/>
       <c r="T75" s="4"/>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2</v>
       </c>
@@ -4318,7 +4320,7 @@
       </c>
       <c r="T76" s="4"/>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2</v>
       </c>
@@ -4362,7 +4364,7 @@
       </c>
       <c r="T77" s="4"/>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2</v>
       </c>
@@ -4399,7 +4401,7 @@
       <c r="P78" s="5"/>
       <c r="T78" s="4"/>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2</v>
       </c>
@@ -4447,7 +4449,7 @@
       <c r="S79" s="30"/>
       <c r="T79" s="31"/>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2</v>
       </c>
@@ -4484,7 +4486,7 @@
       <c r="P80" s="5"/>
       <c r="T80" s="4"/>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2</v>
       </c>
@@ -4521,7 +4523,7 @@
       <c r="P81" s="5"/>
       <c r="T81" s="4"/>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2</v>
       </c>
@@ -4564,7 +4566,7 @@
       <c r="S82" s="7"/>
       <c r="T82" s="8"/>
     </row>
-    <row r="84" spans="1:20" ht="18" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B84" s="14" t="s">
         <v>0</v>
       </c>
@@ -4578,7 +4580,7 @@
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
@@ -4586,7 +4588,7 @@
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B86" s="9" t="s">
         <v>1</v>
       </c>
@@ -4614,7 +4616,7 @@
       <c r="S86" s="91"/>
       <c r="T86" s="91"/>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B87" s="9" t="s">
         <v>10</v>
       </c>
@@ -4670,7 +4672,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>4</v>
       </c>
@@ -4705,7 +4707,7 @@
       <c r="P88" s="5"/>
       <c r="T88" s="4"/>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>4</v>
       </c>
@@ -4749,7 +4751,7 @@
       </c>
       <c r="T89" s="4"/>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>4</v>
       </c>
@@ -4801,7 +4803,7 @@
       <c r="S90" s="30"/>
       <c r="T90" s="31"/>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>4</v>
       </c>
@@ -4848,7 +4850,7 @@
       </c>
       <c r="T91" s="4"/>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>4</v>
       </c>
@@ -4869,9 +4871,7 @@
       <c r="F92" s="2">
         <v>81</v>
       </c>
-      <c r="G92" s="3">
-        <v>97</v>
-      </c>
+      <c r="G92" s="93"/>
       <c r="J92" s="4"/>
       <c r="L92" s="5">
         <f t="shared" si="7"/>
@@ -4890,7 +4890,7 @@
       <c r="P92" s="5"/>
       <c r="T92" s="4"/>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>4</v>
       </c>
@@ -4908,9 +4908,7 @@
       <c r="E93">
         <v>194</v>
       </c>
-      <c r="F93" s="2">
-        <v>96</v>
-      </c>
+      <c r="F93" s="92"/>
       <c r="J93" s="4"/>
       <c r="L93" s="5">
         <f t="shared" si="7"/>
@@ -4929,7 +4927,7 @@
       <c r="P93" s="5"/>
       <c r="T93" s="4"/>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>4</v>
       </c>
@@ -4973,7 +4971,7 @@
       </c>
       <c r="T94" s="4"/>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>4</v>
       </c>
@@ -5027,7 +5025,7 @@
       <c r="S95" s="30"/>
       <c r="T95" s="31"/>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>4</v>
       </c>
@@ -5068,7 +5066,7 @@
       </c>
       <c r="T96" s="4"/>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>4</v>
       </c>
@@ -5120,7 +5118,7 @@
       <c r="S97" s="30"/>
       <c r="T97" s="31"/>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>4</v>
       </c>
@@ -5169,7 +5167,7 @@
       <c r="S98" s="30"/>
       <c r="T98" s="31"/>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>4</v>
       </c>
@@ -5187,9 +5185,7 @@
       <c r="E99">
         <v>200</v>
       </c>
-      <c r="F99" s="92">
-        <v>96</v>
-      </c>
+      <c r="F99" s="94"/>
       <c r="J99" s="4"/>
       <c r="L99" s="5">
         <f t="shared" si="7"/>
@@ -5210,7 +5206,7 @@
       </c>
       <c r="T99" s="4"/>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>4</v>
       </c>
@@ -5228,9 +5224,7 @@
       <c r="E100">
         <v>201</v>
       </c>
-      <c r="F100" s="2">
-        <v>96</v>
-      </c>
+      <c r="F100" s="92"/>
       <c r="J100" s="4"/>
       <c r="L100" s="5">
         <f t="shared" si="7"/>
@@ -5251,7 +5245,7 @@
       </c>
       <c r="T100" s="4"/>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>4</v>
       </c>
@@ -5272,9 +5266,7 @@
       <c r="F101" s="2">
         <v>9</v>
       </c>
-      <c r="G101" s="3">
-        <v>97</v>
-      </c>
+      <c r="G101" s="93"/>
       <c r="J101" s="4"/>
       <c r="L101" s="5">
         <f t="shared" si="7"/>
@@ -5295,7 +5287,7 @@
       </c>
       <c r="T101" s="4"/>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>4</v>
       </c>
@@ -5347,7 +5339,7 @@
       <c r="S102" s="30"/>
       <c r="T102" s="31"/>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>4</v>
       </c>
@@ -5394,7 +5386,7 @@
       </c>
       <c r="T103" s="4"/>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>4</v>
       </c>
@@ -5438,7 +5430,7 @@
       </c>
       <c r="T104" s="4"/>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>4</v>
       </c>
@@ -5482,7 +5474,7 @@
       </c>
       <c r="T105" s="4"/>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>4</v>
       </c>
@@ -5526,7 +5518,7 @@
       </c>
       <c r="T106" s="4"/>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>4</v>
       </c>
@@ -5570,7 +5562,7 @@
       </c>
       <c r="T107" s="4"/>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>4</v>
       </c>
@@ -5614,7 +5606,7 @@
       </c>
       <c r="T108" s="4"/>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>4</v>
       </c>
@@ -5635,9 +5627,7 @@
       <c r="F109" s="2">
         <v>27</v>
       </c>
-      <c r="G109" s="3">
-        <v>96</v>
-      </c>
+      <c r="G109" s="93"/>
       <c r="J109" s="4"/>
       <c r="L109" s="5">
         <f t="shared" si="7"/>
@@ -5658,7 +5648,7 @@
       </c>
       <c r="T109" s="4"/>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>4</v>
       </c>
@@ -5702,7 +5692,7 @@
       </c>
       <c r="T110" s="4"/>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>4</v>
       </c>
@@ -5755,7 +5745,7 @@
       </c>
       <c r="T111" s="4"/>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>4</v>
       </c>
@@ -5808,7 +5798,7 @@
       </c>
       <c r="T112" s="4"/>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>4</v>
       </c>
@@ -5862,7 +5852,7 @@
       <c r="S113" s="30"/>
       <c r="T113" s="31"/>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>4</v>
       </c>
@@ -5907,7 +5897,7 @@
       <c r="Q114" s="73"/>
       <c r="T114" s="4"/>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>4</v>
       </c>
@@ -5925,7 +5915,15 @@
       <c r="E115">
         <v>216</v>
       </c>
-      <c r="F115" s="5"/>
+      <c r="F115" s="2">
+        <v>96</v>
+      </c>
+      <c r="G115" s="3">
+        <v>96</v>
+      </c>
+      <c r="H115" s="3">
+        <v>97</v>
+      </c>
       <c r="J115" s="4"/>
       <c r="L115" s="5">
         <f t="shared" si="7"/>
@@ -5944,7 +5942,7 @@
       <c r="P115" s="5"/>
       <c r="T115" s="4"/>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>4</v>
       </c>
@@ -5962,9 +5960,15 @@
       <c r="E116">
         <v>217</v>
       </c>
-      <c r="F116" s="6"/>
-      <c r="G116" s="7"/>
-      <c r="H116" s="7"/>
+      <c r="F116" s="69">
+        <v>96</v>
+      </c>
+      <c r="G116" s="18">
+        <v>96</v>
+      </c>
+      <c r="H116" s="18">
+        <v>97</v>
+      </c>
       <c r="I116" s="7"/>
       <c r="J116" s="8"/>
       <c r="L116" s="6">
@@ -5987,7 +5991,7 @@
       <c r="S116" s="7"/>
       <c r="T116" s="8"/>
     </row>
-    <row r="118" spans="1:20" ht="18" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B118" s="14" t="s">
         <v>0</v>
       </c>
@@ -5999,7 +6003,7 @@
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
@@ -6007,7 +6011,7 @@
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B120" s="9" t="s">
         <v>1</v>
       </c>
@@ -6034,7 +6038,7 @@
       <c r="S120" s="91"/>
       <c r="T120" s="91"/>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B121" s="9" t="s">
         <v>10</v>
       </c>
@@ -6090,7 +6094,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>8</v>
       </c>
@@ -6129,7 +6133,7 @@
       <c r="S122" s="30"/>
       <c r="T122" s="31"/>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>8</v>
       </c>
@@ -6166,7 +6170,7 @@
       </c>
       <c r="T123" s="4"/>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>8</v>
       </c>
@@ -6219,7 +6223,7 @@
       <c r="S124" s="30"/>
       <c r="T124" s="31"/>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>8</v>
       </c>
@@ -6271,7 +6275,7 @@
       </c>
       <c r="T125" s="4"/>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>8</v>
       </c>
@@ -6323,7 +6327,7 @@
       </c>
       <c r="T126" s="4"/>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>8</v>
       </c>
@@ -6377,7 +6381,7 @@
       <c r="S127" s="30"/>
       <c r="T127" s="31"/>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>8</v>
       </c>
@@ -6430,7 +6434,7 @@
       <c r="S128" s="30"/>
       <c r="T128" s="31"/>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>8</v>
       </c>
@@ -6484,7 +6488,7 @@
       <c r="S129" s="30"/>
       <c r="T129" s="31"/>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>8</v>
       </c>
@@ -6535,7 +6539,7 @@
       <c r="S130" s="30"/>
       <c r="T130" s="31"/>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>8</v>
       </c>
@@ -6587,7 +6591,7 @@
       </c>
       <c r="T131" s="4"/>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>8</v>
       </c>
@@ -6639,7 +6643,7 @@
       </c>
       <c r="T132" s="4"/>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>8</v>
       </c>
@@ -6691,7 +6695,7 @@
       </c>
       <c r="T133" s="4"/>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>8</v>
       </c>
@@ -6744,7 +6748,7 @@
       </c>
       <c r="T134" s="4"/>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>8</v>
       </c>
@@ -6798,7 +6802,7 @@
       </c>
       <c r="T135" s="4"/>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>8</v>
       </c>
@@ -6853,7 +6857,7 @@
       <c r="S136" s="30"/>
       <c r="T136" s="31"/>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>8</v>
       </c>
@@ -6886,7 +6890,7 @@
       <c r="P137" s="5"/>
       <c r="T137" s="4"/>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>8</v>
       </c>
@@ -6925,7 +6929,7 @@
       <c r="S138" s="7"/>
       <c r="T138" s="8"/>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>40</v>
       </c>
@@ -6945,7 +6949,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>41</v>
       </c>
@@ -6953,7 +6957,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B143">
         <v>125</v>
       </c>
@@ -6961,7 +6965,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B144">
         <v>126</v>
       </c>
@@ -6969,7 +6973,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="146" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>42</v>
       </c>
@@ -6977,7 +6981,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="147" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B147" t="str">
         <f ca="1">"3,1,"&amp;INDIRECT(D141&amp;B143)&amp;","&amp;INDIRECT(D141&amp;B144)&amp;",0,-1,NONE,NONE,SO MINISCAN "&amp;A138&amp;"KHZ STARTING ORDER "&amp;INDIRECT(C141&amp;B143)&amp;" &amp; "&amp;INDIRECT(C141&amp;B144)</f>
         <v>3,1,223,224,0,-1,NONE,NONE,SO MINISCAN 8KHZ STARTING ORDER 128 &amp; 134</v>

</xml_diff>

<commit_message>
MTP100 done; new script added to sort incomings. DV calc ongoing
</commit_message>
<xml_diff>
--- a/observations/calibrations/solar_calibrations.xlsx
+++ b/observations/calibrations/solar_calibrations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A43ABF-C57A-4DB0-B64C-9CA8E45701C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E5C648-F6E9-4733-B8BB-B07F433AB15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1296" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="48">
   <si>
     <t>MINISCANS</t>
   </si>
@@ -177,9 +177,6 @@
   </si>
   <si>
     <t>O</t>
-  </si>
-  <si>
-    <t>RUN SOME LOW ORDERS</t>
   </si>
   <si>
     <t>MTP021+ COP Row</t>
@@ -911,7 +908,7 @@
     <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1022,8 +1019,6 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1036,6 +1031,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -1359,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1568,13 +1568,13 @@
       <c r="E10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="88" t="s">
+      <c r="F10" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="89"/>
-      <c r="H10" s="89"/>
-      <c r="I10" s="89"/>
-      <c r="J10" s="89"/>
+      <c r="G10" s="87"/>
+      <c r="H10" s="87"/>
+      <c r="I10" s="87"/>
+      <c r="J10" s="87"/>
       <c r="K10" s="71"/>
       <c r="L10" s="71"/>
       <c r="M10" s="71"/>
@@ -1730,26 +1730,26 @@
       <c r="C17" s="13"/>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="90" t="s">
+      <c r="F17" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="91"/>
-      <c r="H17" s="91"/>
-      <c r="I17" s="91"/>
-      <c r="J17" s="91"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="89"/>
+      <c r="I17" s="89"/>
+      <c r="J17" s="89"/>
       <c r="L17" s="9" t="s">
         <v>2</v>
       </c>
       <c r="M17" s="13"/>
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
-      <c r="P17" s="90" t="s">
+      <c r="P17" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="Q17" s="91"/>
-      <c r="R17" s="91"/>
-      <c r="S17" s="91"/>
-      <c r="T17" s="91"/>
+      <c r="Q17" s="89"/>
+      <c r="R17" s="89"/>
+      <c r="S17" s="89"/>
+      <c r="T17" s="89"/>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B18" s="39" t="s">
@@ -1762,7 +1762,7 @@
         <v>21</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>11</v>
@@ -1789,7 +1789,7 @@
         <v>21</v>
       </c>
       <c r="O18" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P18" s="10" t="s">
         <v>11</v>
@@ -2595,16 +2595,17 @@
       <c r="E34" s="79">
         <v>69</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="81">
         <v>50</v>
       </c>
       <c r="G34" s="79">
         <v>87</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H34" s="79">
         <v>99</v>
       </c>
-      <c r="J34" s="4"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="85"/>
       <c r="L34" s="74">
         <v>168</v>
       </c>
@@ -3316,26 +3317,26 @@
       <c r="C52" s="13"/>
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
-      <c r="F52" s="90" t="s">
+      <c r="F52" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="G52" s="91"/>
-      <c r="H52" s="91"/>
-      <c r="I52" s="91"/>
-      <c r="J52" s="91"/>
+      <c r="G52" s="89"/>
+      <c r="H52" s="89"/>
+      <c r="I52" s="89"/>
+      <c r="J52" s="89"/>
       <c r="L52" s="9" t="s">
         <v>2</v>
       </c>
       <c r="M52" s="13"/>
       <c r="N52" s="9"/>
       <c r="O52" s="9"/>
-      <c r="P52" s="90" t="s">
+      <c r="P52" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="Q52" s="91"/>
-      <c r="R52" s="91"/>
-      <c r="S52" s="91"/>
-      <c r="T52" s="91"/>
+      <c r="Q52" s="89"/>
+      <c r="R52" s="89"/>
+      <c r="S52" s="89"/>
+      <c r="T52" s="89"/>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B53" s="9" t="s">
@@ -4601,26 +4602,26 @@
       <c r="C86" s="13"/>
       <c r="D86" s="9"/>
       <c r="E86" s="33"/>
-      <c r="F86" s="90" t="s">
+      <c r="F86" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="G86" s="91"/>
-      <c r="H86" s="91"/>
-      <c r="I86" s="91"/>
-      <c r="J86" s="91"/>
+      <c r="G86" s="89"/>
+      <c r="H86" s="89"/>
+      <c r="I86" s="89"/>
+      <c r="J86" s="89"/>
       <c r="L86" s="9" t="s">
         <v>2</v>
       </c>
       <c r="M86" s="13"/>
       <c r="N86" s="9"/>
       <c r="O86" s="33"/>
-      <c r="P86" s="90" t="s">
+      <c r="P86" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="Q86" s="91"/>
-      <c r="R86" s="91"/>
-      <c r="S86" s="91"/>
-      <c r="T86" s="91"/>
+      <c r="Q86" s="89"/>
+      <c r="R86" s="89"/>
+      <c r="S86" s="89"/>
+      <c r="T86" s="89"/>
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B87" s="9" t="s">
@@ -4694,8 +4695,8 @@
       <c r="E88">
         <v>189</v>
       </c>
-      <c r="F88" s="5" t="s">
-        <v>47</v>
+      <c r="F88" s="2">
+        <v>100</v>
       </c>
       <c r="J88" s="4"/>
       <c r="L88" s="5">
@@ -4827,16 +4828,17 @@
       <c r="E91" s="73">
         <v>192</v>
       </c>
-      <c r="F91" s="2">
+      <c r="F91" s="81">
         <v>57</v>
       </c>
       <c r="G91" s="79">
         <v>81</v>
       </c>
-      <c r="H91" s="3">
+      <c r="H91" s="79">
         <v>86</v>
       </c>
-      <c r="J91" s="4"/>
+      <c r="I91" s="73"/>
+      <c r="J91" s="85"/>
       <c r="L91" s="35">
         <f t="shared" si="7"/>
         <v>128</v>
@@ -4913,7 +4915,9 @@
       <c r="E93">
         <v>194</v>
       </c>
-      <c r="F93" s="5"/>
+      <c r="F93" s="2">
+        <v>100</v>
+      </c>
       <c r="J93" s="4"/>
       <c r="L93" s="5">
         <f t="shared" si="7"/>
@@ -4953,7 +4957,7 @@
       <c r="F94" s="2">
         <v>9</v>
       </c>
-      <c r="G94">
+      <c r="G94" s="3">
         <v>82</v>
       </c>
       <c r="J94" s="4"/>
@@ -4994,17 +4998,17 @@
       <c r="E95" s="79">
         <v>196</v>
       </c>
-      <c r="F95" s="29">
+      <c r="F95" s="80">
         <v>7</v>
       </c>
-      <c r="G95" s="32">
+      <c r="G95" s="82">
         <v>15</v>
       </c>
-      <c r="H95" s="30">
+      <c r="H95" s="82">
         <v>82</v>
       </c>
-      <c r="I95" s="30"/>
-      <c r="J95" s="31"/>
+      <c r="I95" s="91"/>
+      <c r="J95" s="92"/>
       <c r="K95" s="30"/>
       <c r="L95" s="80">
         <f t="shared" si="7"/>
@@ -5048,7 +5052,7 @@
       <c r="E96">
         <v>197</v>
       </c>
-      <c r="F96" s="5">
+      <c r="F96" s="2">
         <v>82</v>
       </c>
       <c r="J96" s="4"/>
@@ -5089,17 +5093,17 @@
       <c r="E97" s="79">
         <v>198</v>
       </c>
-      <c r="F97" s="29">
+      <c r="F97" s="80">
         <v>8</v>
       </c>
-      <c r="G97" s="32">
+      <c r="G97" s="82">
         <v>21</v>
       </c>
-      <c r="H97" s="30">
+      <c r="H97" s="82">
         <v>82</v>
       </c>
-      <c r="I97" s="30"/>
-      <c r="J97" s="31"/>
+      <c r="I97" s="91"/>
+      <c r="J97" s="92"/>
       <c r="K97" s="30"/>
       <c r="L97" s="80">
         <f t="shared" si="7"/>
@@ -5190,7 +5194,9 @@
       <c r="E99">
         <v>200</v>
       </c>
-      <c r="F99" s="64"/>
+      <c r="F99" s="90">
+        <v>100</v>
+      </c>
       <c r="J99" s="4"/>
       <c r="L99" s="5">
         <f t="shared" si="7"/>
@@ -5229,7 +5235,9 @@
       <c r="E100">
         <v>201</v>
       </c>
-      <c r="F100" s="5"/>
+      <c r="F100" s="2">
+        <v>100</v>
+      </c>
       <c r="J100" s="4"/>
       <c r="L100" s="5">
         <f t="shared" si="7"/>
@@ -5361,13 +5369,15 @@
       <c r="E103" s="73">
         <v>204</v>
       </c>
-      <c r="F103" s="2">
+      <c r="F103" s="81">
         <v>47</v>
       </c>
       <c r="G103" s="79">
         <v>95</v>
       </c>
-      <c r="J103" s="4"/>
+      <c r="H103" s="73"/>
+      <c r="I103" s="73"/>
+      <c r="J103" s="85"/>
       <c r="L103" s="35">
         <f t="shared" si="7"/>
         <v>164</v>
@@ -5408,13 +5418,15 @@
       <c r="E104" s="73">
         <v>205</v>
       </c>
-      <c r="F104" s="2">
+      <c r="F104" s="81">
         <v>7</v>
       </c>
-      <c r="G104" s="3">
+      <c r="G104" s="79">
         <v>47</v>
       </c>
-      <c r="J104" s="4"/>
+      <c r="H104" s="73"/>
+      <c r="I104" s="73"/>
+      <c r="J104" s="85"/>
       <c r="L104" s="81">
         <f t="shared" si="7"/>
         <v>167</v>
@@ -5713,19 +5725,19 @@
       <c r="E111" s="73">
         <v>212</v>
       </c>
-      <c r="F111" s="2">
+      <c r="F111" s="81">
         <v>38</v>
       </c>
-      <c r="G111" s="3">
+      <c r="G111" s="79">
         <v>47</v>
       </c>
-      <c r="H111" s="3">
+      <c r="H111" s="79">
         <v>62</v>
       </c>
-      <c r="I111" s="3">
+      <c r="I111" s="79">
         <v>78</v>
       </c>
-      <c r="J111" s="4"/>
+      <c r="J111" s="85"/>
       <c r="L111" s="35">
         <f t="shared" si="7"/>
         <v>188</v>
@@ -5819,17 +5831,17 @@
       <c r="E113" s="79">
         <v>214</v>
       </c>
-      <c r="F113" s="29">
+      <c r="F113" s="80">
         <v>7</v>
       </c>
-      <c r="G113" s="32">
+      <c r="G113" s="82">
         <v>13</v>
       </c>
-      <c r="H113" s="32">
+      <c r="H113" s="82">
         <v>78</v>
       </c>
-      <c r="I113" s="30"/>
-      <c r="J113" s="31"/>
+      <c r="I113" s="91"/>
+      <c r="J113" s="92"/>
       <c r="K113" s="30"/>
       <c r="L113" s="80">
         <f t="shared" si="7"/>
@@ -5873,13 +5885,15 @@
       <c r="E114" s="73">
         <v>215</v>
       </c>
-      <c r="F114" s="2">
+      <c r="F114" s="81">
         <v>8</v>
       </c>
       <c r="G114" s="79">
         <v>78</v>
       </c>
-      <c r="J114" s="4"/>
+      <c r="H114" s="73"/>
+      <c r="I114" s="73"/>
+      <c r="J114" s="85"/>
       <c r="L114" s="35">
         <f t="shared" si="7"/>
         <v>197</v>
@@ -6020,26 +6034,26 @@
       </c>
       <c r="C120" s="40"/>
       <c r="D120" s="9"/>
-      <c r="F120" s="90" t="s">
+      <c r="F120" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="G120" s="91"/>
-      <c r="H120" s="91"/>
-      <c r="I120" s="91"/>
-      <c r="J120" s="91"/>
+      <c r="G120" s="89"/>
+      <c r="H120" s="89"/>
+      <c r="I120" s="89"/>
+      <c r="J120" s="89"/>
       <c r="L120" s="9" t="s">
         <v>2</v>
       </c>
       <c r="M120" s="40"/>
       <c r="N120" s="9"/>
       <c r="O120" s="33"/>
-      <c r="P120" s="90" t="s">
+      <c r="P120" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="Q120" s="91"/>
-      <c r="R120" s="91"/>
-      <c r="S120" s="91"/>
-      <c r="T120" s="91"/>
+      <c r="Q120" s="89"/>
+      <c r="R120" s="89"/>
+      <c r="S120" s="89"/>
+      <c r="T120" s="89"/>
     </row>
     <row r="121" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B121" s="9" t="s">
@@ -6198,7 +6212,7 @@
       <c r="H124" s="32">
         <v>37</v>
       </c>
-      <c r="I124" s="30">
+      <c r="I124" s="32">
         <v>76</v>
       </c>
       <c r="J124" s="31"/>
@@ -6242,19 +6256,19 @@
       <c r="E125" s="73">
         <v>223</v>
       </c>
-      <c r="F125" s="2">
+      <c r="F125" s="81">
         <v>14</v>
       </c>
-      <c r="G125" s="3">
+      <c r="G125" s="79">
         <v>32</v>
       </c>
       <c r="H125" s="79">
         <v>52</v>
       </c>
-      <c r="I125">
+      <c r="I125" s="79">
         <v>76</v>
       </c>
-      <c r="J125" s="4"/>
+      <c r="J125" s="85"/>
       <c r="L125" s="35">
         <v>128</v>
       </c>
@@ -6346,19 +6360,19 @@
       <c r="E127" s="79">
         <v>225</v>
       </c>
-      <c r="F127" s="29">
+      <c r="F127" s="80">
         <v>10</v>
       </c>
-      <c r="G127" s="32">
+      <c r="G127" s="82">
         <v>12</v>
       </c>
-      <c r="H127" s="32">
+      <c r="H127" s="82">
         <v>53</v>
       </c>
-      <c r="I127" s="30">
+      <c r="I127" s="82">
         <v>76</v>
       </c>
-      <c r="J127" s="31"/>
+      <c r="J127" s="92"/>
       <c r="K127" s="30"/>
       <c r="L127" s="80">
         <v>140</v>
@@ -6400,19 +6414,19 @@
       <c r="E128" s="79">
         <v>226</v>
       </c>
-      <c r="F128" s="29">
+      <c r="F128" s="80">
         <v>14</v>
       </c>
-      <c r="G128" s="32">
+      <c r="G128" s="82">
         <v>23</v>
       </c>
-      <c r="H128" s="32">
+      <c r="H128" s="82">
         <v>53</v>
       </c>
-      <c r="I128" s="30">
+      <c r="I128" s="82">
         <v>76</v>
       </c>
-      <c r="J128" s="31"/>
+      <c r="J128" s="92"/>
       <c r="L128" s="80">
         <v>146</v>
       </c>
@@ -6462,7 +6476,7 @@
       <c r="H129" s="3">
         <v>51</v>
       </c>
-      <c r="I129" s="30">
+      <c r="I129" s="32">
         <v>76</v>
       </c>
       <c r="J129" s="4"/>
@@ -6558,19 +6572,19 @@
       <c r="E131" s="73">
         <v>229</v>
       </c>
-      <c r="F131" s="2">
+      <c r="F131" s="81">
         <v>18</v>
       </c>
-      <c r="G131" s="3">
+      <c r="G131" s="79">
         <v>28</v>
       </c>
       <c r="H131" s="79">
         <v>51</v>
       </c>
-      <c r="I131" s="3">
+      <c r="I131" s="79">
         <v>66</v>
       </c>
-      <c r="J131" s="4"/>
+      <c r="J131" s="85"/>
       <c r="L131" s="35">
         <v>164</v>
       </c>
@@ -6767,19 +6781,19 @@
       <c r="E135" s="73">
         <v>233</v>
       </c>
-      <c r="F135" s="2">
+      <c r="F135" s="81">
         <v>33</v>
       </c>
-      <c r="G135" s="3">
+      <c r="G135" s="79">
         <v>37</v>
       </c>
-      <c r="H135" s="3">
+      <c r="H135" s="79">
         <v>41</v>
       </c>
-      <c r="I135" s="3">
+      <c r="I135" s="79">
         <v>59</v>
       </c>
-      <c r="J135" s="86">
+      <c r="J135" s="93">
         <v>75</v>
       </c>
       <c r="L135" s="35">
@@ -6821,19 +6835,19 @@
       <c r="E136" s="79">
         <v>234</v>
       </c>
-      <c r="F136" s="29">
+      <c r="F136" s="80">
         <v>10</v>
       </c>
-      <c r="G136" s="32">
+      <c r="G136" s="82">
         <v>12</v>
       </c>
-      <c r="H136" s="32">
+      <c r="H136" s="82">
         <v>42</v>
       </c>
-      <c r="I136" s="32">
+      <c r="I136" s="82">
         <v>59</v>
       </c>
-      <c r="J136" s="87">
+      <c r="J136" s="94">
         <v>75</v>
       </c>
       <c r="L136" s="80">

</xml_diff>